<commit_message>
Working on course plan
</commit_message>
<xml_diff>
--- a/updates/Updates.xlsx
+++ b/updates/Updates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="64">
   <si>
     <t>Task</t>
   </si>
@@ -174,6 +174,45 @@
   </si>
   <si>
     <t>Last Week's Tasks</t>
+  </si>
+  <si>
+    <t>Read all article Abstracts</t>
+  </si>
+  <si>
+    <t>Add hours to Update Sheet</t>
+  </si>
+  <si>
+    <t>Update Publication Plan to Account for summer conference</t>
+  </si>
+  <si>
+    <t>No, I should assume I'll work during the summer and still take another semester after that.</t>
+  </si>
+  <si>
+    <t>Yes, I can. The key is I can't take more than 3 hours under 5000 in Engineering.</t>
+  </si>
+  <si>
+    <t>Yes, look through the catalog and see what interests me then talk to Gerber about it</t>
+  </si>
+  <si>
+    <t>Just depends on where I am in my studies</t>
+  </si>
+  <si>
+    <t>No specific number. Just cover what is interesting to me.</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Organizing My Tasks</t>
+  </si>
+  <si>
+    <t>Messing around with JabRef</t>
+  </si>
+  <si>
+    <t>Finish a complete class plan</t>
+  </si>
+  <si>
+    <t>Organizing Course Catalog</t>
   </si>
 </sst>
 </file>
@@ -382,7 +421,7 @@
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -444,6 +483,7 @@
     <xf numFmtId="165" fontId="8" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma 2" xfId="3"/>
@@ -452,7 +492,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="31">
     <dxf>
       <fill>
         <patternFill>
@@ -523,6 +563,21 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -591,41 +646,44 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tasks" displayName="Tasks" ref="A1:G24" totalsRowShown="0">
-  <autoFilter ref="A1:G24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tasks" displayName="Tasks" ref="A1:G28" totalsRowShown="0">
+  <autoFilter ref="A1:G28">
     <filterColumn colId="4">
       <filters blank="1"/>
     </filterColumn>
   </autoFilter>
-  <sortState ref="A14:G24">
+  <sortState ref="A14:G28">
     <sortCondition ref="E2:E24"/>
     <sortCondition ref="D2:D24"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="8" name="Id" dataDxfId="25"/>
+    <tableColumn id="8" name="Id" dataDxfId="30"/>
     <tableColumn id="1" name="Description"/>
     <tableColumn id="2" name="Comments"/>
-    <tableColumn id="4" name="Due" dataDxfId="24"/>
-    <tableColumn id="5" name="Done" dataDxfId="23"/>
-    <tableColumn id="3" name="Report" dataDxfId="22"/>
-    <tableColumn id="6" name="Add" dataDxfId="21"/>
+    <tableColumn id="4" name="Due" dataDxfId="29"/>
+    <tableColumn id="5" name="Done" dataDxfId="28"/>
+    <tableColumn id="3" name="Report" dataDxfId="27"/>
+    <tableColumn id="6" name="Add" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:F3" totalsRowShown="0">
-  <autoFilter ref="A1:F3"/>
-  <tableColumns count="6">
-    <tableColumn id="2" name="TaskId"/>
-    <tableColumn id="3" name="Task">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:G7" totalsRowShown="0">
+  <autoFilter ref="A1:G7"/>
+  <tableColumns count="7">
+    <tableColumn id="4" name="Work"/>
+    <tableColumn id="5" name="Date"/>
+    <tableColumn id="6" name="Start" dataDxfId="13"/>
+    <tableColumn id="7" name="End" dataDxfId="12"/>
+    <tableColumn id="1" name="Hours" dataDxfId="11">
+      <calculatedColumnFormula>Table5[[#This Row],[End]]-Table5[[#This Row],[Start]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" name="TaskId" dataDxfId="10"/>
+    <tableColumn id="3" name="Task" dataDxfId="9">
       <calculatedColumnFormula>VLOOKUP(Table5[[#This Row],[TaskId]], Tasks[], 2, FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Work"/>
-    <tableColumn id="5" name="Date"/>
-    <tableColumn id="6" name="Start"/>
-    <tableColumn id="7" name="End"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -647,8 +705,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Updates" displayName="Updates" ref="A1:B2" totalsRowShown="0">
   <autoFilter ref="A1:B2"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Start" dataDxfId="20"/>
-    <tableColumn id="2" name="End" dataDxfId="19">
+    <tableColumn id="1" name="Start" dataDxfId="25"/>
+    <tableColumn id="2" name="End" dataDxfId="24">
       <calculatedColumnFormula>Updates[[#This Row],[Start]] + (7)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -664,14 +722,14 @@
     <sortCondition ref="G2:G21"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="2" name="Index" dataDxfId="18"/>
-    <tableColumn id="1" name="Description" dataDxfId="17">
+    <tableColumn id="2" name="Index" dataDxfId="23"/>
+    <tableColumn id="1" name="Description" dataDxfId="22">
       <calculatedColumnFormula array="1">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[Start])) * (NOT(ISBLANK(Tasks[Report]))) * ((Tasks[Done] &gt; MAX(Updates[Start])) + (ISBLANK(Tasks[Done]))),  Tasks[Description], "" ), COUNT(Tasks[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Done" dataDxfId="16">
+    <tableColumn id="3" name="Done" dataDxfId="21">
       <calculatedColumnFormula array="1">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[Start])) * (Tasks[Done] &gt; MAX(Updates[Start])) * (NOT(ISBLANK(Tasks[Done]))),  Tasks[Done], "" ), COUNT(Tasks[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Report" dataDxfId="15">
+    <tableColumn id="4" name="Report" dataDxfId="20">
       <calculatedColumnFormula array="1">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[Start])) * ((Tasks[Done] &gt; MAX(Updates[Start])) + (ISBLANK(Tasks[Done]))) * (NOT(ISBLANK(Tasks[Report]))),  Tasks[Report], "" ), COUNT(Tasks[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -686,14 +744,14 @@
     <sortCondition ref="L1:L21"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="2" name="Index" dataDxfId="14"/>
-    <tableColumn id="1" name="Description" dataDxfId="13">
+    <tableColumn id="2" name="Index" dataDxfId="19"/>
+    <tableColumn id="1" name="Description" dataDxfId="18">
       <calculatedColumnFormula array="1">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[End])) * (NOT(ISBLANK(Tasks[Report]))) * ISBLANK(Tasks[Done]),  Tasks[Description], "" ), COUNT(Tasks[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Done" dataDxfId="12">
+    <tableColumn id="3" name="Done" dataDxfId="17">
       <calculatedColumnFormula array="1">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[End])) * (Tasks[Done] &gt; MAX(Updates[End])) * (NOT(ISBLANK(Tasks[Done]))),  Tasks[Done], "" ), COUNT(Tasks[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Report" dataDxfId="11">
+    <tableColumn id="4" name="Report" dataDxfId="16">
       <calculatedColumnFormula array="1">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[End])) * (NOT(ISBLANK(Tasks[Report]))) * ISBLANK(Tasks[Done]),  Tasks[Report], "" ), COUNT(Tasks[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -708,8 +766,8 @@
     <sortCondition descending="1" ref="N1:N21"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="2" name="Index" dataDxfId="10"/>
-    <tableColumn id="1" name="Question" dataDxfId="9">
+    <tableColumn id="2" name="Index" dataDxfId="15"/>
+    <tableColumn id="1" name="Question" dataDxfId="14">
       <calculatedColumnFormula array="1">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1004,10 +1062,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1287,7 +1345,7 @@
         <v>48</v>
       </c>
       <c r="D14" s="2">
-        <v>42522</v>
+        <v>42529</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2">
@@ -1305,7 +1363,7 @@
         <v>11</v>
       </c>
       <c r="D15" s="2">
-        <v>42522</v>
+        <v>42529</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2">
@@ -1315,7 +1373,7 @@
         <v>42515</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1325,7 +1383,9 @@
       <c r="D16" s="2">
         <v>42522</v>
       </c>
-      <c r="E16" s="2"/>
+      <c r="E16" s="2">
+        <v>42524</v>
+      </c>
       <c r="F16" s="2">
         <v>42515</v>
       </c>
@@ -1333,7 +1393,7 @@
         <v>42515</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>23</v>
       </c>
@@ -1343,7 +1403,9 @@
       <c r="D17" s="2">
         <v>42522</v>
       </c>
-      <c r="E17" s="2"/>
+      <c r="E17" s="2">
+        <v>42524</v>
+      </c>
       <c r="F17" s="2">
         <v>42515</v>
       </c>
@@ -1353,80 +1415,85 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="D18" s="2">
-        <v>42577</v>
+        <v>42529</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="F18" s="2">
+        <v>42529</v>
+      </c>
       <c r="G18" s="2">
-        <v>42518</v>
+        <v>42524</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <v>17</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" t="s">
-        <v>10</v>
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
       </c>
       <c r="D19" s="2">
-        <v>42583</v>
+        <v>42529</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="F19" s="2">
+        <v>42529</v>
+      </c>
       <c r="G19" s="2">
-        <v>42518</v>
+        <v>42524</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="D20" s="2">
-        <v>42583</v>
+        <v>42529</v>
       </c>
       <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="F20" s="2">
+        <v>42529</v>
+      </c>
       <c r="G20" s="2">
-        <v>42518</v>
+        <v>42524</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="D21" s="2">
-        <v>42583</v>
+        <v>42529</v>
       </c>
       <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="F21" s="2">
+        <v>42529</v>
+      </c>
       <c r="G21" s="2">
-        <v>42518</v>
+        <v>42524</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D22" s="2">
-        <v>42583</v>
+        <v>42577</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -1436,10 +1503,13 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
       </c>
       <c r="D23" s="2">
         <v>42583</v>
@@ -1453,10 +1523,10 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D24" s="2">
         <v>42583</v>
@@ -1464,6 +1534,70 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2">
+        <v>42518</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="2">
+        <v>42583</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2">
+        <v>42518</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>20</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="2">
+        <v>42583</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2">
+        <v>42518</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>21</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="2">
+        <v>42583</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2">
+        <v>42518</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>22</v>
+      </c>
+      <c r="B28" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="2">
+        <v>42583</v>
+      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2">
         <v>42519</v>
       </c>
     </row>
@@ -1471,12 +1605,12 @@
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" location="heading=h.q544jq4bo7vu" display="https://docs.google.com/document/d/1WtVePtADr7xStL5Ac2lepzWibRBYoZs5Y_515wGqzFw/edit - heading=h.q544jq4bo7vu"/>
     <hyperlink ref="B7" r:id="rId2" location="heading=h.q544jq4bo7vu" display="https://docs.google.com/document/d/1WtVePtADr7xStL5Ac2lepzWibRBYoZs5Y_515wGqzFw/edit - heading=h.q544jq4bo7vu"/>
-    <hyperlink ref="B19" r:id="rId3" location="inbox/154e7d1ce0153b1e"/>
+    <hyperlink ref="B23" r:id="rId3" location="inbox/154e7d1ce0153b1e"/>
     <hyperlink ref="B11" r:id="rId4" location="heading=h.4uv9il96waak" display="https://docs.google.com/document/d/1WtVePtADr7xStL5Ac2lepzWibRBYoZs5Y_515wGqzFw/edit - heading=h.4uv9il96waak"/>
     <hyperlink ref="B12" r:id="rId5" location="heading=h.kwuhphhohs6l" display="https://docs.google.com/document/d/1WtVePtADr7xStL5Ac2lepzWibRBYoZs5Y_515wGqzFw/edit - heading=h.kwuhphhohs6l"/>
     <hyperlink ref="B13" r:id="rId6" location="heading=h.kwuhphhohs6l" display="https://docs.google.com/document/d/1WtVePtADr7xStL5Ac2lepzWibRBYoZs5Y_515wGqzFw/edit - heading=h.kwuhphhohs6l"/>
     <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B23" r:id="rId8"/>
+    <hyperlink ref="B27" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId9"/>
@@ -1488,93 +1622,204 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" customWidth="1"/>
-    <col min="3" max="3" width="70.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="55.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="56.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
         <v>38</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="3">
+        <v>42521</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E2" s="6">
+        <f>Table5[[#This Row],[End]]-Table5[[#This Row],[Start]]</f>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="F2">
         <v>23</v>
       </c>
-      <c r="B2" t="str">
+      <c r="G2" t="str">
         <f>VLOOKUP(Table5[[#This Row],[TaskId]], Tasks[], 2, FALSE)</f>
         <v>Create Task Spreadsheet</v>
       </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="3">
-        <v>42521</v>
-      </c>
-      <c r="E2" s="6">
-        <v>0.625</v>
-      </c>
-      <c r="F2" s="6">
-        <v>0.70833333333333337</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="3">
+        <v>42522</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E3" s="6">
+        <f>Table5[[#This Row],[End]]-Table5[[#This Row],[Start]]</f>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="F3">
         <v>23</v>
       </c>
-      <c r="B3" t="str">
+      <c r="G3" t="str">
         <f>VLOOKUP(Table5[[#This Row],[TaskId]], Tasks[], 2, FALSE)</f>
         <v>Create Task Spreadsheet</v>
       </c>
-      <c r="C3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="3">
-        <v>42522</v>
-      </c>
-      <c r="E3" s="6">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="F3" s="6">
-        <v>0.52083333333333337</v>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="3">
+        <v>42524</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0.71875</v>
+      </c>
+      <c r="E4" s="6">
+        <f>Table5[[#This Row],[End]]-Table5[[#This Row],[Start]]</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="G4" t="e">
+        <f>VLOOKUP(Table5[[#This Row],[TaskId]], Tasks[], 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="3">
+        <v>42524</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.71875</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="E5" s="6">
+        <f>Table5[[#This Row],[End]]-Table5[[#This Row],[Start]]</f>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="F5">
+        <v>24</v>
+      </c>
+      <c r="G5" t="str">
+        <f>VLOOKUP(Table5[[#This Row],[TaskId]], Tasks[], 2, FALSE)</f>
+        <v>Read all article Abstracts</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="3">
+        <v>42524</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.78125</v>
+      </c>
+      <c r="E6" s="6">
+        <f>Table5[[#This Row],[End]]-Table5[[#This Row],[Start]]</f>
+        <v>5.208333333333337E-2</v>
+      </c>
+      <c r="F6" s="47">
+        <v>27</v>
+      </c>
+      <c r="G6" s="6" t="str">
+        <f>VLOOKUP(Table5[[#This Row],[TaskId]], Tasks[], 2, FALSE)</f>
+        <v>Finish a complete class plan</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="3">
+        <v>42525</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="E7" s="6">
+        <f>Table5[[#This Row],[End]]-Table5[[#This Row],[Start]]</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F7" s="47">
+        <v>27</v>
+      </c>
+      <c r="G7" s="6" t="str">
+        <f>VLOOKUP(Table5[[#This Row],[TaskId]], Tasks[], 2, FALSE)</f>
+        <v>Finish a complete class plan</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A2:A3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="F2:F7">
       <formula1>TaskIds</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" sqref="B2:B3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" sqref="G2:G7"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1584,13 +1829,13 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="65.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.28515625" customWidth="1"/>
+    <col min="2" max="2" width="83" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1608,25 +1853,55 @@
       <c r="A2" t="s">
         <v>23</v>
       </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="3">
+        <v>42522</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="3">
+        <v>42522</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="3">
+        <v>42522</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="3">
+        <v>42522</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="3">
+        <v>42522</v>
       </c>
     </row>
   </sheetData>
@@ -1710,11 +1985,11 @@
       </c>
       <c r="E2" t="str">
         <f t="array" ref="E2">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[Start])) * (NOT(ISBLANK(Tasks[Report]))) * ((Tasks[Done] &gt; MAX(Updates[Start])) + (ISBLANK(Tasks[Done]))),  Tasks[Description], "" ), COUNT(Tasks[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>Create Linux instance on AWS with R installed</v>
-      </c>
-      <c r="F2" s="2">
+        <v>Introduction to Statistical Learning Chp 2</v>
+      </c>
+      <c r="F2" s="2" t="str">
         <f t="array" ref="F2">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[Start])) * (Tasks[Done] &gt; MAX(Updates[Start])) * (NOT(ISBLANK(Tasks[Done]))),  Tasks[Done], "" ), COUNT(Tasks[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>42516</v>
+        <v/>
       </c>
       <c r="G2" s="2">
         <f t="array" ref="G2">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[Start])) * ((Tasks[Done] &gt; MAX(Updates[Start])) + (ISBLANK(Tasks[Done]))) * (NOT(ISBLANK(Tasks[Report]))),  Tasks[Report], "" ), COUNT(Tasks[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
@@ -1726,22 +2001,22 @@
       </c>
       <c r="J2" t="str">
         <f t="array" ref="J2">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[End])) * (NOT(ISBLANK(Tasks[Report]))) * ISBLANK(Tasks[Done]),  Tasks[Description], "" ), COUNT(Tasks[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>Reinforcement Learning an Introduction</v>
+        <v/>
       </c>
       <c r="K2" s="2" t="str">
         <f t="array" ref="K2">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[End])) * (Tasks[Done] &gt; MAX(Updates[End])) * (NOT(ISBLANK(Tasks[Done]))),  Tasks[Done], "" ), COUNT(Tasks[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
         <v/>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="2" t="str">
         <f t="array" ref="L2">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[End])) * (NOT(ISBLANK(Tasks[Report]))) * ISBLANK(Tasks[Done]),  Tasks[Report], "" ), COUNT(Tasks[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>42515</v>
+        <v/>
       </c>
       <c r="N2" s="5">
         <v>-1</v>
       </c>
       <c r="O2" t="str">
         <f t="array" ref="O2">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v>How many articles should I cover in my survey presentation?</v>
+        <v/>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1751,15 +2026,15 @@
       </c>
       <c r="E3" t="str">
         <f t="array" ref="E3">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[Start])) * (NOT(ISBLANK(Tasks[Report]))) * ((Tasks[Done] &gt; MAX(Updates[Start])) + (ISBLANK(Tasks[Done]))),  Tasks[Description], "" ), COUNT(Tasks[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>Create thesis plan</v>
+        <v>Create Task Spreadsheet</v>
       </c>
       <c r="F3" s="2">
         <f t="array" ref="F3">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[Start])) * (Tasks[Done] &gt; MAX(Updates[Start])) * (NOT(ISBLANK(Tasks[Done]))),  Tasks[Done], "" ), COUNT(Tasks[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>42519</v>
+        <v>42524</v>
       </c>
       <c r="G3" s="2">
         <f t="array" ref="G3">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[Start])) * ((Tasks[Done] &gt; MAX(Updates[Start])) + (ISBLANK(Tasks[Done]))) * (NOT(ISBLANK(Tasks[Report]))),  Tasks[Report], "" ), COUNT(Tasks[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>42508</v>
+        <v>42515</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="5">
@@ -1767,22 +2042,22 @@
       </c>
       <c r="J3" t="str">
         <f t="array" ref="J3">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[End])) * (NOT(ISBLANK(Tasks[Report]))) * ISBLANK(Tasks[Done]),  Tasks[Description], "" ), COUNT(Tasks[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>Introduction to Statistical Learning Chp 2</v>
+        <v/>
       </c>
       <c r="K3" s="2" t="str">
         <f t="array" ref="K3">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[End])) * (Tasks[Done] &gt; MAX(Updates[End])) * (NOT(ISBLANK(Tasks[Done]))),  Tasks[Done], "" ), COUNT(Tasks[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
         <v/>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="2" t="str">
         <f t="array" ref="L3">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[End])) * (NOT(ISBLANK(Tasks[Report]))) * ISBLANK(Tasks[Done]),  Tasks[Report], "" ), COUNT(Tasks[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>42515</v>
+        <v/>
       </c>
       <c r="N3" s="5">
         <v>-2</v>
       </c>
       <c r="O3" t="str">
         <f t="array" ref="O3">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v>What pace should I be going through these articles?</v>
+        <v/>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1791,15 +2066,15 @@
       </c>
       <c r="E4" t="str">
         <f t="array" ref="E4">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[Start])) * (NOT(ISBLANK(Tasks[Report]))) * ((Tasks[Done] &gt; MAX(Updates[Start])) + (ISBLANK(Tasks[Done]))),  Tasks[Description], "" ), COUNT(Tasks[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>Create publication plan</v>
+        <v>Determine Appropriate Pace for Article Survey</v>
       </c>
       <c r="F4" s="2">
         <f t="array" ref="F4">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[Start])) * (Tasks[Done] &gt; MAX(Updates[Start])) * (NOT(ISBLANK(Tasks[Done]))),  Tasks[Done], "" ), COUNT(Tasks[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>42519</v>
+        <v>42524</v>
       </c>
       <c r="G4" s="2">
         <f t="array" ref="G4">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[Start])) * ((Tasks[Done] &gt; MAX(Updates[Start])) + (ISBLANK(Tasks[Done]))) * (NOT(ISBLANK(Tasks[Report]))),  Tasks[Report], "" ), COUNT(Tasks[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>42508</v>
+        <v>42515</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="5">
@@ -1807,22 +2082,22 @@
       </c>
       <c r="J4" t="str">
         <f t="array" ref="J4">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[End])) * (NOT(ISBLANK(Tasks[Report]))) * ISBLANK(Tasks[Done]),  Tasks[Description], "" ), COUNT(Tasks[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>Determine Appropriate Pace for Article Survey</v>
+        <v/>
       </c>
       <c r="K4" s="2" t="str">
         <f t="array" ref="K4">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[End])) * (Tasks[Done] &gt; MAX(Updates[End])) * (NOT(ISBLANK(Tasks[Done]))),  Tasks[Done], "" ), COUNT(Tasks[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
         <v/>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="2" t="str">
         <f t="array" ref="L4">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[End])) * (NOT(ISBLANK(Tasks[Report]))) * ISBLANK(Tasks[Done]),  Tasks[Report], "" ), COUNT(Tasks[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>42515</v>
+        <v/>
       </c>
       <c r="N4" s="5">
         <v>-3</v>
       </c>
       <c r="O4" t="str">
         <f t="array" ref="O4">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v>Do I want any Sociology/Policy Classes for a CHS focus?</v>
+        <v/>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1831,15 +2106,15 @@
       </c>
       <c r="E5" t="str">
         <f t="array" ref="E5">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[Start])) * (NOT(ISBLANK(Tasks[Report]))) * ((Tasks[Done] &gt; MAX(Updates[Start])) + (ISBLANK(Tasks[Done]))),  Tasks[Description], "" ), COUNT(Tasks[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>Create curriculum plan</v>
-      </c>
-      <c r="F5" s="2">
+        <v>Reinforcement Learning an Introduction</v>
+      </c>
+      <c r="F5" s="2" t="str">
         <f t="array" ref="F5">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[Start])) * (Tasks[Done] &gt; MAX(Updates[Start])) * (NOT(ISBLANK(Tasks[Done]))),  Tasks[Done], "" ), COUNT(Tasks[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>42519</v>
+        <v/>
       </c>
       <c r="G5" s="2">
         <f t="array" ref="G5">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[Start])) * ((Tasks[Done] &gt; MAX(Updates[Start])) + (ISBLANK(Tasks[Done]))) * (NOT(ISBLANK(Tasks[Report]))),  Tasks[Report], "" ), COUNT(Tasks[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>42508</v>
+        <v>42515</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="5">
@@ -1847,22 +2122,22 @@
       </c>
       <c r="J5" t="str">
         <f t="array" ref="J5">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[End])) * (NOT(ISBLANK(Tasks[Report]))) * ISBLANK(Tasks[Done]),  Tasks[Description], "" ), COUNT(Tasks[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>Create Task Spreadsheet</v>
+        <v/>
       </c>
       <c r="K5" s="2" t="str">
         <f t="array" ref="K5">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[End])) * (Tasks[Done] &gt; MAX(Updates[End])) * (NOT(ISBLANK(Tasks[Done]))),  Tasks[Done], "" ), COUNT(Tasks[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
         <v/>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="2" t="str">
         <f t="array" ref="L5">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[End])) * (NOT(ISBLANK(Tasks[Report]))) * ISBLANK(Tasks[Done]),  Tasks[Report], "" ), COUNT(Tasks[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>42515</v>
+        <v/>
       </c>
       <c r="N5" s="5">
         <v>-4</v>
       </c>
       <c r="O5" t="str">
         <f t="array" ref="O5">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v>Can I take non SYS classes to meet Course requirements? (e.g., CS 6316)</v>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1871,15 +2146,15 @@
       </c>
       <c r="E6" t="str">
         <f t="array" ref="E6">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[Start])) * (NOT(ISBLANK(Tasks[Report]))) * ((Tasks[Done] &gt; MAX(Updates[Start])) + (ISBLANK(Tasks[Done]))),  Tasks[Description], "" ), COUNT(Tasks[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>Reinforcement Learning an Introduction</v>
+        <v/>
       </c>
       <c r="F6" s="2" t="str">
         <f t="array" ref="F6">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[Start])) * (Tasks[Done] &gt; MAX(Updates[Start])) * (NOT(ISBLANK(Tasks[Done]))),  Tasks[Done], "" ), COUNT(Tasks[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
         <v/>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="2" t="str">
         <f t="array" ref="G6">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[Start])) * ((Tasks[Done] &gt; MAX(Updates[Start])) + (ISBLANK(Tasks[Done]))) * (NOT(ISBLANK(Tasks[Report]))),  Tasks[Report], "" ), COUNT(Tasks[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>42515</v>
+        <v/>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="5">
@@ -1902,7 +2177,7 @@
       </c>
       <c r="O6" t="str">
         <f t="array" ref="O6">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v>Do I want to rework my course schedule skipping summer 2017?</v>
+        <v/>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1911,15 +2186,15 @@
       </c>
       <c r="E7" t="str">
         <f t="array" ref="E7">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[Start])) * (NOT(ISBLANK(Tasks[Report]))) * ((Tasks[Done] &gt; MAX(Updates[Start])) + (ISBLANK(Tasks[Done]))),  Tasks[Description], "" ), COUNT(Tasks[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>Introduction to Statistical Learning Chp 2</v>
+        <v/>
       </c>
       <c r="F7" s="2" t="str">
         <f t="array" ref="F7">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[Start])) * (Tasks[Done] &gt; MAX(Updates[Start])) * (NOT(ISBLANK(Tasks[Done]))),  Tasks[Done], "" ), COUNT(Tasks[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
         <v/>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="2" t="str">
         <f t="array" ref="G7">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[Start])) * ((Tasks[Done] &gt; MAX(Updates[Start])) + (ISBLANK(Tasks[Done]))) * (NOT(ISBLANK(Tasks[Report]))),  Tasks[Report], "" ), COUNT(Tasks[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>42515</v>
+        <v/>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="5">
@@ -1949,15 +2224,15 @@
       </c>
       <c r="E8" t="str">
         <f t="array" ref="E8">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[Start])) * (NOT(ISBLANK(Tasks[Report]))) * ((Tasks[Done] &gt; MAX(Updates[Start])) + (ISBLANK(Tasks[Done]))),  Tasks[Description], "" ), COUNT(Tasks[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>Determine Appropriate Pace for Article Survey</v>
+        <v/>
       </c>
       <c r="F8" s="2" t="str">
         <f t="array" ref="F8">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[Start])) * (Tasks[Done] &gt; MAX(Updates[Start])) * (NOT(ISBLANK(Tasks[Done]))),  Tasks[Done], "" ), COUNT(Tasks[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
         <v/>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="2" t="str">
         <f t="array" ref="G8">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[Start])) * ((Tasks[Done] &gt; MAX(Updates[Start])) + (ISBLANK(Tasks[Done]))) * (NOT(ISBLANK(Tasks[Report]))),  Tasks[Report], "" ), COUNT(Tasks[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>42515</v>
+        <v/>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="5">
@@ -1989,15 +2264,15 @@
       </c>
       <c r="E9" t="str">
         <f t="array" ref="E9">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[Start])) * (NOT(ISBLANK(Tasks[Report]))) * ((Tasks[Done] &gt; MAX(Updates[Start])) + (ISBLANK(Tasks[Done]))),  Tasks[Description], "" ), COUNT(Tasks[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>Create Task Spreadsheet</v>
+        <v/>
       </c>
       <c r="F9" s="2" t="str">
         <f t="array" ref="F9">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[Start])) * (Tasks[Done] &gt; MAX(Updates[Start])) * (NOT(ISBLANK(Tasks[Done]))),  Tasks[Done], "" ), COUNT(Tasks[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
         <v/>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="2" t="str">
         <f t="array" ref="G9">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[Start])) * ((Tasks[Done] &gt; MAX(Updates[Start])) + (ISBLANK(Tasks[Done]))) * (NOT(ISBLANK(Tasks[Report]))),  Tasks[Report], "" ), COUNT(Tasks[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>42515</v>
+        <v/>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="5">
@@ -2160,9 +2435,9 @@
         <f t="array" ref="J13">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[End])) * (NOT(ISBLANK(Tasks[Report]))) * ISBLANK(Tasks[Done]),  Tasks[Description], "" ), COUNT(Tasks[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
         <v/>
       </c>
-      <c r="K13" s="2" t="str">
+      <c r="K13" s="2">
         <f t="array" ref="K13">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[End])) * (Tasks[Done] &gt; MAX(Updates[End])) * (NOT(ISBLANK(Tasks[Done]))),  Tasks[Done], "" ), COUNT(Tasks[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
+        <v>42524</v>
       </c>
       <c r="L13" s="2" t="str">
         <f t="array" ref="L13">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[End])) * (NOT(ISBLANK(Tasks[Report]))) * ISBLANK(Tasks[Done]),  Tasks[Report], "" ), COUNT(Tasks[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
@@ -2193,9 +2468,9 @@
         <f t="array" ref="J14">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[End])) * (NOT(ISBLANK(Tasks[Report]))) * ISBLANK(Tasks[Done]),  Tasks[Description], "" ), COUNT(Tasks[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
         <v/>
       </c>
-      <c r="K14" s="2" t="str">
+      <c r="K14" s="2">
         <f t="array" ref="K14">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[End])) * (Tasks[Done] &gt; MAX(Updates[End])) * (NOT(ISBLANK(Tasks[Done]))),  Tasks[Done], "" ), COUNT(Tasks[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
+        <v>42524</v>
       </c>
       <c r="L14" s="2" t="str">
         <f t="array" ref="L14">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[End])) * (NOT(ISBLANK(Tasks[Report]))) * ISBLANK(Tasks[Done]),  Tasks[Report], "" ), COUNT(Tasks[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
@@ -2224,15 +2499,15 @@
       </c>
       <c r="J15" t="str">
         <f t="array" ref="J15">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[End])) * (NOT(ISBLANK(Tasks[Report]))) * ISBLANK(Tasks[Done]),  Tasks[Description], "" ), COUNT(Tasks[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
+        <v>Reinforcement Learning an Introduction</v>
       </c>
       <c r="K15" s="2" t="str">
         <f t="array" ref="K15">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[End])) * (Tasks[Done] &gt; MAX(Updates[End])) * (NOT(ISBLANK(Tasks[Done]))),  Tasks[Done], "" ), COUNT(Tasks[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
         <v/>
       </c>
-      <c r="L15" s="2" t="str">
+      <c r="L15" s="2">
         <f t="array" ref="L15">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[End])) * (NOT(ISBLANK(Tasks[Report]))) * ISBLANK(Tasks[Done]),  Tasks[Report], "" ), COUNT(Tasks[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
+        <v>42515</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -2257,15 +2532,15 @@
       </c>
       <c r="J16" t="str">
         <f t="array" ref="J16">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[End])) * (NOT(ISBLANK(Tasks[Report]))) * ISBLANK(Tasks[Done]),  Tasks[Description], "" ), COUNT(Tasks[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
+        <v>Introduction to Statistical Learning Chp 2</v>
       </c>
       <c r="K16" s="2" t="str">
         <f t="array" ref="K16">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[End])) * (Tasks[Done] &gt; MAX(Updates[End])) * (NOT(ISBLANK(Tasks[Done]))),  Tasks[Done], "" ), COUNT(Tasks[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
         <v/>
       </c>
-      <c r="L16" s="2" t="str">
+      <c r="L16" s="2">
         <f t="array" ref="L16">INDEX(IF((Tasks[Report] &lt;= MAX(Updates[End])) * (NOT(ISBLANK(Tasks[Report]))) * ISBLANK(Tasks[Done]),  Tasks[Report], "" ), COUNT(Tasks[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
+        <v>42515</v>
       </c>
     </row>
     <row r="17" spans="8:8" x14ac:dyDescent="0.25">
@@ -2298,8 +2573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" view="pageLayout" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView showGridLines="0" showRuler="0" view="pageLayout" topLeftCell="A3" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2370,19 +2645,19 @@
     <row r="4" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="str">
         <f t="array" ref="A4:A18">LastWeekTasks[Description]</f>
-        <v>Create Linux instance on AWS with R installed</v>
+        <v>Introduction to Statistical Learning Chp 2</v>
       </c>
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
-      <c r="E4" s="33">
+      <c r="E4" s="33" t="str">
         <f t="array" ref="E4:E18">LastWeekTasks[Done]</f>
-        <v>42516</v>
+        <v/>
       </c>
       <c r="F4" s="17"/>
       <c r="H4" s="26" t="str">
         <f t="array" ref="H4:H18">ThisWeekTasks[Description]</f>
-        <v>Reinforcement Learning an Introduction</v>
+        <v/>
       </c>
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
@@ -2390,17 +2665,17 @@
     </row>
     <row r="5" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="str">
-        <v>Create thesis plan</v>
+        <v>Create Task Spreadsheet</v>
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
       <c r="E5" s="34">
-        <v>42519</v>
+        <v>42524</v>
       </c>
       <c r="F5" s="16"/>
       <c r="H5" s="27" t="str">
-        <v>Introduction to Statistical Learning Chp 2</v>
+        <v/>
       </c>
       <c r="I5" s="19"/>
       <c r="J5" s="19"/>
@@ -2409,17 +2684,17 @@
     </row>
     <row r="6" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="28" t="str">
-        <v>Create publication plan</v>
+        <v>Determine Appropriate Pace for Article Survey</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="33">
-        <v>42519</v>
+        <v>42524</v>
       </c>
       <c r="F6" s="16"/>
       <c r="H6" s="28" t="str">
-        <v>Determine Appropriate Pace for Article Survey</v>
+        <v/>
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
@@ -2428,17 +2703,17 @@
     </row>
     <row r="7" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="28" t="str">
-        <v>Create curriculum plan</v>
+        <v>Reinforcement Learning an Introduction</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
-      <c r="E7" s="33">
-        <v>42519</v>
+      <c r="E7" s="33" t="str">
+        <v/>
       </c>
       <c r="F7" s="16"/>
       <c r="H7" s="28" t="str">
-        <v>Create Task Spreadsheet</v>
+        <v/>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -2447,7 +2722,7 @@
     </row>
     <row r="8" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="28" t="str">
-        <v>Reinforcement Learning an Introduction</v>
+        <v/>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -2467,7 +2742,7 @@
     </row>
     <row r="9" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="28" t="str">
-        <v>Introduction to Statistical Learning Chp 2</v>
+        <v/>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -2487,7 +2762,7 @@
     </row>
     <row r="10" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="28" t="str">
-        <v>Determine Appropriate Pace for Article Survey</v>
+        <v/>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -2507,7 +2782,7 @@
     </row>
     <row r="11" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="28" t="str">
-        <v>Create Task Spreadsheet</v>
+        <v/>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -2638,7 +2913,7 @@
       <c r="F17" s="13"/>
       <c r="G17" s="14"/>
       <c r="H17" s="20" t="str">
-        <v/>
+        <v>Reinforcement Learning an Introduction</v>
       </c>
       <c r="I17" s="20"/>
       <c r="J17" s="20"/>
@@ -2658,7 +2933,7 @@
       <c r="F18" s="13"/>
       <c r="G18" s="14"/>
       <c r="H18" s="20" t="str">
-        <v/>
+        <v>Introduction to Statistical Learning Chp 2</v>
       </c>
       <c r="I18" s="20"/>
       <c r="J18" s="20"/>
@@ -2700,7 +2975,7 @@
     <row r="21" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A21" s="26" t="str">
         <f t="array" ref="A21:A30">ThisWeekQuestions[Question]</f>
-        <v>How many articles should I cover in my survey presentation?</v>
+        <v/>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -2717,7 +2992,7 @@
     </row>
     <row r="22" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A22" s="27" t="str">
-        <v>What pace should I be going through these articles?</v>
+        <v/>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -2734,7 +3009,7 @@
     </row>
     <row r="23" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A23" s="28" t="str">
-        <v>Do I want any Sociology/Policy Classes for a CHS focus?</v>
+        <v/>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -2751,7 +3026,7 @@
     </row>
     <row r="24" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="str">
-        <v>Can I take non SYS classes to meet Course requirements? (e.g., CS 6316)</v>
+        <v/>
       </c>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -2768,7 +3043,7 @@
     </row>
     <row r="25" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A25" s="28" t="str">
-        <v>Do I want to rework my course schedule skipping summer 2017?</v>
+        <v/>
       </c>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>

</xml_diff>

<commit_message>
Revising publication plan for earlier conference submission
</commit_message>
<xml_diff>
--- a/updates/Updates.xlsx
+++ b/updates/Updates.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="71">
   <si>
     <t>Install JabRef on my personal machine</t>
   </si>
@@ -189,24 +189,6 @@
   </si>
   <si>
     <t>Scanning Courses From Other Departments</t>
-  </si>
-  <si>
-    <t>Which week do I plan on completing a task?</t>
-  </si>
-  <si>
-    <t>Which week do I plan on starting to work on a task?</t>
-  </si>
-  <si>
-    <t>If I worked on it in a week show in last week</t>
-  </si>
-  <si>
-    <t>If I showed it in last week but didn't finish show in next week</t>
-  </si>
-  <si>
-    <t>Last Week -- everything I worked on</t>
-  </si>
-  <si>
-    <t>Next Week -- whatever I choose to put here</t>
   </si>
   <si>
     <t>Period</t>
@@ -512,23 +494,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="41">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="40">
     <dxf>
       <border>
         <right style="thin">
@@ -655,6 +621,22 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -663,9 +645,6 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -743,13 +722,13 @@
     <sortCondition ref="D2:D24"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="8" name="Id" dataDxfId="40"/>
+    <tableColumn id="8" name="Id" dataDxfId="39"/>
     <tableColumn id="1" name="Description"/>
     <tableColumn id="2" name="Comments"/>
-    <tableColumn id="4" name="Due" dataDxfId="39"/>
-    <tableColumn id="3" name="Started" dataDxfId="38"/>
-    <tableColumn id="5" name="Finished" dataDxfId="37"/>
-    <tableColumn id="6" name="Added" dataDxfId="36"/>
+    <tableColumn id="4" name="Due" dataDxfId="38"/>
+    <tableColumn id="3" name="Started" dataDxfId="37"/>
+    <tableColumn id="5" name="Finished" dataDxfId="36"/>
+    <tableColumn id="6" name="Added" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -762,13 +741,13 @@
     <tableColumn id="4" name="Work"/>
     <tableColumn id="9" name="Period"/>
     <tableColumn id="5" name="Date"/>
-    <tableColumn id="6" name="Start" dataDxfId="35"/>
-    <tableColumn id="7" name="End" dataDxfId="34"/>
-    <tableColumn id="1" name="Hours" dataDxfId="33">
+    <tableColumn id="6" name="Start" dataDxfId="34"/>
+    <tableColumn id="7" name="End" dataDxfId="33"/>
+    <tableColumn id="1" name="Hours" dataDxfId="32">
       <calculatedColumnFormula>Times[[#This Row],[End]]-Times[[#This Row],[Start]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Goal" dataDxfId="32"/>
-    <tableColumn id="3" name="Goal Description" dataDxfId="31">
+    <tableColumn id="2" name="Goal" dataDxfId="31"/>
+    <tableColumn id="3" name="Goal Description" dataDxfId="30">
       <calculatedColumnFormula>VLOOKUP(Times[[#This Row],[Goal]], Goals[], 2, FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -792,9 +771,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Periods" displayName="Periods" ref="A1:C6" totalsRowShown="0">
   <autoFilter ref="A1:C6"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Id" dataDxfId="30"/>
-    <tableColumn id="2" name="Start" dataDxfId="29"/>
-    <tableColumn id="3" name="End" dataDxfId="28">
+    <tableColumn id="1" name="Id" dataDxfId="29"/>
+    <tableColumn id="2" name="Start" dataDxfId="28"/>
+    <tableColumn id="3" name="End" dataDxfId="27">
       <calculatedColumnFormula>Periods[[#This Row],[Start]] + (7)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -809,20 +788,20 @@
     <sortCondition descending="1" ref="J1:J21"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="2" name="Index" dataDxfId="27"/>
-    <tableColumn id="4" name="Period" dataDxfId="26">
+    <tableColumn id="2" name="Index" dataDxfId="26"/>
+    <tableColumn id="4" name="Period" dataDxfId="25">
       <calculatedColumnFormula>MAX(Periods[Id]) -1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Goal" dataDxfId="25">
+    <tableColumn id="5" name="Goal" dataDxfId="24">
       <calculatedColumnFormula array="1">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Goal Description" dataDxfId="2">
+    <tableColumn id="1" name="Goal Description" dataDxfId="17">
       <calculatedColumnFormula>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Hours" dataDxfId="3">
+    <tableColumn id="6" name="Hours" dataDxfId="18">
       <calculatedColumnFormula array="1">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Done" dataDxfId="1">
+    <tableColumn id="3" name="Done" dataDxfId="16">
       <calculatedColumnFormula>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -831,24 +810,21 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="ThisWeekTasks" displayName="ThisWeekTasks" ref="L1:P21" totalsRowShown="0">
-  <autoFilter ref="L1:P21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="ThisWeekTasks" displayName="ThisWeekTasks" ref="L1:O21" totalsRowShown="0">
+  <autoFilter ref="L1:O21"/>
   <sortState ref="L2:P21">
     <sortCondition descending="1" ref="O1:O21"/>
   </sortState>
-  <tableColumns count="5">
-    <tableColumn id="2" name="Index" dataDxfId="24"/>
+  <tableColumns count="4">
+    <tableColumn id="2" name="Index" dataDxfId="23"/>
     <tableColumn id="6" name="Period" dataDxfId="20">
       <calculatedColumnFormula>MAX(Periods[Id])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Goal" dataDxfId="4">
+    <tableColumn id="5" name="Goal" dataDxfId="19">
       <calculatedColumnFormula array="1">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Description" dataDxfId="0">
+    <tableColumn id="1" name="Description" dataDxfId="15">
       <calculatedColumnFormula>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" name="Done" dataDxfId="23">
-      <calculatedColumnFormula array="1">INDEX(IF((Goals[Started] &lt;= MAX(Periods[Start])) * (Goals[Finished] &gt; MAX(Periods[Start])) * (NOT(ISBLANK(Goals[Finished]))),  Goals[Finished], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -856,10 +832,10 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="ThisWeekQuestions" displayName="ThisWeekQuestions" ref="R1:S11" totalsRowShown="0">
-  <autoFilter ref="R1:S11"/>
-  <sortState ref="R2:S21">
-    <sortCondition descending="1" ref="R1:R21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="ThisWeekQuestions" displayName="ThisWeekQuestions" ref="Q1:R11" totalsRowShown="0">
+  <autoFilter ref="Q1:R11"/>
+  <sortState ref="Q2:R21">
+    <sortCondition descending="1" ref="Q1:Q21"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="2" name="Index" dataDxfId="22"/>
@@ -1161,7 +1137,7 @@
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1176,7 +1152,7 @@
     <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -1190,20 +1166,20 @@
         <v>33</v>
       </c>
       <c r="E1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="G1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="I1" t="str">
         <f xml:space="preserve"> "Current Period: " &amp; MAX(Periods[Id]) -1</f>
         <v>Current Period: 4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1223,7 +1199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1243,7 +1219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1263,12 +1239,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D5" s="2">
         <v>42509</v>
@@ -1282,11 +1258,8 @@
       <c r="G5" s="30">
         <v>1</v>
       </c>
-      <c r="K5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1305,11 +1278,8 @@
       <c r="G6" s="30">
         <v>1</v>
       </c>
-      <c r="K6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1329,7 +1299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>8</v>
       </c>
@@ -1348,11 +1318,8 @@
       <c r="G8" s="30">
         <v>2</v>
       </c>
-      <c r="K8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>9</v>
       </c>
@@ -1371,11 +1338,8 @@
       <c r="G9" s="30">
         <v>3</v>
       </c>
-      <c r="K9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>7</v>
       </c>
@@ -1395,7 +1359,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1414,11 +1378,8 @@
       <c r="G11" s="30">
         <v>2</v>
       </c>
-      <c r="K11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1437,11 +1398,8 @@
       <c r="G12" s="30">
         <v>2</v>
       </c>
-      <c r="K12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1461,7 +1419,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>23</v>
       </c>
@@ -1481,12 +1439,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D15" s="2">
         <v>42522</v>
@@ -1501,7 +1459,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>13</v>
       </c>
@@ -1580,7 +1538,7 @@
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D20" s="2">
         <v>42529</v>
@@ -1588,7 +1546,9 @@
       <c r="E20" s="30">
         <v>4</v>
       </c>
-      <c r="F20" s="30"/>
+      <c r="F20" s="30">
+        <v>4</v>
+      </c>
       <c r="G20" s="30">
         <v>4</v>
       </c>
@@ -1616,7 +1576,7 @@
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D22" s="2">
         <v>42577</v>
@@ -1732,7 +1692,7 @@
         <v>999</v>
       </c>
       <c r="B29" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="30"/>
@@ -1782,7 +1742,7 @@
         <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C1" t="s">
         <v>23</v>
@@ -1797,10 +1757,10 @@
         <v>51</v>
       </c>
       <c r="G1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2001,7 +1961,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -2029,7 +1989,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -2158,10 +2118,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S21"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2181,11 +2141,11 @@
     <col min="13" max="13" width="5" customWidth="1"/>
     <col min="14" max="14" width="6" customWidth="1"/>
     <col min="15" max="15" width="43.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.42578125" customWidth="1"/>
-    <col min="19" max="19" width="65.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.42578125" customWidth="1"/>
+    <col min="18" max="18" width="65.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -2199,13 +2159,13 @@
         <v>39</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="I1" t="s">
         <v>51</v>
@@ -2217,25 +2177,22 @@
         <v>39</v>
       </c>
       <c r="M1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="N1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="O1" t="s">
         <v>29</v>
       </c>
-      <c r="P1" t="s">
-        <v>34</v>
+      <c r="Q1" t="s">
+        <v>39</v>
       </c>
       <c r="R1" t="s">
-        <v>39</v>
-      </c>
-      <c r="S1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="30">
         <v>1</v>
       </c>
@@ -2286,19 +2243,15 @@
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v>Reinforcement Learning an Introduction</v>
       </c>
-      <c r="P2" s="2" t="str">
-        <f t="array" ref="P2">INDEX(IF((Goals[Started] &lt;= MAX(Periods[Start])) * (Goals[Finished] &gt; MAX(Periods[Start])) * (NOT(ISBLANK(Goals[Finished]))),  Goals[Finished], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="R2" s="5">
+      <c r="Q2" s="5">
         <v>-1</v>
       </c>
-      <c r="S2" t="str">
-        <f t="array" ref="S2">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R2" t="str">
+        <f t="array" ref="R2">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="30">
         <v>2</v>
       </c>
@@ -2331,7 +2284,7 @@
       </c>
       <c r="J3" s="30" t="b">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="5">
@@ -2349,19 +2302,15 @@
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v>Read all article Abstracts</v>
       </c>
-      <c r="P3" s="2" t="str">
-        <f t="array" ref="P3">INDEX(IF((Goals[Started] &lt;= MAX(Periods[Start])) * (Goals[Finished] &gt; MAX(Periods[Start])) * (NOT(ISBLANK(Goals[Finished]))),  Goals[Finished], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="R3" s="5">
+      <c r="Q3" s="5">
         <v>-2</v>
       </c>
-      <c r="S3" t="str">
-        <f t="array" ref="S3">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R3" t="str">
+        <f t="array" ref="R3">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="30">
         <v>3</v>
       </c>
@@ -2411,19 +2360,15 @@
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v>Introduction to Statistical Learning Chp 2</v>
       </c>
-      <c r="P4" s="2" t="str">
-        <f t="array" ref="P4">INDEX(IF((Goals[Started] &lt;= MAX(Periods[Start])) * (Goals[Finished] &gt; MAX(Periods[Start])) * (NOT(ISBLANK(Goals[Finished]))),  Goals[Finished], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="R4" s="5">
+      <c r="Q4" s="5">
         <v>-3</v>
       </c>
-      <c r="S4" t="str">
-        <f t="array" ref="S4">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R4" t="str">
+        <f t="array" ref="R4">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="30">
         <v>4</v>
       </c>
@@ -2473,19 +2418,15 @@
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v>Finish a complete class plan</v>
       </c>
-      <c r="P5" s="2" t="str">
-        <f t="array" ref="P5">INDEX(IF((Goals[Started] &lt;= MAX(Periods[Start])) * (Goals[Finished] &gt; MAX(Periods[Start])) * (NOT(ISBLANK(Goals[Finished]))),  Goals[Finished], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="R5" s="5">
+      <c r="Q5" s="5">
         <v>-4</v>
       </c>
-      <c r="S5" t="str">
-        <f t="array" ref="S5">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R5" t="str">
+        <f t="array" ref="R5">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="30">
         <v>5</v>
       </c>
@@ -2521,7 +2462,7 @@
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="5">
-        <v>-11</v>
+        <v>-10</v>
       </c>
       <c r="M6" s="30">
         <f>MAX(Periods[Id])</f>
@@ -2535,19 +2476,15 @@
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="P6" s="2" t="str">
-        <f t="array" ref="P6">INDEX(IF((Goals[Started] &lt;= MAX(Periods[Start])) * (Goals[Finished] &gt; MAX(Periods[Start])) * (NOT(ISBLANK(Goals[Finished]))),  Goals[Finished], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="R6" s="5">
+      <c r="Q6" s="5">
         <v>-5</v>
       </c>
-      <c r="S6" t="str">
-        <f t="array" ref="S6">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R6" t="str">
+        <f t="array" ref="R6">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E7" s="5">
         <v>-13</v>
       </c>
@@ -2573,33 +2510,29 @@
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="5">
-        <v>-10</v>
+        <v>-11</v>
       </c>
       <c r="M7" s="30">
         <f>MAX(Periods[Id])</f>
         <v>5</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="5" t="str">
         <f t="array" ref="N7">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>26</v>
+        <v/>
       </c>
       <c r="O7" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v>Account for Conferences In Pub Plan</v>
-      </c>
-      <c r="P7" s="2" t="str">
-        <f t="array" ref="P7">INDEX(IF((Goals[Started] &lt;= MAX(Periods[Start])) * (Goals[Finished] &gt; MAX(Periods[Start])) * (NOT(ISBLANK(Goals[Finished]))),  Goals[Finished], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="R7" s="5">
+        <v/>
+      </c>
+      <c r="Q7" s="5">
         <v>-6</v>
       </c>
-      <c r="S7" t="str">
-        <f t="array" ref="S7">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R7" t="str">
+        <f t="array" ref="R7">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E8" s="5">
         <v>-15</v>
       </c>
@@ -2639,19 +2572,15 @@
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="P8" s="2" t="str">
-        <f t="array" ref="P8">INDEX(IF((Goals[Started] &lt;= MAX(Periods[Start])) * (Goals[Finished] &gt; MAX(Periods[Start])) * (NOT(ISBLANK(Goals[Finished]))),  Goals[Finished], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="R8" s="5">
+      <c r="Q8" s="5">
         <v>-7</v>
       </c>
-      <c r="S8" t="str">
-        <f t="array" ref="S8">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R8" t="str">
+        <f t="array" ref="R8">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E9" s="5">
         <v>-16</v>
       </c>
@@ -2691,19 +2620,15 @@
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="P9" s="2" t="str">
-        <f t="array" ref="P9">INDEX(IF((Goals[Started] &lt;= MAX(Periods[Start])) * (Goals[Finished] &gt; MAX(Periods[Start])) * (NOT(ISBLANK(Goals[Finished]))),  Goals[Finished], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="R9" s="5">
+      <c r="Q9" s="5">
         <v>-8</v>
       </c>
-      <c r="S9" t="str">
-        <f t="array" ref="S9">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R9" t="str">
+        <f t="array" ref="R9">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E10" s="5">
         <v>-17</v>
       </c>
@@ -2743,19 +2668,15 @@
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="P10" s="2" t="str">
-        <f t="array" ref="P10">INDEX(IF((Goals[Started] &lt;= MAX(Periods[Start])) * (Goals[Finished] &gt; MAX(Periods[Start])) * (NOT(ISBLANK(Goals[Finished]))),  Goals[Finished], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="R10" s="5">
+      <c r="Q10" s="5">
         <v>-9</v>
       </c>
-      <c r="S10" t="str">
-        <f t="array" ref="S10">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R10" t="str">
+        <f t="array" ref="R10">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E11" s="5">
         <v>-18</v>
       </c>
@@ -2795,19 +2716,15 @@
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="P11" s="2" t="str">
-        <f t="array" ref="P11">INDEX(IF((Goals[Started] &lt;= MAX(Periods[Start])) * (Goals[Finished] &gt; MAX(Periods[Start])) * (NOT(ISBLANK(Goals[Finished]))),  Goals[Finished], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="R11" s="5">
+      <c r="Q11" s="5">
         <v>-10</v>
       </c>
-      <c r="S11" t="str">
-        <f t="array" ref="S11">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R11" t="str">
+        <f t="array" ref="R11">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E12" s="5">
         <v>-19</v>
       </c>
@@ -2847,12 +2764,8 @@
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="P12" s="2" t="str">
-        <f t="array" ref="P12">INDEX(IF((Goals[Started] &lt;= MAX(Periods[Start])) * (Goals[Finished] &gt; MAX(Periods[Start])) * (NOT(ISBLANK(Goals[Finished]))),  Goals[Finished], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E13" s="5">
         <v>-20</v>
       </c>
@@ -2892,12 +2805,8 @@
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="P13" s="2" t="str">
-        <f t="array" ref="P13">INDEX(IF((Goals[Started] &lt;= MAX(Periods[Start])) * (Goals[Finished] &gt; MAX(Periods[Start])) * (NOT(ISBLANK(Goals[Finished]))),  Goals[Finished], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E14" s="5">
         <v>-8</v>
       </c>
@@ -2937,12 +2846,8 @@
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="P14" s="2" t="str">
-        <f t="array" ref="P14">INDEX(IF((Goals[Started] &lt;= MAX(Periods[Start])) * (Goals[Finished] &gt; MAX(Periods[Start])) * (NOT(ISBLANK(Goals[Finished]))),  Goals[Finished], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E15" s="5">
         <v>-7</v>
       </c>
@@ -2982,12 +2887,8 @@
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="P15" s="2" t="str">
-        <f t="array" ref="P15">INDEX(IF((Goals[Started] &lt;= MAX(Periods[Start])) * (Goals[Finished] &gt; MAX(Periods[Start])) * (NOT(ISBLANK(Goals[Finished]))),  Goals[Finished], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E16" s="5">
         <v>-6</v>
       </c>
@@ -3027,12 +2928,8 @@
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="P16" s="2" t="str">
-        <f t="array" ref="P16">INDEX(IF((Goals[Started] &lt;= MAX(Periods[Start])) * (Goals[Finished] &gt; MAX(Periods[Start])) * (NOT(ISBLANK(Goals[Finished]))),  Goals[Finished], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="5:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E17" s="5">
         <v>-5</v>
       </c>
@@ -3072,12 +2969,8 @@
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="P17" s="2" t="str">
-        <f t="array" ref="P17">INDEX(IF((Goals[Started] &lt;= MAX(Periods[Start])) * (Goals[Finished] &gt; MAX(Periods[Start])) * (NOT(ISBLANK(Goals[Finished]))),  Goals[Finished], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="5:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E18" s="5">
         <v>-4</v>
       </c>
@@ -3117,12 +3010,8 @@
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="P18" s="2" t="str">
-        <f t="array" ref="P18">INDEX(IF((Goals[Started] &lt;= MAX(Periods[Start])) * (Goals[Finished] &gt; MAX(Periods[Start])) * (NOT(ISBLANK(Goals[Finished]))),  Goals[Finished], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="5:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E19" s="5">
         <v>-3</v>
       </c>
@@ -3162,12 +3051,8 @@
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="P19" s="2" t="str">
-        <f t="array" ref="P19">INDEX(IF((Goals[Started] &lt;= MAX(Periods[Start])) * (Goals[Finished] &gt; MAX(Periods[Start])) * (NOT(ISBLANK(Goals[Finished]))),  Goals[Finished], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="5:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E20" s="5">
         <v>-2</v>
       </c>
@@ -3207,12 +3092,8 @@
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="P20" s="2" t="str">
-        <f t="array" ref="P20">INDEX(IF((Goals[Started] &lt;= MAX(Periods[Start])) * (Goals[Finished] &gt; MAX(Periods[Start])) * (NOT(ISBLANK(Goals[Finished]))),  Goals[Finished], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="5:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E21" s="5">
         <v>-1</v>
       </c>
@@ -3250,10 +3131,6 @@
       </c>
       <c r="O21" s="30" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="P21" s="2" t="str">
-        <f t="array" ref="P21">INDEX(IF((Goals[Started] &lt;= MAX(Periods[Start])) * (Goals[Finished] &gt; MAX(Periods[Start])) * (NOT(ISBLANK(Goals[Finished]))),  Goals[Finished], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
         <v/>
       </c>
     </row>
@@ -3330,7 +3207,7 @@
       <c r="B3" s="27"/>
       <c r="C3" s="27"/>
       <c r="D3" s="38" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E3" s="37" t="s">
         <v>34</v>
@@ -3343,7 +3220,7 @@
       <c r="J3" s="28"/>
       <c r="K3" s="29"/>
       <c r="L3" s="34" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
@@ -3370,7 +3247,7 @@
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
       <c r="L4" s="34" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
@@ -3383,7 +3260,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="15"/>
       <c r="H5" s="32" t="str">
@@ -3393,7 +3270,7 @@
       <c r="J5" s="33"/>
       <c r="K5" s="33"/>
       <c r="L5" s="34" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M5"/>
     </row>
@@ -3417,7 +3294,7 @@
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
       <c r="L6" s="34" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M6"/>
     </row>
@@ -3441,7 +3318,7 @@
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
       <c r="L7" s="34" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M7"/>
     </row>
@@ -3466,7 +3343,7 @@
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
       <c r="L8" s="34" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M8"/>
     </row>
@@ -3485,13 +3362,13 @@
       <c r="F9" s="15"/>
       <c r="G9" s="13"/>
       <c r="H9" s="10" t="str">
-        <v>Account for Conferences In Pub Plan</v>
+        <v/>
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
       <c r="L9" s="34" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M9"/>
     </row>
@@ -3516,7 +3393,7 @@
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
       <c r="L10" s="34" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M10"/>
     </row>
@@ -3541,7 +3418,7 @@
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
       <c r="L11" s="34" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M11"/>
     </row>
@@ -3566,7 +3443,7 @@
       <c r="J12" s="19"/>
       <c r="K12" s="19"/>
       <c r="L12" s="34" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M12"/>
     </row>
@@ -4004,65 +3881,65 @@
     <mergeCell ref="J1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:E18">
-    <cfRule type="expression" dxfId="19" priority="13">
+    <cfRule type="expression" dxfId="14" priority="13">
       <formula>INDIRECT("A"&amp;ROW()) &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="14">
+    <cfRule type="expression" dxfId="13" priority="14">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="15">
+    <cfRule type="expression" dxfId="12" priority="15">
       <formula>INDIRECT("A"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:K18">
-    <cfRule type="expression" dxfId="16" priority="10">
+    <cfRule type="expression" dxfId="11" priority="10">
       <formula>INDIRECT("H"&amp;ROW()) &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="11">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="12">
+    <cfRule type="expression" dxfId="9" priority="12">
       <formula>INDIRECT("H"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:K30">
-    <cfRule type="expression" dxfId="13" priority="7">
+    <cfRule type="expression" dxfId="8" priority="7">
       <formula>INDIRECT("A"&amp;ROW()) &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="8">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="9">
+    <cfRule type="expression" dxfId="6" priority="9">
       <formula>INDIRECT("A"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H12">
-    <cfRule type="expression" dxfId="10" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>INDIRECT("H"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:K12">
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>INDIRECT("H"&amp;ROW()) &lt;&gt; ""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A12">
-    <cfRule type="expression" dxfId="8" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>INDIRECT("A"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E12">
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>INDIRECT("A"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:A30">
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>INDIRECT("A"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21:K30">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>INDIRECT("A"&amp;ROW()) &lt;&gt; ""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Recording my work for tonight
</commit_message>
<xml_diff>
--- a/updates/Updates.xlsx
+++ b/updates/Updates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Goals" sheetId="1" r:id="rId1"/>
@@ -17,8 +17,67 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="B26" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ID Cards To receive your University I.D. card you will need to go to the University I.D. Card Office, Observatory Hill Dining Hall between the hours of 8:30 a.m. and 4:30 p.m. after completion of your registration.  For information regarding the University ID Card Office visit http://www.virginia.edu/idoffice/.  Please remember to bring with you a valid state or government issued picture identification card (either your U.S. driver’s license, passport or U.S. military ID) in order to pick up your University ID. You will need your UVA email account first.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B28" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ll students are required to have health insurance. Once you arrive on Grounds, and have picked up your ID card, you will be able to sign up for health insurance through the University sponsored health plan.  If health insurance subsidy is included in your Financial Aid package, please go tohttp://www.aetnastudenthealth.com/stu_conn/student_connection.aspx?groupID=812806   to complete the Aetna Health Plan enrollment. This initial enrollment will cover the summer, through mid-August.  You will need to pay for the insurance, and then request reimbursement from the department, because of your summer start date.  You will register again for a full year in August, and will need documentation of your immunizations at that time.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="77">
   <si>
     <t>Install JabRef on my personal machine</t>
   </si>
@@ -41,15 +100,9 @@
     <t>Create Linux instance on AWS with R installed</t>
   </si>
   <si>
-    <t>Sign up as TA</t>
-  </si>
-  <si>
     <t>Get campus ID card</t>
   </si>
   <si>
-    <t>Get campus parking pass</t>
-  </si>
-  <si>
     <t>Create curriculum plan</t>
   </si>
   <si>
@@ -158,9 +211,6 @@
     <t>Finished</t>
   </si>
   <si>
-    <t>Added</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -236,7 +286,28 @@
     <t>Account for conferences in pub plan</t>
   </si>
   <si>
-    <t>Get in touch with HR about TA</t>
+    <t>Reading Abstracts</t>
+  </si>
+  <si>
+    <t>Can we design a CHS conceptual framework that works in all situations</t>
+  </si>
+  <si>
+    <t>How have HHS systems been modeled?</t>
+  </si>
+  <si>
+    <t>What classes am I "qualified" to GTA?</t>
+  </si>
+  <si>
+    <t>Write Jayne my TA preferences</t>
+  </si>
+  <si>
+    <t>Sign up for Health Insurance</t>
+  </si>
+  <si>
+    <t>Register for classes</t>
+  </si>
+  <si>
+    <t>Going through Jayne's Emails</t>
   </si>
 </sst>
 </file>
@@ -249,7 +320,7 @@
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -333,6 +404,19 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -500,7 +584,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="39">
     <dxf>
       <border>
         <right style="thin">
@@ -626,21 +710,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="25" formatCode="h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="h:mm"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -692,7 +761,19 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -721,43 +802,55 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Goals" displayName="Goals" ref="A1:G29" totalsRowShown="0">
-  <autoFilter ref="A1:G29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Goals" displayName="Goals" ref="A1:F29" totalsRowShown="0">
+  <autoFilter ref="A1:F29">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="14"/>
+        <filter val="16"/>
+        <filter val="17"/>
+        <filter val="18"/>
+        <filter val="19"/>
+        <filter val="22"/>
+        <filter val="24"/>
+        <filter val="27"/>
+        <filter val="28"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="5">
       <filters blank="1"/>
     </filterColumn>
   </autoFilter>
-  <sortState ref="A17:G30">
+  <sortState ref="A17:F29">
     <sortCondition ref="F2:F24"/>
     <sortCondition ref="D2:D24"/>
   </sortState>
-  <tableColumns count="7">
-    <tableColumn id="8" name="Id" dataDxfId="39"/>
+  <tableColumns count="6">
+    <tableColumn id="8" name="Id" dataDxfId="38"/>
     <tableColumn id="1" name="Description"/>
     <tableColumn id="2" name="Comments"/>
-    <tableColumn id="4" name="Due" dataDxfId="38"/>
-    <tableColumn id="3" name="Started" dataDxfId="37"/>
-    <tableColumn id="5" name="Finished" dataDxfId="36"/>
-    <tableColumn id="6" name="Added" dataDxfId="35"/>
+    <tableColumn id="4" name="Due" dataDxfId="37"/>
+    <tableColumn id="3" name="Started" dataDxfId="36"/>
+    <tableColumn id="5" name="Finished" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Times" displayName="Times" ref="A1:H12" totalsRowShown="0">
-  <autoFilter ref="A1:H12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Times" displayName="Times" ref="A1:H14" totalsRowShown="0">
+  <autoFilter ref="A1:H14"/>
   <tableColumns count="8">
     <tableColumn id="4" name="Work"/>
     <tableColumn id="9" name="Period"/>
     <tableColumn id="5" name="Date"/>
-    <tableColumn id="6" name="Start" dataDxfId="19"/>
-    <tableColumn id="7" name="End" dataDxfId="18"/>
-    <tableColumn id="1" name="Hours" dataDxfId="17">
+    <tableColumn id="6" name="Start" dataDxfId="34"/>
+    <tableColumn id="7" name="End" dataDxfId="33"/>
+    <tableColumn id="1" name="Hours" dataDxfId="32">
       <calculatedColumnFormula>Times[[#This Row],[End]]-Times[[#This Row],[Start]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Goal" dataDxfId="16"/>
-    <tableColumn id="3" name="Goal Description" dataDxfId="15">
+    <tableColumn id="2" name="Goal" dataDxfId="31"/>
+    <tableColumn id="3" name="Goal Description" dataDxfId="30">
       <calculatedColumnFormula>VLOOKUP(Times[[#This Row],[Goal]], Goals[], 2, FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -766,8 +859,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Questions" displayName="Questions" ref="A1:C6" totalsRowShown="0">
-  <autoFilter ref="A1:C6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Questions" displayName="Questions" ref="A1:C9" totalsRowShown="0">
+  <autoFilter ref="A1:C9"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Question"/>
     <tableColumn id="2" name="Answer"/>
@@ -781,9 +874,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Periods" displayName="Periods" ref="A1:C6" totalsRowShown="0">
   <autoFilter ref="A1:C6"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Id" dataDxfId="34"/>
-    <tableColumn id="2" name="Start" dataDxfId="33"/>
-    <tableColumn id="3" name="End" dataDxfId="32">
+    <tableColumn id="1" name="Id" dataDxfId="29"/>
+    <tableColumn id="2" name="Start" dataDxfId="28"/>
+    <tableColumn id="3" name="End" dataDxfId="27">
       <calculatedColumnFormula>Periods[[#This Row],[Start]] + (7)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -798,20 +891,20 @@
     <sortCondition descending="1" ref="J1:J21"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="2" name="Index" dataDxfId="31"/>
-    <tableColumn id="4" name="Period" dataDxfId="30">
+    <tableColumn id="2" name="Index" dataDxfId="26"/>
+    <tableColumn id="4" name="Period" dataDxfId="25">
       <calculatedColumnFormula>MAX(Periods[Id]) -1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Goal" dataDxfId="29">
+    <tableColumn id="5" name="Goal" dataDxfId="24">
       <calculatedColumnFormula array="1">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Goal Description" dataDxfId="28">
+    <tableColumn id="1" name="Goal Description" dataDxfId="23">
       <calculatedColumnFormula>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Hours" dataDxfId="27">
+    <tableColumn id="6" name="Hours" dataDxfId="22">
       <calculatedColumnFormula array="1">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Done" dataDxfId="26">
+    <tableColumn id="3" name="Done" dataDxfId="21">
       <calculatedColumnFormula>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -826,14 +919,14 @@
     <sortCondition descending="1" ref="O1:O21"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="2" name="Index" dataDxfId="25"/>
-    <tableColumn id="6" name="Period" dataDxfId="24">
+    <tableColumn id="2" name="Index" dataDxfId="20"/>
+    <tableColumn id="6" name="Period" dataDxfId="19">
       <calculatedColumnFormula>MAX(Periods[Id])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Goal" dataDxfId="23">
+    <tableColumn id="5" name="Goal" dataDxfId="18">
       <calculatedColumnFormula array="1">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Description" dataDxfId="22">
+    <tableColumn id="1" name="Description" dataDxfId="17">
       <calculatedColumnFormula>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -848,8 +941,8 @@
     <sortCondition descending="1" ref="Q1:Q21"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="2" name="Index" dataDxfId="21"/>
-    <tableColumn id="1" name="Question" dataDxfId="20">
+    <tableColumn id="2" name="Index" dataDxfId="16"/>
+    <tableColumn id="1" name="Question" dataDxfId="15">
       <calculatedColumnFormula array="1">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1143,11 +1236,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1162,34 +1255,31 @@
     <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I1" t="str">
+        <v>43</v>
+      </c>
+      <c r="H1" t="str">
         <f xml:space="preserve"> "Current Period: " &amp; MAX(Periods[Id]) -1</f>
         <v>Current Period: 4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1205,11 +1295,8 @@
       <c r="F2" s="30">
         <v>2</v>
       </c>
-      <c r="G2" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1225,16 +1312,13 @@
       <c r="F3" s="30">
         <v>2</v>
       </c>
-      <c r="G3" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D4" s="2">
         <v>42508</v>
@@ -1245,16 +1329,13 @@
       <c r="F4" s="30">
         <v>2</v>
       </c>
-      <c r="G4" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D5" s="2">
         <v>42509</v>
@@ -1265,16 +1346,13 @@
       <c r="F5" s="30">
         <v>2</v>
       </c>
-      <c r="G5" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D6" s="2">
         <v>42509</v>
@@ -1285,16 +1363,13 @@
       <c r="F6" s="30">
         <v>2</v>
       </c>
-      <c r="G6" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D7" s="2">
         <v>42509</v>
@@ -1305,16 +1380,13 @@
       <c r="F7" s="30">
         <v>2</v>
       </c>
-      <c r="G7" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D8" s="2">
         <v>42515</v>
@@ -1325,16 +1397,13 @@
       <c r="F8" s="30">
         <v>3</v>
       </c>
-      <c r="G8" s="30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D9" s="2">
         <v>42515</v>
@@ -1345,11 +1414,8 @@
       <c r="F9" s="30">
         <v>3</v>
       </c>
-      <c r="G9" s="30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>7</v>
       </c>
@@ -1365,16 +1431,13 @@
       <c r="F10" s="30">
         <v>3</v>
       </c>
-      <c r="G10" s="30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D11" s="2">
         <v>42522</v>
@@ -1385,16 +1448,13 @@
       <c r="F11" s="30">
         <v>3</v>
       </c>
-      <c r="G11" s="30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D12" s="2">
         <v>42522</v>
@@ -1405,16 +1465,13 @@
       <c r="F12" s="30">
         <v>3</v>
       </c>
-      <c r="G12" s="30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D13" s="2">
         <v>42522</v>
@@ -1425,16 +1482,13 @@
       <c r="F13" s="30">
         <v>3</v>
       </c>
-      <c r="G13" s="30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D14" s="2">
         <v>42522</v>
@@ -1445,16 +1499,13 @@
       <c r="F14" s="30">
         <v>3</v>
       </c>
-      <c r="G14" s="30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D15" s="2">
         <v>42522</v>
@@ -1465,16 +1516,13 @@
       <c r="F15" s="30">
         <v>3</v>
       </c>
-      <c r="G15" s="30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D16" s="2">
         <v>42529</v>
@@ -1485,11 +1533,8 @@
       <c r="F16" s="30">
         <v>4</v>
       </c>
-      <c r="G16" s="30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>14</v>
       </c>
@@ -1503,16 +1548,13 @@
         <v>3</v>
       </c>
       <c r="F17" s="30"/>
-      <c r="G17" s="30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D18" s="2">
         <v>42529</v>
@@ -1521,16 +1563,13 @@
         <v>4</v>
       </c>
       <c r="F18" s="30"/>
-      <c r="G18" s="30">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D19" s="2">
         <v>42529</v>
@@ -1541,16 +1580,13 @@
       <c r="F19" s="30">
         <v>4</v>
       </c>
-      <c r="G19" s="30">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D20" s="2">
         <v>42529</v>
@@ -1561,16 +1597,13 @@
       <c r="F20" s="30">
         <v>4</v>
       </c>
-      <c r="G20" s="30">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D21" s="2">
         <v>42529</v>
@@ -1579,151 +1612,128 @@
         <v>4</v>
       </c>
       <c r="F21" s="30"/>
-      <c r="G21" s="30">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
+        <v>18</v>
+      </c>
+      <c r="B22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="2">
+        <v>42538</v>
+      </c>
+      <c r="E22" s="30">
+        <v>5</v>
+      </c>
+      <c r="F22" s="30"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
         <v>16</v>
       </c>
-      <c r="B22" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="2">
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="2">
         <v>42577</v>
-      </c>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
-        <v>17</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="2">
-        <v>42583</v>
       </c>
       <c r="E23" s="30"/>
       <c r="F23" s="30"/>
-      <c r="G23" s="30">
-        <v>3</v>
-      </c>
-      <c r="N23" s="8"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M23" s="8"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D24" s="2">
         <v>42583</v>
       </c>
       <c r="E24" s="30"/>
       <c r="F24" s="30"/>
-      <c r="G24" s="30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="D25" s="2">
-        <v>42583</v>
+        <v>42585</v>
       </c>
       <c r="E25" s="30"/>
       <c r="F25" s="30"/>
-      <c r="G25" s="30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D26" s="2">
-        <v>42583</v>
+        <v>42586</v>
       </c>
       <c r="E26" s="30"/>
       <c r="F26" s="30"/>
-      <c r="G26" s="30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>72</v>
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
       </c>
       <c r="D27" s="2">
-        <v>42583</v>
+        <v>42587</v>
       </c>
       <c r="E27" s="30"/>
       <c r="F27" s="30"/>
-      <c r="G27" s="30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
       <c r="D28" s="2">
-        <v>42583</v>
+        <v>42587</v>
       </c>
       <c r="E28" s="30"/>
       <c r="F28" s="30"/>
-      <c r="G28" s="30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="30"/>
       <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" location="heading=h.q544jq4bo7vu" display="https://docs.google.com/document/d/1WtVePtADr7xStL5Ac2lepzWibRBYoZs5Y_515wGqzFw/edit - heading=h.q544jq4bo7vu"/>
     <hyperlink ref="B7" r:id="rId2" location="heading=h.q544jq4bo7vu" display="https://docs.google.com/document/d/1WtVePtADr7xStL5Ac2lepzWibRBYoZs5Y_515wGqzFw/edit - heading=h.q544jq4bo7vu"/>
-    <hyperlink ref="B23" r:id="rId3" location="inbox/154e7d1ce0153b1e"/>
+    <hyperlink ref="B27" r:id="rId3" location="inbox/154e7d1ce0153b1e"/>
     <hyperlink ref="B11" r:id="rId4" location="heading=h.4uv9il96waak" display="https://docs.google.com/document/d/1WtVePtADr7xStL5Ac2lepzWibRBYoZs5Y_515wGqzFw/edit - heading=h.4uv9il96waak"/>
     <hyperlink ref="B12" r:id="rId5" location="heading=h.kwuhphhohs6l" display="https://docs.google.com/document/d/1WtVePtADr7xStL5Ac2lepzWibRBYoZs5Y_515wGqzFw/edit - heading=h.kwuhphhohs6l"/>
     <hyperlink ref="B13" r:id="rId6" location="heading=h.kwuhphhohs6l" display="https://docs.google.com/document/d/1WtVePtADr7xStL5Ac2lepzWibRBYoZs5Y_515wGqzFw/edit - heading=h.kwuhphhohs6l"/>
     <hyperlink ref="B8" r:id="rId7" display="Read Prof. Gerber's Thoughts"/>
-    <hyperlink ref="B27" r:id="rId8" display="Get in touch with Human Resources about TA"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
+  <legacyDrawing r:id="rId9"/>
   <tableParts count="1">
     <tablePart r:id="rId10"/>
   </tableParts>
@@ -1732,10 +1742,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1751,33 +1761,33 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -1805,7 +1815,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -1833,7 +1843,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -1859,7 +1869,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1887,7 +1897,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -1915,7 +1925,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -1943,7 +1953,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -1971,7 +1981,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -1999,7 +2009,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -2027,7 +2037,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B11">
         <v>4</v>
@@ -2053,7 +2063,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B12">
         <v>4</v>
@@ -2079,10 +2089,64 @@
         <v>Introduction to Statistical Learning Chp 2</v>
       </c>
     </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13" s="3">
+        <v>42527</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0.84375</v>
+      </c>
+      <c r="F13" s="6">
+        <f>Times[[#This Row],[End]]-Times[[#This Row],[Start]]</f>
+        <v>5.208333333333337E-2</v>
+      </c>
+      <c r="G13" s="30">
+        <v>24</v>
+      </c>
+      <c r="H13" s="6" t="str">
+        <f>VLOOKUP(Times[[#This Row],[Goal]], Goals[], 2, FALSE)</f>
+        <v>Read all article abstracts</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14" s="3">
+        <v>42161</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0.84375</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0.88541666666666663</v>
+      </c>
+      <c r="F14" s="6">
+        <f>Times[[#This Row],[End]]-Times[[#This Row],[Start]]</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="G14" s="30"/>
+      <c r="H14" s="6" t="str">
+        <f>VLOOKUP(Times[[#This Row],[Goal]], Goals[], 2, FALSE)</f>
+        <v>Miscellaneous</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" sqref="G2:H12"/>
+    <dataValidation allowBlank="1" showInputMessage="1" sqref="G2:H14"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2094,10 +2158,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2108,21 +2172,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
         <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" s="3">
         <v>42522</v>
@@ -2130,10 +2194,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C3" s="3">
         <v>42522</v>
@@ -2141,10 +2205,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C4" s="3">
         <v>42522</v>
@@ -2152,10 +2216,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C5" s="3">
         <v>42522</v>
@@ -2163,13 +2227,37 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C6" s="3">
         <v>42522</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="3">
+        <v>42527</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="3">
+        <v>42527</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="3">
+        <v>42527</v>
       </c>
     </row>
   </sheetData>
@@ -2185,7 +2273,7 @@
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2211,49 +2299,49 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J1" t="s">
-        <v>28</v>
-      </c>
       <c r="L1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="N1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Q1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="R1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -2269,7 +2357,7 @@
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="5">
-        <v>-11</v>
+        <v>-10</v>
       </c>
       <c r="F2" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -2277,15 +2365,15 @@
       </c>
       <c r="G2" s="30">
         <f t="array" ref="G2">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H2" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v>Add hours to update sheet</v>
+        <v>Account for conferences in pub plan</v>
       </c>
       <c r="I2" s="6">
         <f t="array" ref="I2">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v>0.17708333333333326</v>
+        <v>0</v>
       </c>
       <c r="J2" s="30" t="b">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</f>
@@ -2293,26 +2381,26 @@
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="5">
-        <v>-13</v>
+        <v>-5</v>
       </c>
       <c r="M2" s="30">
         <f>MAX(Periods[Id])</f>
         <v>5</v>
       </c>
-      <c r="N2" s="5">
+      <c r="N2" s="5" t="str">
         <f t="array" ref="N2">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>14</v>
+        <v/>
       </c>
       <c r="O2" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v>Reinforcement Learning an Introduction</v>
+        <v/>
       </c>
       <c r="Q2" s="5">
         <v>-1</v>
       </c>
       <c r="R2" t="str">
         <f t="array" ref="R2">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v/>
+        <v>What classes am I "qualified" to GTA?</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -2328,7 +2416,7 @@
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="5">
-        <v>-10</v>
+        <v>-13</v>
       </c>
       <c r="F3" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -2336,11 +2424,11 @@
       </c>
       <c r="G3" s="30">
         <f t="array" ref="G3">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="H3" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v>Account for conferences in pub plan</v>
+        <v>Reinforcement Learning an Introduction</v>
       </c>
       <c r="I3" s="6">
         <f t="array" ref="I3">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
@@ -2348,7 +2436,7 @@
       </c>
       <c r="J3" s="30" t="b">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="5">
@@ -2371,7 +2459,7 @@
       </c>
       <c r="R3" t="str">
         <f t="array" ref="R3">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v/>
+        <v>How have HHS systems been modeled?</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -2386,7 +2474,7 @@
         <v>42522</v>
       </c>
       <c r="E4" s="5">
-        <v>-14</v>
+        <v>-9</v>
       </c>
       <c r="F4" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -2394,42 +2482,42 @@
       </c>
       <c r="G4" s="30">
         <f t="array" ref="G4">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>13</v>
-      </c>
-      <c r="H4" t="str">
+        <v>27</v>
+      </c>
+      <c r="H4" s="15" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v>Introduction to Statistical Learning Chp 2</v>
+        <v>Finish a complete class plan</v>
       </c>
       <c r="I4" s="6">
         <f t="array" ref="I4">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v>2.083333333333337E-2</v>
+        <v>0.19791666666666674</v>
       </c>
       <c r="J4" s="30" t="b">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="5">
-        <v>-9</v>
+        <v>-11</v>
       </c>
       <c r="M4" s="30">
         <f>MAX(Periods[Id])</f>
         <v>5</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="5" t="str">
         <f t="array" ref="N4">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>27</v>
+        <v/>
       </c>
       <c r="O4" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v>Finish a complete class plan</v>
+        <v/>
       </c>
       <c r="Q4" s="5">
         <v>-3</v>
       </c>
       <c r="R4" t="str">
         <f t="array" ref="R4">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v/>
+        <v>Can we design a CHS conceptual framework that works in all situations</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -2444,7 +2532,7 @@
         <v>42529</v>
       </c>
       <c r="E5" s="5">
-        <v>-12</v>
+        <v>-11</v>
       </c>
       <c r="F5" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -2452,35 +2540,35 @@
       </c>
       <c r="G5" s="30">
         <f t="array" ref="G5">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H5" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v>Read all article abstracts</v>
+        <v>Add hours to update sheet</v>
       </c>
       <c r="I5" s="6">
         <f t="array" ref="I5">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v>1.041666666666663E-2</v>
+        <v>0.17708333333333326</v>
       </c>
       <c r="J5" s="30" t="b">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="5">
-        <v>-14</v>
+        <v>-8</v>
       </c>
       <c r="M5" s="30">
         <f>MAX(Periods[Id])</f>
         <v>5</v>
       </c>
-      <c r="N5" s="5" t="str">
+      <c r="N5" s="5">
         <f t="array" ref="N5">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
+        <v>18</v>
       </c>
       <c r="O5" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v/>
+        <v>Write Jayne my TA preferences</v>
       </c>
       <c r="Q5" s="5">
         <v>-4</v>
@@ -2502,7 +2590,7 @@
         <v>42536</v>
       </c>
       <c r="E6" s="5">
-        <v>-13</v>
+        <v>-12</v>
       </c>
       <c r="F6" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -2510,15 +2598,15 @@
       </c>
       <c r="G6" s="30">
         <f t="array" ref="G6">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="H6" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v>Reinforcement Learning an Introduction</v>
+        <v>Read all article abstracts</v>
       </c>
       <c r="I6" s="6">
         <f t="array" ref="I6">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="J6" s="30" t="b">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</f>
@@ -2526,19 +2614,19 @@
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="5">
-        <v>-10</v>
+        <v>-13</v>
       </c>
       <c r="M6" s="30">
         <f>MAX(Periods[Id])</f>
         <v>5</v>
       </c>
-      <c r="N6" s="5" t="str">
+      <c r="N6" s="5">
         <f t="array" ref="N6">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
+        <v>14</v>
       </c>
       <c r="O6" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v/>
+        <v>Reinforcement Learning an Introduction</v>
       </c>
       <c r="Q6" s="5">
         <v>-5</v>
@@ -2550,43 +2638,43 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E7" s="5">
-        <v>-9</v>
+        <v>-8</v>
       </c>
       <c r="F7" s="30">
         <f>MAX(Periods[Id]) -1</f>
         <v>4</v>
       </c>
-      <c r="G7" s="30">
+      <c r="G7" s="30" t="str">
         <f t="array" ref="G7">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>27</v>
-      </c>
-      <c r="H7" s="15" t="str">
+        <v/>
+      </c>
+      <c r="H7" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v>Finish a complete class plan</v>
-      </c>
-      <c r="I7" s="6">
+        <v/>
+      </c>
+      <c r="I7" s="6" t="str">
         <f t="array" ref="I7">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v>0.19791666666666674</v>
-      </c>
-      <c r="J7" s="30" t="b">
+        <v/>
+      </c>
+      <c r="J7" s="30" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="5">
-        <v>-11</v>
+        <v>-9</v>
       </c>
       <c r="M7" s="30">
         <f>MAX(Periods[Id])</f>
         <v>5</v>
       </c>
-      <c r="N7" s="5" t="str">
+      <c r="N7" s="5">
         <f t="array" ref="N7">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
+        <v>27</v>
       </c>
       <c r="O7" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v/>
+        <v>Finish a complete class plan</v>
       </c>
       <c r="Q7" s="5">
         <v>-6</v>
@@ -2598,31 +2686,31 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E8" s="5">
-        <v>-15</v>
+        <v>-14</v>
       </c>
       <c r="F8" s="30">
         <f>MAX(Periods[Id]) -1</f>
         <v>4</v>
       </c>
-      <c r="G8" s="30" t="str">
+      <c r="G8" s="30">
         <f t="array" ref="G8">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
+        <v>13</v>
       </c>
       <c r="H8" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="I8" s="6" t="str">
+        <v>Introduction to Statistical Learning Chp 2</v>
+      </c>
+      <c r="I8" s="6">
         <f t="array" ref="I8">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v/>
-      </c>
-      <c r="J8" s="30" t="str">
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="J8" s="30" t="b">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="5">
-        <v>-16</v>
+        <v>-14</v>
       </c>
       <c r="M8" s="30">
         <f>MAX(Periods[Id])</f>
@@ -2632,7 +2720,7 @@
         <f t="array" ref="N8">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
         <v/>
       </c>
-      <c r="O8" s="30" t="str">
+      <c r="O8" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
@@ -2646,7 +2734,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E9" s="5">
-        <v>-16</v>
+        <v>-15</v>
       </c>
       <c r="F9" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -2656,7 +2744,7 @@
         <f t="array" ref="G9">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
         <v/>
       </c>
-      <c r="H9" s="30" t="str">
+      <c r="H9" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
@@ -2670,7 +2758,7 @@
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="5">
-        <v>-15</v>
+        <v>-10</v>
       </c>
       <c r="M9" s="30">
         <f>MAX(Periods[Id])</f>
@@ -2694,7 +2782,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E10" s="5">
-        <v>-17</v>
+        <v>-16</v>
       </c>
       <c r="F10" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -2718,7 +2806,7 @@
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="5">
-        <v>-8</v>
+        <v>-16</v>
       </c>
       <c r="M10" s="30">
         <f>MAX(Periods[Id])</f>
@@ -2728,7 +2816,7 @@
         <f t="array" ref="N10">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
         <v/>
       </c>
-      <c r="O10" t="str">
+      <c r="O10" s="30" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
@@ -2742,7 +2830,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E11" s="5">
-        <v>-18</v>
+        <v>-17</v>
       </c>
       <c r="F11" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -2766,7 +2854,7 @@
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="5">
-        <v>-1</v>
+        <v>-15</v>
       </c>
       <c r="M11" s="30">
         <f>MAX(Periods[Id])</f>
@@ -2790,7 +2878,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E12" s="5">
-        <v>-19</v>
+        <v>-18</v>
       </c>
       <c r="F12" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -2814,7 +2902,7 @@
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="5">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="M12" s="30">
         <f>MAX(Periods[Id])</f>
@@ -2831,7 +2919,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E13" s="5">
-        <v>-20</v>
+        <v>-19</v>
       </c>
       <c r="F13" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -2855,7 +2943,7 @@
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="5">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="M13" s="30">
         <f>MAX(Periods[Id])</f>
@@ -2872,7 +2960,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E14" s="5">
-        <v>-8</v>
+        <v>-20</v>
       </c>
       <c r="F14" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -2882,7 +2970,7 @@
         <f t="array" ref="G14">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
         <v/>
       </c>
-      <c r="H14" t="str">
+      <c r="H14" s="30" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
@@ -2896,7 +2984,7 @@
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="5">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="M14" s="30">
         <f>MAX(Periods[Id])</f>
@@ -2937,7 +3025,7 @@
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="5">
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="M15" s="30">
         <f>MAX(Periods[Id])</f>
@@ -3234,7 +3322,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -3267,37 +3355,37 @@
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B3" s="27"/>
       <c r="C3" s="27"/>
       <c r="D3" s="38" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F3" s="16"/>
       <c r="H3" s="25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I3" s="28"/>
       <c r="J3" s="28"/>
       <c r="K3" s="29"/>
       <c r="L3" s="34" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="str">
         <f t="array" ref="A4:A18">LastWeekTasks[Goal Description]</f>
-        <v>Add hours to update sheet</v>
+        <v>Account for conferences in pub plan</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="43">
         <f t="array" ref="D4:D12">LastWeekTasks[Hours]</f>
-        <v>0.17708333333333326</v>
+        <v>0</v>
       </c>
       <c r="E4" s="35" t="b">
         <f t="array" ref="E4:E18">LastWeekTasks[Done]</f>
@@ -3306,18 +3394,18 @@
       <c r="F4" s="16"/>
       <c r="H4" s="10" t="str">
         <f t="array" ref="H4:H18">ThisWeekTasks[Description]</f>
-        <v>Reinforcement Learning an Introduction</v>
+        <v/>
       </c>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
       <c r="L4" s="34" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="32" t="str">
-        <v>Account for conferences in pub plan</v>
+        <v>Reinforcement Learning an Introduction</v>
       </c>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
@@ -3325,7 +3413,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="15"/>
       <c r="H5" s="32" t="str">
@@ -3335,66 +3423,66 @@
       <c r="J5" s="33"/>
       <c r="K5" s="33"/>
       <c r="L5" s="34" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M5"/>
     </row>
     <row r="6" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="str">
-        <v>Introduction to Statistical Learning Chp 2</v>
+        <v>Finish a complete class plan</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="45">
-        <v>2.083333333333337E-2</v>
+        <v>0.19791666666666674</v>
       </c>
       <c r="E6" s="35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="15"/>
       <c r="H6" s="10" t="str">
-        <v>Finish a complete class plan</v>
+        <v/>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
       <c r="L6" s="34" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M6"/>
     </row>
     <row r="7" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="str">
-        <v>Read all article abstracts</v>
+        <v>Add hours to update sheet</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="45">
-        <v>1.041666666666663E-2</v>
+        <v>0.17708333333333326</v>
       </c>
       <c r="E7" s="35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="15"/>
       <c r="H7" s="10" t="str">
-        <v/>
+        <v>Write Jayne my TA preferences</v>
       </c>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
       <c r="L7" s="34" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M7"/>
     </row>
     <row r="8" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="str">
-        <v>Reinforcement Learning an Introduction</v>
+        <v>Read all article abstracts</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="45">
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="E8" s="35" t="b">
         <v>0</v>
@@ -3402,52 +3490,52 @@
       <c r="F8" s="15"/>
       <c r="G8" s="13"/>
       <c r="H8" s="10" t="str">
-        <v/>
+        <v>Reinforcement Learning an Introduction</v>
       </c>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
       <c r="L8" s="34" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M8"/>
     </row>
     <row r="9" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="str">
-        <v>Finish a complete class plan</v>
+        <v/>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
-      <c r="D9" s="45">
-        <v>0.19791666666666674</v>
-      </c>
-      <c r="E9" s="35" t="b">
-        <v>0</v>
+      <c r="D9" s="45" t="str">
+        <v/>
+      </c>
+      <c r="E9" s="35" t="str">
+        <v/>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="13"/>
       <c r="H9" s="10" t="str">
-        <v/>
+        <v>Finish a complete class plan</v>
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
       <c r="L9" s="34" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M9"/>
     </row>
     <row r="10" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="str">
-        <v/>
+        <v>Introduction to Statistical Learning Chp 2</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
-      <c r="D10" s="45" t="str">
-        <v/>
-      </c>
-      <c r="E10" s="35" t="str">
-        <v/>
+      <c r="D10" s="45">
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E10" s="35" t="b">
+        <v>1</v>
       </c>
       <c r="F10" s="15"/>
       <c r="G10" s="13"/>
@@ -3458,7 +3546,7 @@
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
       <c r="L10" s="34" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M10"/>
     </row>
@@ -3483,7 +3571,7 @@
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
       <c r="L11" s="34" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M11"/>
     </row>
@@ -3508,7 +3596,7 @@
       <c r="J12" s="19"/>
       <c r="K12" s="19"/>
       <c r="L12" s="34" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M12"/>
     </row>
@@ -3649,7 +3737,7 @@
     </row>
     <row r="20" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A20" s="31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
@@ -3667,7 +3755,7 @@
     <row r="21" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="str">
         <f t="array" ref="A21:A30">ThisWeekQuestions[Question]</f>
-        <v/>
+        <v>What classes am I "qualified" to GTA?</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -3684,7 +3772,7 @@
     </row>
     <row r="22" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A22" s="32" t="str">
-        <v/>
+        <v>How have HHS systems been modeled?</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
@@ -3701,7 +3789,7 @@
     </row>
     <row r="23" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="str">
-        <v/>
+        <v>Can we design a CHS conceptual framework that works in all situations</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>

</xml_diff>

<commit_message>
Adding new integration task. Finishing update
</commit_message>
<xml_diff>
--- a/updates/Updates.xlsx
+++ b/updates/Updates.xlsx
@@ -23,7 +23,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B26" authorId="0" shapeId="0">
+    <comment ref="B27" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B28" authorId="0" shapeId="0">
+    <comment ref="B30" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="80">
   <si>
     <t>Install JabRef on my personal machine</t>
   </si>
@@ -298,9 +298,6 @@
     <t>What classes am I "qualified" to GTA?</t>
   </si>
   <si>
-    <t>Write Jayne my TA preferences</t>
-  </si>
-  <si>
     <t>Sign up for Health Insurance</t>
   </si>
   <si>
@@ -308,6 +305,18 @@
   </si>
   <si>
     <t>Going through Jayne's Emails</t>
+  </si>
+  <si>
+    <t>Send Jayne my TA preferences</t>
+  </si>
+  <si>
+    <t>Playing with JabRef</t>
+  </si>
+  <si>
+    <t>Can I use my own branch in literature?</t>
+  </si>
+  <si>
+    <t>Integrate into UVA System</t>
   </si>
 </sst>
 </file>
@@ -511,7 +520,7 @@
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -555,8 +564,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -567,15 +574,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma 2" xfId="3"/>
@@ -584,7 +604,146 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="39">
+  <dxfs count="54">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <border>
         <right style="thin">
@@ -732,9 +891,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="25" formatCode="h:mm"/>
     </dxf>
     <dxf>
@@ -759,21 +915,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="h:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -802,8 +943,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Goals" displayName="Goals" ref="A1:F29" totalsRowShown="0">
-  <autoFilter ref="A1:F29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Goals" displayName="Goals" ref="A1:F30" totalsRowShown="0">
+  <autoFilter ref="A1:F30">
     <filterColumn colId="0">
       <filters>
         <filter val="14"/>
@@ -815,42 +956,44 @@
         <filter val="24"/>
         <filter val="27"/>
         <filter val="28"/>
+        <filter val="29"/>
       </filters>
     </filterColumn>
     <filterColumn colId="5">
       <filters blank="1"/>
     </filterColumn>
   </autoFilter>
-  <sortState ref="A17:F29">
-    <sortCondition ref="F2:F24"/>
-    <sortCondition ref="D2:D24"/>
+  <sortState ref="A17:F30">
+    <sortCondition ref="F2:F30"/>
+    <sortCondition ref="E2:E30"/>
+    <sortCondition ref="D2:D30"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="8" name="Id" dataDxfId="38"/>
+    <tableColumn id="8" name="Id" dataDxfId="53"/>
     <tableColumn id="1" name="Description"/>
     <tableColumn id="2" name="Comments"/>
-    <tableColumn id="4" name="Due" dataDxfId="37"/>
-    <tableColumn id="3" name="Started" dataDxfId="36"/>
-    <tableColumn id="5" name="Finished" dataDxfId="35"/>
+    <tableColumn id="4" name="Due" dataDxfId="52"/>
+    <tableColumn id="3" name="Started" dataDxfId="51"/>
+    <tableColumn id="5" name="Finished" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Times" displayName="Times" ref="A1:H14" totalsRowShown="0">
-  <autoFilter ref="A1:H14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Times" displayName="Times" ref="A1:H15" totalsRowShown="0">
+  <autoFilter ref="A1:H15"/>
   <tableColumns count="8">
     <tableColumn id="4" name="Work"/>
     <tableColumn id="9" name="Period"/>
     <tableColumn id="5" name="Date"/>
-    <tableColumn id="6" name="Start" dataDxfId="34"/>
-    <tableColumn id="7" name="End" dataDxfId="33"/>
-    <tableColumn id="1" name="Hours" dataDxfId="32">
+    <tableColumn id="6" name="Start" dataDxfId="5"/>
+    <tableColumn id="7" name="End" dataDxfId="4"/>
+    <tableColumn id="1" name="Hours" dataDxfId="3">
       <calculatedColumnFormula>Times[[#This Row],[End]]-Times[[#This Row],[Start]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Goal" dataDxfId="31"/>
-    <tableColumn id="3" name="Goal Description" dataDxfId="30">
+    <tableColumn id="2" name="Goal" dataDxfId="2"/>
+    <tableColumn id="3" name="Goal Description" dataDxfId="1">
       <calculatedColumnFormula>VLOOKUP(Times[[#This Row],[Goal]], Goals[], 2, FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -859,8 +1002,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Questions" displayName="Questions" ref="A1:C9" totalsRowShown="0">
-  <autoFilter ref="A1:C9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Questions" displayName="Questions" ref="A1:C10" totalsRowShown="0">
+  <autoFilter ref="A1:C10"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Question"/>
     <tableColumn id="2" name="Answer"/>
@@ -874,9 +1017,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Periods" displayName="Periods" ref="A1:C6" totalsRowShown="0">
   <autoFilter ref="A1:C6"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Id" dataDxfId="29"/>
-    <tableColumn id="2" name="Start" dataDxfId="28"/>
-    <tableColumn id="3" name="End" dataDxfId="27">
+    <tableColumn id="1" name="Id" dataDxfId="49"/>
+    <tableColumn id="2" name="Start" dataDxfId="48"/>
+    <tableColumn id="3" name="End" dataDxfId="47">
       <calculatedColumnFormula>Periods[[#This Row],[Start]] + (7)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -891,21 +1034,21 @@
     <sortCondition descending="1" ref="J1:J21"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="2" name="Index" dataDxfId="26"/>
-    <tableColumn id="4" name="Period" dataDxfId="25">
+    <tableColumn id="2" name="Index" dataDxfId="46"/>
+    <tableColumn id="4" name="Period" dataDxfId="45">
       <calculatedColumnFormula>MAX(Periods[Id]) -1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Goal" dataDxfId="24">
+    <tableColumn id="5" name="Goal" dataDxfId="44">
       <calculatedColumnFormula array="1">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Goal Description" dataDxfId="23">
+    <tableColumn id="1" name="Goal Description" dataDxfId="43">
       <calculatedColumnFormula>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Hours" dataDxfId="22">
+    <tableColumn id="6" name="Hours" dataDxfId="42">
       <calculatedColumnFormula array="1">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Done" dataDxfId="21">
-      <calculatedColumnFormula>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</calculatedColumnFormula>
+    <tableColumn id="3" name="Done" dataDxfId="0">
+      <calculatedColumnFormula>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -919,14 +1062,14 @@
     <sortCondition descending="1" ref="O1:O21"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="2" name="Index" dataDxfId="20"/>
-    <tableColumn id="6" name="Period" dataDxfId="19">
+    <tableColumn id="2" name="Index" dataDxfId="41"/>
+    <tableColumn id="6" name="Period" dataDxfId="40">
       <calculatedColumnFormula>MAX(Periods[Id])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Goal" dataDxfId="18">
+    <tableColumn id="5" name="Goal" dataDxfId="39">
       <calculatedColumnFormula array="1">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Description" dataDxfId="17">
+    <tableColumn id="1" name="Description" dataDxfId="38">
       <calculatedColumnFormula>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -941,8 +1084,8 @@
     <sortCondition descending="1" ref="Q1:Q21"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="2" name="Index" dataDxfId="16"/>
-    <tableColumn id="1" name="Question" dataDxfId="15">
+    <tableColumn id="2" name="Index" dataDxfId="37"/>
+    <tableColumn id="1" name="Question" dataDxfId="36">
       <calculatedColumnFormula array="1">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1237,10 +1380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="B22" sqref="B22:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1615,94 +1758,96 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <v>18</v>
-      </c>
-      <c r="B22" t="s">
-        <v>73</v>
+        <v>29</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>79</v>
       </c>
       <c r="D22" s="2">
-        <v>42538</v>
+        <v>42597</v>
       </c>
       <c r="E22" s="30">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" s="30"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="D23" s="2">
-        <v>42577</v>
-      </c>
-      <c r="E23" s="30"/>
+        <v>42538</v>
+      </c>
+      <c r="E23" s="30">
+        <v>5</v>
+      </c>
       <c r="F23" s="30"/>
       <c r="M23" s="8"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="D24" s="2">
-        <v>42583</v>
+        <v>42577</v>
       </c>
       <c r="E24" s="30"/>
       <c r="F24" s="30"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="D25" s="2">
-        <v>42585</v>
+        <v>42583</v>
       </c>
       <c r="E25" s="30"/>
       <c r="F25" s="30"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>74</v>
       </c>
       <c r="D26" s="2">
-        <v>42586</v>
+        <v>42585</v>
       </c>
       <c r="E26" s="30"/>
       <c r="F26" s="30"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
-        <v>17</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" t="s">
-        <v>4</v>
+        <v>19</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>7</v>
       </c>
       <c r="D27" s="2">
-        <v>42587</v>
+        <v>42586</v>
       </c>
       <c r="E27" s="30"/>
       <c r="F27" s="30"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>74</v>
+        <v>17</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
       </c>
       <c r="D28" s="2">
         <v>42587</v>
@@ -1720,12 +1865,25 @@
       <c r="D29" s="2"/>
       <c r="E29" s="30"/>
       <c r="F29" s="30"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" s="2">
+        <v>42587</v>
+      </c>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" location="heading=h.q544jq4bo7vu" display="https://docs.google.com/document/d/1WtVePtADr7xStL5Ac2lepzWibRBYoZs5Y_515wGqzFw/edit - heading=h.q544jq4bo7vu"/>
     <hyperlink ref="B7" r:id="rId2" location="heading=h.q544jq4bo7vu" display="https://docs.google.com/document/d/1WtVePtADr7xStL5Ac2lepzWibRBYoZs5Y_515wGqzFw/edit - heading=h.q544jq4bo7vu"/>
-    <hyperlink ref="B27" r:id="rId3" location="inbox/154e7d1ce0153b1e"/>
+    <hyperlink ref="B28" r:id="rId3" location="inbox/154e7d1ce0153b1e"/>
     <hyperlink ref="B11" r:id="rId4" location="heading=h.4uv9il96waak" display="https://docs.google.com/document/d/1WtVePtADr7xStL5Ac2lepzWibRBYoZs5Y_515wGqzFw/edit - heading=h.4uv9il96waak"/>
     <hyperlink ref="B12" r:id="rId5" location="heading=h.kwuhphhohs6l" display="https://docs.google.com/document/d/1WtVePtADr7xStL5Ac2lepzWibRBYoZs5Y_515wGqzFw/edit - heading=h.kwuhphhohs6l"/>
     <hyperlink ref="B13" r:id="rId6" location="heading=h.kwuhphhohs6l" display="https://docs.google.com/document/d/1WtVePtADr7xStL5Ac2lepzWibRBYoZs5Y_515wGqzFw/edit - heading=h.kwuhphhohs6l"/>
@@ -1742,10 +1900,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2055,10 +2213,12 @@
         <f>Times[[#This Row],[End]]-Times[[#This Row],[Start]]</f>
         <v>5.2083333333333259E-2</v>
       </c>
-      <c r="G11" s="30"/>
+      <c r="G11" s="30">
+        <v>29</v>
+      </c>
       <c r="H11" s="6" t="str">
         <f>VLOOKUP(Times[[#This Row],[Goal]], Goals[], 2, FALSE)</f>
-        <v>Miscellaneous</v>
+        <v>Integrate into UVA System</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2119,7 +2279,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -2137,16 +2297,46 @@
         <f>Times[[#This Row],[End]]-Times[[#This Row],[Start]]</f>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="G14" s="30"/>
+      <c r="G14" s="30">
+        <v>29</v>
+      </c>
       <c r="H14" s="6" t="str">
         <f>VLOOKUP(Times[[#This Row],[Goal]], Goals[], 2, FALSE)</f>
-        <v>Miscellaneous</v>
+        <v>Integrate into UVA System</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15" s="3">
+        <v>42528</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E15" s="6">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="F15" s="6">
+        <f>Times[[#This Row],[End]]-Times[[#This Row],[Start]]</f>
+        <v>9.375E-2</v>
+      </c>
+      <c r="G15" s="30">
+        <v>24</v>
+      </c>
+      <c r="H15" s="6" t="str">
+        <f>VLOOKUP(Times[[#This Row],[Goal]], Goals[], 2, FALSE)</f>
+        <v>Read all article abstracts</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" sqref="G2:H14"/>
+    <dataValidation allowBlank="1" showInputMessage="1" sqref="G2:H15"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2158,10 +2348,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2258,6 +2448,14 @@
       </c>
       <c r="C9" s="3">
         <v>42527</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="3">
+        <v>42528</v>
       </c>
     </row>
   </sheetData>
@@ -2273,7 +2471,7 @@
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2357,7 +2555,7 @@
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="5">
-        <v>-10</v>
+        <v>-11</v>
       </c>
       <c r="F2" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -2375,32 +2573,32 @@
         <f t="array" ref="I2">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v>0</v>
       </c>
-      <c r="J2" s="30" t="b">
-        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</f>
-        <v>1</v>
+      <c r="J2" s="48" t="str">
+        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
+        <v>X</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="5">
-        <v>-5</v>
+        <v>-8</v>
       </c>
       <c r="M2" s="30">
         <f>MAX(Periods[Id])</f>
         <v>5</v>
       </c>
-      <c r="N2" s="5" t="str">
+      <c r="N2" s="5">
         <f t="array" ref="N2">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
+        <v>18</v>
       </c>
       <c r="O2" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v/>
+        <v>Send Jayne my TA preferences</v>
       </c>
       <c r="Q2" s="5">
         <v>-1</v>
       </c>
       <c r="R2" t="str">
         <f t="array" ref="R2">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v>What classes am I "qualified" to GTA?</v>
+        <v>Can I use my own branch in literature?</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -2416,7 +2614,7 @@
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="5">
-        <v>-13</v>
+        <v>-12</v>
       </c>
       <c r="F3" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -2424,23 +2622,23 @@
       </c>
       <c r="G3" s="30">
         <f t="array" ref="G3">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="H3" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v>Reinforcement Learning an Introduction</v>
+        <v>Add hours to update sheet</v>
       </c>
       <c r="I3" s="6">
         <f t="array" ref="I3">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v>0</v>
-      </c>
-      <c r="J3" s="30" t="b">
-        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</f>
-        <v>0</v>
+        <v>0.17708333333333326</v>
+      </c>
+      <c r="J3" s="30" t="str">
+        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
+        <v>X</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="5">
-        <v>-12</v>
+        <v>-14</v>
       </c>
       <c r="M3" s="30">
         <f>MAX(Periods[Id])</f>
@@ -2448,18 +2646,18 @@
       </c>
       <c r="N3" s="5">
         <f t="array" ref="N3">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="O3" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v>Read all article abstracts</v>
+        <v>Reinforcement Learning an Introduction</v>
       </c>
       <c r="Q3" s="5">
         <v>-2</v>
       </c>
       <c r="R3" t="str">
         <f t="array" ref="R3">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v>How have HHS systems been modeled?</v>
+        <v>What classes am I "qualified" to GTA?</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -2474,7 +2672,7 @@
         <v>42522</v>
       </c>
       <c r="E4" s="5">
-        <v>-9</v>
+        <v>-15</v>
       </c>
       <c r="F4" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -2482,42 +2680,42 @@
       </c>
       <c r="G4" s="30">
         <f t="array" ref="G4">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>27</v>
-      </c>
-      <c r="H4" s="15" t="str">
+        <v>13</v>
+      </c>
+      <c r="H4" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v>Finish a complete class plan</v>
+        <v>Introduction to Statistical Learning Chp 2</v>
       </c>
       <c r="I4" s="6">
         <f t="array" ref="I4">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v>0.19791666666666674</v>
-      </c>
-      <c r="J4" s="30" t="b">
-        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</f>
-        <v>0</v>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="J4" s="30" t="str">
+        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
+        <v>X</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="5">
-        <v>-11</v>
+        <v>-13</v>
       </c>
       <c r="M4" s="30">
         <f>MAX(Periods[Id])</f>
         <v>5</v>
       </c>
-      <c r="N4" s="5" t="str">
+      <c r="N4" s="5">
         <f t="array" ref="N4">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
+        <v>24</v>
       </c>
       <c r="O4" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v/>
+        <v>Read all article abstracts</v>
       </c>
       <c r="Q4" s="5">
         <v>-3</v>
       </c>
       <c r="R4" t="str">
         <f t="array" ref="R4">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v>Can we design a CHS conceptual framework that works in all situations</v>
+        <v>How have HHS systems been modeled?</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -2532,7 +2730,7 @@
         <v>42529</v>
       </c>
       <c r="E5" s="5">
-        <v>-11</v>
+        <v>-10</v>
       </c>
       <c r="F5" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -2540,23 +2738,23 @@
       </c>
       <c r="G5" s="30">
         <f t="array" ref="G5">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H5" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v>Add hours to update sheet</v>
+        <v>Finish a complete class plan</v>
       </c>
       <c r="I5" s="6">
         <f t="array" ref="I5">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v>0.17708333333333326</v>
-      </c>
-      <c r="J5" s="30" t="b">
-        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</f>
-        <v>1</v>
+        <v>0.19791666666666674</v>
+      </c>
+      <c r="J5" s="30" t="str">
+        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
+        <v/>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="5">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="M5" s="30">
         <f>MAX(Periods[Id])</f>
@@ -2564,18 +2762,18 @@
       </c>
       <c r="N5" s="5">
         <f t="array" ref="N5">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="O5" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v>Write Jayne my TA preferences</v>
+        <v>Integrate into UVA System</v>
       </c>
       <c r="Q5" s="5">
         <v>-4</v>
       </c>
       <c r="R5" t="str">
         <f t="array" ref="R5">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v/>
+        <v>Can we design a CHS conceptual framework that works in all situations</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -2590,7 +2788,7 @@
         <v>42536</v>
       </c>
       <c r="E6" s="5">
-        <v>-12</v>
+        <v>-14</v>
       </c>
       <c r="F6" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -2598,23 +2796,23 @@
       </c>
       <c r="G6" s="30">
         <f t="array" ref="G6">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="H6" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v>Read all article abstracts</v>
+        <v>Reinforcement Learning an Introduction</v>
       </c>
       <c r="I6" s="6">
         <f t="array" ref="I6">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v>6.25E-2</v>
-      </c>
-      <c r="J6" s="30" t="b">
-        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</f>
         <v>0</v>
+      </c>
+      <c r="J6" s="30" t="str">
+        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
+        <v/>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="5">
-        <v>-13</v>
+        <v>-10</v>
       </c>
       <c r="M6" s="30">
         <f>MAX(Periods[Id])</f>
@@ -2622,11 +2820,11 @@
       </c>
       <c r="N6" s="5">
         <f t="array" ref="N6">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="O6" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v>Reinforcement Learning an Introduction</v>
+        <v>Finish a complete class plan</v>
       </c>
       <c r="Q6" s="5">
         <v>-5</v>
@@ -2638,43 +2836,43 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E7" s="5">
-        <v>-8</v>
+        <v>-13</v>
       </c>
       <c r="F7" s="30">
         <f>MAX(Periods[Id]) -1</f>
         <v>4</v>
       </c>
-      <c r="G7" s="30" t="str">
+      <c r="G7" s="30">
         <f t="array" ref="G7">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
+        <v>24</v>
       </c>
       <c r="H7" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="I7" s="6" t="str">
+        <v>Read all article abstracts</v>
+      </c>
+      <c r="I7" s="6">
         <f t="array" ref="I7">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v/>
+        <v>0.15625</v>
       </c>
       <c r="J7" s="30" t="str">
-        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</f>
+        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="5">
-        <v>-9</v>
+        <v>-12</v>
       </c>
       <c r="M7" s="30">
         <f>MAX(Periods[Id])</f>
         <v>5</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="5" t="str">
         <f t="array" ref="N7">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>27</v>
+        <v/>
       </c>
       <c r="O7" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v>Finish a complete class plan</v>
+        <v/>
       </c>
       <c r="Q7" s="5">
         <v>-6</v>
@@ -2686,7 +2884,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E8" s="5">
-        <v>-14</v>
+        <v>-9</v>
       </c>
       <c r="F8" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -2694,23 +2892,23 @@
       </c>
       <c r="G8" s="30">
         <f t="array" ref="G8">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>13</v>
-      </c>
-      <c r="H8" t="str">
+        <v>29</v>
+      </c>
+      <c r="H8" s="15" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v>Introduction to Statistical Learning Chp 2</v>
+        <v>Integrate into UVA System</v>
       </c>
       <c r="I8" s="6">
         <f t="array" ref="I8">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v>2.083333333333337E-2</v>
-      </c>
-      <c r="J8" s="30" t="b">
-        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</f>
-        <v>1</v>
+        <v>9.3749999999999889E-2</v>
+      </c>
+      <c r="J8" s="30" t="str">
+        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
+        <v/>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="5">
-        <v>-14</v>
+        <v>-5</v>
       </c>
       <c r="M8" s="30">
         <f>MAX(Periods[Id])</f>
@@ -2734,7 +2932,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E9" s="5">
-        <v>-15</v>
+        <v>-8</v>
       </c>
       <c r="F9" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -2753,12 +2951,12 @@
         <v/>
       </c>
       <c r="J9" s="30" t="str">
-        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</f>
+        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="5">
-        <v>-10</v>
+        <v>-11</v>
       </c>
       <c r="M9" s="30">
         <f>MAX(Periods[Id])</f>
@@ -2801,7 +2999,7 @@
         <v/>
       </c>
       <c r="J10" s="30" t="str">
-        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</f>
+        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
       <c r="K10" s="2"/>
@@ -2849,7 +3047,7 @@
         <v/>
       </c>
       <c r="J11" s="30" t="str">
-        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</f>
+        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
       <c r="K11" s="2"/>
@@ -2897,7 +3095,7 @@
         <v/>
       </c>
       <c r="J12" s="30" t="str">
-        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</f>
+        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
       <c r="K12" s="2"/>
@@ -2938,7 +3136,7 @@
         <v/>
       </c>
       <c r="J13" s="30" t="str">
-        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</f>
+        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
       <c r="K13" s="2"/>
@@ -2979,7 +3177,7 @@
         <v/>
       </c>
       <c r="J14" s="30" t="str">
-        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</f>
+        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
       <c r="K14" s="2"/>
@@ -3020,7 +3218,7 @@
         <v/>
       </c>
       <c r="J15" s="30" t="str">
-        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</f>
+        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
       <c r="K15" s="2"/>
@@ -3061,7 +3259,7 @@
         <v/>
       </c>
       <c r="J16" s="30" t="str">
-        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</f>
+        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
       <c r="K16" s="2"/>
@@ -3102,7 +3300,7 @@
         <v/>
       </c>
       <c r="J17" s="30" t="str">
-        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</f>
+        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
       <c r="K17" s="2"/>
@@ -3143,7 +3341,7 @@
         <v/>
       </c>
       <c r="J18" s="30" t="str">
-        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</f>
+        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
       <c r="K18" s="2"/>
@@ -3184,7 +3382,7 @@
         <v/>
       </c>
       <c r="J19" s="30" t="str">
-        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</f>
+        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
       <c r="K19" s="2"/>
@@ -3225,7 +3423,7 @@
         <v/>
       </c>
       <c r="J20" s="30" t="str">
-        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</f>
+        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
       <c r="K20" s="2"/>
@@ -3266,7 +3464,7 @@
         <v/>
       </c>
       <c r="J21" s="30" t="str">
-        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))))</f>
+        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
       <c r="K21" s="2"/>
@@ -3303,7 +3501,7 @@
   <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView showGridLines="0" showRuler="0" view="pageLayout" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3332,11 +3530,11 @@
       <c r="G1" s="24"/>
       <c r="H1" s="24"/>
       <c r="I1" s="23"/>
-      <c r="J1" s="46">
+      <c r="J1" s="41">
         <f>MAX(Periods[Start])</f>
         <v>42529</v>
       </c>
-      <c r="K1" s="47"/>
+      <c r="K1" s="42"/>
       <c r="L1" s="13"/>
       <c r="M1" s="7"/>
     </row>
@@ -3359,10 +3557,10 @@
       </c>
       <c r="B3" s="27"/>
       <c r="C3" s="27"/>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="37" t="s">
+      <c r="E3" s="35" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="16"/>
@@ -3383,18 +3581,18 @@
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
-      <c r="D4" s="43">
+      <c r="D4" s="45">
         <f t="array" ref="D4:D12">LastWeekTasks[Hours]</f>
         <v>0</v>
       </c>
-      <c r="E4" s="35" t="b">
+      <c r="E4" s="43" t="str">
         <f t="array" ref="E4:E18">LastWeekTasks[Done]</f>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="F4" s="16"/>
-      <c r="H4" s="10" t="str">
+      <c r="H4" s="17" t="str">
         <f t="array" ref="H4:H18">ThisWeekTasks[Description]</f>
-        <v/>
+        <v>Send Jayne my TA preferences</v>
       </c>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
@@ -3405,19 +3603,19 @@
     </row>
     <row r="5" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="32" t="str">
-        <v>Reinforcement Learning an Introduction</v>
+        <v>Add hours to update sheet</v>
       </c>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
-      <c r="D5" s="44">
-        <v>0</v>
-      </c>
-      <c r="E5" s="36" t="b">
-        <v>0</v>
+      <c r="D5" s="46">
+        <v>0.17708333333333326</v>
+      </c>
+      <c r="E5" s="44" t="str">
+        <v>X</v>
       </c>
       <c r="F5" s="15"/>
       <c r="H5" s="32" t="str">
-        <v>Read all article abstracts</v>
+        <v>Reinforcement Learning an Introduction</v>
       </c>
       <c r="I5" s="33"/>
       <c r="J5" s="33"/>
@@ -3429,19 +3627,19 @@
     </row>
     <row r="6" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="str">
-        <v>Finish a complete class plan</v>
+        <v>Introduction to Statistical Learning Chp 2</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
-      <c r="D6" s="45">
-        <v>0.19791666666666674</v>
-      </c>
-      <c r="E6" s="35" t="b">
-        <v>0</v>
+      <c r="D6" s="47">
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E6" s="43" t="str">
+        <v>X</v>
       </c>
       <c r="F6" s="15"/>
       <c r="H6" s="10" t="str">
-        <v/>
+        <v>Read all article abstracts</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
@@ -3453,19 +3651,19 @@
     </row>
     <row r="7" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="str">
-        <v>Add hours to update sheet</v>
+        <v>Finish a complete class plan</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
-      <c r="D7" s="45">
-        <v>0.17708333333333326</v>
-      </c>
-      <c r="E7" s="35" t="b">
-        <v>1</v>
+      <c r="D7" s="47">
+        <v>0.19791666666666674</v>
+      </c>
+      <c r="E7" s="43" t="str">
+        <v/>
       </c>
       <c r="F7" s="15"/>
       <c r="H7" s="10" t="str">
-        <v>Write Jayne my TA preferences</v>
+        <v>Integrate into UVA System</v>
       </c>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
@@ -3477,20 +3675,20 @@
     </row>
     <row r="8" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="str">
-        <v>Read all article abstracts</v>
+        <v>Reinforcement Learning an Introduction</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
-      <c r="D8" s="45">
-        <v>6.25E-2</v>
-      </c>
-      <c r="E8" s="35" t="b">
+      <c r="D8" s="47">
         <v>0</v>
+      </c>
+      <c r="E8" s="43" t="str">
+        <v/>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="13"/>
       <c r="H8" s="10" t="str">
-        <v>Reinforcement Learning an Introduction</v>
+        <v>Finish a complete class plan</v>
       </c>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
@@ -3502,20 +3700,20 @@
     </row>
     <row r="9" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="str">
-        <v/>
+        <v>Read all article abstracts</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
-      <c r="D9" s="45" t="str">
-        <v/>
-      </c>
-      <c r="E9" s="35" t="str">
+      <c r="D9" s="47">
+        <v>0.15625</v>
+      </c>
+      <c r="E9" s="43" t="str">
         <v/>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="13"/>
       <c r="H9" s="10" t="str">
-        <v>Finish a complete class plan</v>
+        <v/>
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
@@ -3527,15 +3725,15 @@
     </row>
     <row r="10" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="str">
-        <v>Introduction to Statistical Learning Chp 2</v>
+        <v>Integrate into UVA System</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
-      <c r="D10" s="45">
-        <v>2.083333333333337E-2</v>
-      </c>
-      <c r="E10" s="35" t="b">
-        <v>1</v>
+      <c r="D10" s="47">
+        <v>9.3749999999999889E-2</v>
+      </c>
+      <c r="E10" s="43" t="str">
+        <v/>
       </c>
       <c r="F10" s="15"/>
       <c r="G10" s="13"/>
@@ -3556,10 +3754,10 @@
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
-      <c r="D11" s="45" t="str">
-        <v/>
-      </c>
-      <c r="E11" s="35" t="str">
+      <c r="D11" s="47" t="str">
+        <v/>
+      </c>
+      <c r="E11" s="43" t="str">
         <v/>
       </c>
       <c r="F11" s="15"/>
@@ -3581,10 +3779,10 @@
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
-      <c r="D12" s="43" t="str">
-        <v/>
-      </c>
-      <c r="E12" s="35" t="str">
+      <c r="D12" s="45" t="str">
+        <v/>
+      </c>
+      <c r="E12" s="43" t="str">
         <v/>
       </c>
       <c r="F12" s="12"/>
@@ -3742,37 +3940,37 @@
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="41"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="39"/>
       <c r="L20" s="12"/>
       <c r="M20"/>
     </row>
     <row r="21" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="str">
         <f t="array" ref="A21:A30">ThisWeekQuestions[Question]</f>
-        <v>What classes am I "qualified" to GTA?</v>
+        <v>Can I use my own branch in literature?</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="42"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
       <c r="L21" s="14"/>
       <c r="M21"/>
     </row>
     <row r="22" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A22" s="32" t="str">
-        <v>How have HHS systems been modeled?</v>
+        <v>What classes am I "qualified" to GTA?</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
@@ -3789,7 +3987,7 @@
     </row>
     <row r="23" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="str">
-        <v>Can we design a CHS conceptual framework that works in all situations</v>
+        <v>How have HHS systems been modeled?</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
@@ -3806,7 +4004,7 @@
     </row>
     <row r="24" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="str">
-        <v/>
+        <v>Can we design a CHS conceptual framework that works in all situations</v>
       </c>
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
@@ -4034,65 +4232,65 @@
     <mergeCell ref="J1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:E18">
-    <cfRule type="expression" dxfId="14" priority="13">
+    <cfRule type="expression" dxfId="20" priority="13">
       <formula>INDIRECT("A"&amp;ROW()) &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="14">
+    <cfRule type="expression" dxfId="19" priority="14">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="15">
+    <cfRule type="expression" dxfId="18" priority="15">
       <formula>INDIRECT("A"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:K18">
-    <cfRule type="expression" dxfId="11" priority="10">
+    <cfRule type="expression" dxfId="6" priority="10">
       <formula>INDIRECT("H"&amp;ROW()) &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="17" priority="11">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="12">
+    <cfRule type="expression" dxfId="16" priority="12">
       <formula>INDIRECT("H"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:K30">
-    <cfRule type="expression" dxfId="8" priority="7">
+    <cfRule type="expression" dxfId="15" priority="7">
       <formula>INDIRECT("A"&amp;ROW()) &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="14" priority="8">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="9">
+    <cfRule type="expression" dxfId="13" priority="9">
       <formula>INDIRECT("A"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H12">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="12" priority="6">
       <formula>INDIRECT("H"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:K12">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="11" priority="5">
       <formula>INDIRECT("H"&amp;ROW()) &lt;&gt; ""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A12">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="10" priority="4">
       <formula>INDIRECT("A"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E12">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>INDIRECT("A"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:A30">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="8" priority="2">
       <formula>INDIRECT("A"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21:K30">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>INDIRECT("A"&amp;ROW()) &lt;&gt; ""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update and work on course plans
</commit_message>
<xml_diff>
--- a/updates/Updates.xlsx
+++ b/updates/Updates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Goals" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="87">
   <si>
     <t>Install JabRef on my personal machine</t>
   </si>
@@ -289,9 +289,6 @@
     <t>Reading Abstracts</t>
   </si>
   <si>
-    <t>Can we design a CHS conceptual framework that works in all situations</t>
-  </si>
-  <si>
     <t>How have HHS systems been modeled?</t>
   </si>
   <si>
@@ -317,6 +314,30 @@
   </si>
   <si>
     <t>Integrate into UVA System</t>
+  </si>
+  <si>
+    <t>I have a wedding in OKC on January 14th?</t>
+  </si>
+  <si>
+    <t>Can we design a CHS conceptual framework that works in all situations?</t>
+  </si>
+  <si>
+    <t>Human system isn't idempotent. It learns based on past inputs.</t>
+  </si>
+  <si>
+    <t>I'm interested in machine learning but does that help me model?</t>
+  </si>
+  <si>
+    <t>Can we model ubiquitious computing's impact on a community without individuals?</t>
+  </si>
+  <si>
+    <t>Can we model ubiquitious computing's impact on any or just one at a time?</t>
+  </si>
+  <si>
+    <t>Can we look at how physical infrastructure impacts a community for inspiration?</t>
+  </si>
+  <si>
+    <t>Reviewing Course Listings Again</t>
   </si>
 </sst>
 </file>
@@ -520,7 +541,7 @@
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -574,12 +595,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -596,6 +611,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma 2" xfId="3"/>
@@ -604,145 +633,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="54">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
+  <dxfs count="40">
     <dxf>
       <numFmt numFmtId="25" formatCode="h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="h:mm"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <border>
@@ -835,9 +728,6 @@
     </dxf>
     <dxf>
       <border>
-        <left/>
-        <right/>
-        <top/>
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
@@ -870,6 +760,13 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -889,9 +786,6 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="h:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -915,6 +809,21 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -969,31 +878,31 @@
     <sortCondition ref="D2:D30"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="8" name="Id" dataDxfId="53"/>
+    <tableColumn id="8" name="Id" dataDxfId="39"/>
     <tableColumn id="1" name="Description"/>
     <tableColumn id="2" name="Comments"/>
-    <tableColumn id="4" name="Due" dataDxfId="52"/>
-    <tableColumn id="3" name="Started" dataDxfId="51"/>
-    <tableColumn id="5" name="Finished" dataDxfId="50"/>
+    <tableColumn id="4" name="Due" dataDxfId="38"/>
+    <tableColumn id="3" name="Started" dataDxfId="37"/>
+    <tableColumn id="5" name="Finished" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Times" displayName="Times" ref="A1:H15" totalsRowShown="0">
-  <autoFilter ref="A1:H15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Times" displayName="Times" ref="A1:H16" totalsRowShown="0">
+  <autoFilter ref="A1:H16"/>
   <tableColumns count="8">
     <tableColumn id="4" name="Work"/>
     <tableColumn id="9" name="Period"/>
     <tableColumn id="5" name="Date"/>
-    <tableColumn id="6" name="Start" dataDxfId="5"/>
-    <tableColumn id="7" name="End" dataDxfId="4"/>
-    <tableColumn id="1" name="Hours" dataDxfId="3">
+    <tableColumn id="6" name="Start" dataDxfId="35"/>
+    <tableColumn id="7" name="End" dataDxfId="34"/>
+    <tableColumn id="1" name="Hours" dataDxfId="33">
       <calculatedColumnFormula>Times[[#This Row],[End]]-Times[[#This Row],[Start]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Goal" dataDxfId="2"/>
-    <tableColumn id="3" name="Goal Description" dataDxfId="1">
+    <tableColumn id="2" name="Goal" dataDxfId="32"/>
+    <tableColumn id="3" name="Goal Description" dataDxfId="31">
       <calculatedColumnFormula>VLOOKUP(Times[[#This Row],[Goal]], Goals[], 2, FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1002,8 +911,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Questions" displayName="Questions" ref="A1:C10" totalsRowShown="0">
-  <autoFilter ref="A1:C10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Questions" displayName="Questions" ref="A1:C16" totalsRowShown="0">
+  <autoFilter ref="A1:C16"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Question"/>
     <tableColumn id="2" name="Answer"/>
@@ -1014,13 +923,16 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Periods" displayName="Periods" ref="A1:C6" totalsRowShown="0">
-  <autoFilter ref="A1:C6"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Id" dataDxfId="49"/>
-    <tableColumn id="2" name="Start" dataDxfId="48"/>
-    <tableColumn id="3" name="End" dataDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Periods" displayName="Periods" ref="A1:D6" totalsRowShown="0">
+  <autoFilter ref="A1:D6"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Id" dataDxfId="30"/>
+    <tableColumn id="2" name="Start" dataDxfId="29"/>
+    <tableColumn id="3" name="End" dataDxfId="28">
       <calculatedColumnFormula>Periods[[#This Row],[Start]] + (7)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="Hours" dataDxfId="0">
+      <calculatedColumnFormula array="1">SUM((Times[Period] = Periods[[#This Row],[Id]]) * Times[Hours])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1028,26 +940,26 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="LastWeekTasks" displayName="LastWeekTasks" ref="E1:J21" totalsRowShown="0">
-  <autoFilter ref="E1:J21"/>
-  <sortState ref="E2:J21">
-    <sortCondition descending="1" ref="J1:J21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="LastWeekTasks" displayName="LastWeekTasks" ref="F1:K21" totalsRowShown="0">
+  <autoFilter ref="F1:K21"/>
+  <sortState ref="F2:K21">
+    <sortCondition descending="1" ref="K1:K21"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="2" name="Index" dataDxfId="46"/>
-    <tableColumn id="4" name="Period" dataDxfId="45">
+    <tableColumn id="2" name="Index" dataDxfId="27"/>
+    <tableColumn id="4" name="Period" dataDxfId="26">
       <calculatedColumnFormula>MAX(Periods[Id]) -1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Goal" dataDxfId="44">
+    <tableColumn id="5" name="Goal" dataDxfId="25">
       <calculatedColumnFormula array="1">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Goal Description" dataDxfId="43">
+    <tableColumn id="1" name="Goal Description" dataDxfId="24">
       <calculatedColumnFormula>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Hours" dataDxfId="42">
+    <tableColumn id="6" name="Hours" dataDxfId="17">
       <calculatedColumnFormula array="1">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Done" dataDxfId="0">
+    <tableColumn id="3" name="Done" dataDxfId="16">
       <calculatedColumnFormula>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1056,20 +968,20 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="ThisWeekTasks" displayName="ThisWeekTasks" ref="L1:O21" totalsRowShown="0">
-  <autoFilter ref="L1:O21"/>
-  <sortState ref="L2:O21">
-    <sortCondition descending="1" ref="O1:O21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="ThisWeekTasks" displayName="ThisWeekTasks" ref="M1:P21" totalsRowShown="0">
+  <autoFilter ref="M1:P21"/>
+  <sortState ref="M2:P21">
+    <sortCondition descending="1" ref="P1:P21"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="2" name="Index" dataDxfId="41"/>
-    <tableColumn id="6" name="Period" dataDxfId="40">
+    <tableColumn id="2" name="Index" dataDxfId="23"/>
+    <tableColumn id="6" name="Period" dataDxfId="22">
       <calculatedColumnFormula>MAX(Periods[Id])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Goal" dataDxfId="39">
+    <tableColumn id="5" name="Goal" dataDxfId="21">
       <calculatedColumnFormula array="1">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Description" dataDxfId="38">
+    <tableColumn id="1" name="Description" dataDxfId="20">
       <calculatedColumnFormula>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1078,14 +990,14 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="ThisWeekQuestions" displayName="ThisWeekQuestions" ref="Q1:R11" totalsRowShown="0">
-  <autoFilter ref="Q1:R11"/>
-  <sortState ref="Q2:R21">
-    <sortCondition descending="1" ref="Q1:Q21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="ThisWeekQuestions" displayName="ThisWeekQuestions" ref="R1:S12" totalsRowShown="0">
+  <autoFilter ref="R1:S12"/>
+  <sortState ref="R2:S12">
+    <sortCondition descending="1" ref="R1:R21"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="2" name="Index" dataDxfId="37"/>
-    <tableColumn id="1" name="Question" dataDxfId="36">
+    <tableColumn id="2" name="Index" dataDxfId="19"/>
+    <tableColumn id="1" name="Question" dataDxfId="18">
       <calculatedColumnFormula array="1">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1383,7 +1295,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:E22"/>
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1761,7 +1673,7 @@
         <v>29</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D22" s="2">
         <v>42597</v>
@@ -1776,7 +1688,7 @@
         <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D23" s="2">
         <v>42538</v>
@@ -1818,7 +1730,7 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D26" s="2">
         <v>42585</v>
@@ -1871,7 +1783,7 @@
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D30" s="2">
         <v>42587</v>
@@ -1900,10 +1812,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2279,7 +2191,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -2307,7 +2219,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -2333,10 +2245,38 @@
         <v>Read all article abstracts</v>
       </c>
     </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16" s="3">
+        <v>42894</v>
+      </c>
+      <c r="D16" s="6">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E16" s="6">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="F16" s="6">
+        <f>Times[[#This Row],[End]]-Times[[#This Row],[Start]]</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="G16" s="30">
+        <v>27</v>
+      </c>
+      <c r="H16" s="6" t="str">
+        <f>VLOOKUP(Times[[#This Row],[Goal]], Goals[], 2, FALSE)</f>
+        <v>Finish a complete class plan</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" sqref="G2:H15"/>
+    <dataValidation allowBlank="1" showInputMessage="1" sqref="G2:H16"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2348,15 +2288,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="65.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="76.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="83" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2428,7 +2368,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C7" s="3">
         <v>42527</v>
@@ -2436,7 +2376,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C8" s="3">
         <v>42527</v>
@@ -2444,7 +2384,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C9" s="3">
         <v>42527</v>
@@ -2452,10 +2392,40 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C10" s="3">
         <v>42528</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2468,34 +2438,34 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" customWidth="1"/>
-    <col min="6" max="6" width="5.140625" customWidth="1"/>
-    <col min="7" max="7" width="5.28515625" customWidth="1"/>
-    <col min="8" max="8" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.42578125" customWidth="1"/>
-    <col min="12" max="12" width="6.42578125" customWidth="1"/>
-    <col min="13" max="13" width="5" customWidth="1"/>
-    <col min="14" max="14" width="6" customWidth="1"/>
-    <col min="15" max="15" width="43.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.42578125" customWidth="1"/>
-    <col min="18" max="18" width="65.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" customWidth="1"/>
+    <col min="7" max="7" width="5.140625" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" customWidth="1"/>
+    <col min="9" max="9" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.42578125" customWidth="1"/>
+    <col min="13" max="13" width="6.42578125" customWidth="1"/>
+    <col min="14" max="14" width="5" customWidth="1"/>
+    <col min="15" max="15" width="6" customWidth="1"/>
+    <col min="16" max="16" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.42578125" customWidth="1"/>
+    <col min="19" max="19" width="65.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -2505,44 +2475,47 @@
       <c r="C1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>41</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>46</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>47</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>38</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>26</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>29</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>41</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>46</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>29</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="30">
         <v>1</v>
       </c>
@@ -2553,55 +2526,59 @@
         <f>Periods[[#This Row],[Start]] + (7)</f>
         <v>42508</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="5">
+      <c r="D2" s="6">
+        <f t="array" ref="D2">SUM((Times[Period] = Periods[[#This Row],[Id]]) * Times[Hours])</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="5">
         <v>-11</v>
       </c>
-      <c r="F2" s="30">
+      <c r="G2" s="30">
         <f>MAX(Periods[Id]) -1</f>
         <v>4</v>
       </c>
-      <c r="G2" s="30">
-        <f t="array" ref="G2">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
+      <c r="H2" s="30">
+        <f t="array" ref="H2">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
         <v>26</v>
       </c>
-      <c r="H2" t="str">
+      <c r="I2" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v>Account for conferences in pub plan</v>
       </c>
-      <c r="I2" s="6">
-        <f t="array" ref="I2">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
+      <c r="J2" s="6">
+        <f t="array" ref="J2">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v>0</v>
       </c>
-      <c r="J2" s="48" t="str">
+      <c r="K2" s="49" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v>X</v>
       </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="5">
+      <c r="L2" s="2"/>
+      <c r="M2" s="5">
         <v>-8</v>
       </c>
-      <c r="M2" s="30">
+      <c r="N2" s="30">
         <f>MAX(Periods[Id])</f>
         <v>5</v>
       </c>
-      <c r="N2" s="5">
-        <f t="array" ref="N2">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
+      <c r="O2" s="5">
+        <f t="array" ref="O2">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
         <v>18</v>
       </c>
-      <c r="O2" t="str">
+      <c r="P2" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v>Send Jayne my TA preferences</v>
       </c>
-      <c r="Q2" s="5">
+      <c r="R2" s="5">
         <v>-1</v>
       </c>
-      <c r="R2" t="str">
-        <f t="array" ref="R2">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v>Can I use my own branch in literature?</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S2" t="str">
+        <f t="array" ref="S2">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
+        <v>Can we look at how physical infrastructure impacts a community for inspiration?</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="30">
         <v>2</v>
       </c>
@@ -2612,55 +2589,59 @@
         <f>Periods[[#This Row],[Start]] + (7)</f>
         <v>42515</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="5">
+      <c r="D3" s="6">
+        <f t="array" ref="D3">SUM((Times[Period] = Periods[[#This Row],[Id]]) * Times[Hours])</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="5">
         <v>-12</v>
       </c>
-      <c r="F3" s="30">
+      <c r="G3" s="30">
         <f>MAX(Periods[Id]) -1</f>
         <v>4</v>
       </c>
-      <c r="G3" s="30">
-        <f t="array" ref="G3">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
+      <c r="H3" s="30">
+        <f t="array" ref="H3">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
         <v>25</v>
       </c>
-      <c r="H3" t="str">
+      <c r="I3" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v>Add hours to update sheet</v>
       </c>
-      <c r="I3" s="6">
-        <f t="array" ref="I3">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
+      <c r="J3" s="6">
+        <f t="array" ref="J3">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v>0.17708333333333326</v>
       </c>
-      <c r="J3" s="30" t="str">
+      <c r="K3" s="50" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v>X</v>
       </c>
-      <c r="K3" s="2"/>
-      <c r="L3" s="5">
+      <c r="L3" s="2"/>
+      <c r="M3" s="5">
         <v>-14</v>
       </c>
-      <c r="M3" s="30">
+      <c r="N3" s="30">
         <f>MAX(Periods[Id])</f>
         <v>5</v>
       </c>
-      <c r="N3" s="5">
-        <f t="array" ref="N3">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
+      <c r="O3" s="5">
+        <f t="array" ref="O3">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
         <v>14</v>
       </c>
-      <c r="O3" t="str">
+      <c r="P3" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v>Reinforcement Learning an Introduction</v>
       </c>
-      <c r="Q3" s="5">
+      <c r="R3" s="5">
         <v>-2</v>
       </c>
-      <c r="R3" t="str">
-        <f t="array" ref="R3">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v>What classes am I "qualified" to GTA?</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S3" t="str">
+        <f t="array" ref="S3">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
+        <v>Can we model ubiquitious computing's impact on any or just one at a time?</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="30">
         <v>3</v>
       </c>
@@ -2671,54 +2652,58 @@
         <f>Periods[[#This Row],[Start]] + (7)</f>
         <v>42522</v>
       </c>
-      <c r="E4" s="5">
+      <c r="D4" s="6">
+        <f t="array" ref="D4">SUM((Times[Period] = Periods[[#This Row],[Id]]) * Times[Hours])</f>
+        <v>0.25000000000000006</v>
+      </c>
+      <c r="F4" s="5">
         <v>-15</v>
       </c>
-      <c r="F4" s="30">
+      <c r="G4" s="30">
         <f>MAX(Periods[Id]) -1</f>
         <v>4</v>
       </c>
-      <c r="G4" s="30">
-        <f t="array" ref="G4">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
+      <c r="H4" s="30">
+        <f t="array" ref="H4">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
         <v>13</v>
       </c>
-      <c r="H4" t="str">
+      <c r="I4" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v>Introduction to Statistical Learning Chp 2</v>
       </c>
-      <c r="I4" s="6">
-        <f t="array" ref="I4">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
+      <c r="J4" s="6">
+        <f t="array" ref="J4">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v>2.083333333333337E-2</v>
       </c>
-      <c r="J4" s="30" t="str">
+      <c r="K4" s="50" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v>X</v>
       </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="5">
+      <c r="L4" s="2"/>
+      <c r="M4" s="5">
         <v>-13</v>
       </c>
-      <c r="M4" s="30">
+      <c r="N4" s="30">
         <f>MAX(Periods[Id])</f>
         <v>5</v>
       </c>
-      <c r="N4" s="5">
-        <f t="array" ref="N4">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
+      <c r="O4" s="5">
+        <f t="array" ref="O4">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
         <v>24</v>
       </c>
-      <c r="O4" t="str">
+      <c r="P4" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v>Read all article abstracts</v>
       </c>
-      <c r="Q4" s="5">
+      <c r="R4" s="5">
         <v>-3</v>
       </c>
-      <c r="R4" t="str">
-        <f t="array" ref="R4">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v>How have HHS systems been modeled?</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S4" t="str">
+        <f t="array" ref="S4">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
+        <v>Can we model ubiquitious computing's impact on a community without individuals?</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="30">
         <v>4</v>
       </c>
@@ -2729,54 +2714,58 @@
         <f>Periods[[#This Row],[Start]] + (7)</f>
         <v>42529</v>
       </c>
-      <c r="E5" s="5">
+      <c r="D5" s="6">
+        <f t="array" ref="D5">SUM((Times[Period] = Periods[[#This Row],[Id]]) * Times[Hours])</f>
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="F5" s="5">
         <v>-10</v>
       </c>
-      <c r="F5" s="30">
+      <c r="G5" s="30">
         <f>MAX(Periods[Id]) -1</f>
         <v>4</v>
       </c>
-      <c r="G5" s="30">
-        <f t="array" ref="G5">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
+      <c r="H5" s="30">
+        <f t="array" ref="H5">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
         <v>27</v>
       </c>
-      <c r="H5" t="str">
+      <c r="I5" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v>Finish a complete class plan</v>
       </c>
-      <c r="I5" s="6">
-        <f t="array" ref="I5">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v>0.19791666666666674</v>
-      </c>
-      <c r="J5" s="30" t="str">
+      <c r="J5" s="6">
+        <f t="array" ref="J5">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
+        <v>0.26041666666666674</v>
+      </c>
+      <c r="K5" s="50" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
-      <c r="K5" s="2"/>
-      <c r="L5" s="5">
+      <c r="L5" s="2"/>
+      <c r="M5" s="5">
         <v>-9</v>
       </c>
-      <c r="M5" s="30">
+      <c r="N5" s="30">
         <f>MAX(Periods[Id])</f>
         <v>5</v>
       </c>
-      <c r="N5" s="5">
-        <f t="array" ref="N5">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
+      <c r="O5" s="5">
+        <f t="array" ref="O5">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
         <v>29</v>
       </c>
-      <c r="O5" t="str">
+      <c r="P5" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v>Integrate into UVA System</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="R5" s="5">
         <v>-4</v>
       </c>
-      <c r="R5" t="str">
-        <f t="array" ref="R5">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v>Can we design a CHS conceptual framework that works in all situations</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S5" t="str">
+        <f t="array" ref="S5">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
+        <v>I'm interested in machine learning but does that help me model?</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="30">
         <v>5</v>
       </c>
@@ -2787,699 +2776,710 @@
         <f>Periods[[#This Row],[Start]] + (7)</f>
         <v>42536</v>
       </c>
-      <c r="E6" s="5">
+      <c r="D6" s="6">
+        <f t="array" ref="D6">SUM((Times[Period] = Periods[[#This Row],[Id]]) * Times[Hours])</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
         <v>-14</v>
       </c>
-      <c r="F6" s="30">
+      <c r="G6" s="30">
         <f>MAX(Periods[Id]) -1</f>
         <v>4</v>
       </c>
-      <c r="G6" s="30">
-        <f t="array" ref="G6">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
+      <c r="H6" s="30">
+        <f t="array" ref="H6">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
         <v>14</v>
       </c>
-      <c r="H6" t="str">
+      <c r="I6" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v>Reinforcement Learning an Introduction</v>
       </c>
-      <c r="I6" s="6">
-        <f t="array" ref="I6">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
+      <c r="J6" s="6">
+        <f t="array" ref="J6">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v>0</v>
       </c>
-      <c r="J6" s="30" t="str">
+      <c r="K6" s="50" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="5">
+      <c r="L6" s="2"/>
+      <c r="M6" s="5">
         <v>-10</v>
       </c>
-      <c r="M6" s="30">
+      <c r="N6" s="30">
         <f>MAX(Periods[Id])</f>
         <v>5</v>
       </c>
-      <c r="N6" s="5">
-        <f t="array" ref="N6">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
+      <c r="O6" s="5">
+        <f t="array" ref="O6">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
         <v>27</v>
       </c>
-      <c r="O6" t="str">
+      <c r="P6" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v>Finish a complete class plan</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="R6" s="5">
         <v>-5</v>
       </c>
-      <c r="R6" t="str">
-        <f t="array" ref="R6">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E7" s="5">
+      <c r="S6" t="str">
+        <f t="array" ref="S6">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
+        <v>Human system isn't idempotent. It learns based on past inputs.</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F7" s="5">
         <v>-13</v>
       </c>
-      <c r="F7" s="30">
+      <c r="G7" s="30">
         <f>MAX(Periods[Id]) -1</f>
         <v>4</v>
       </c>
-      <c r="G7" s="30">
-        <f t="array" ref="G7">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
+      <c r="H7" s="30">
+        <f t="array" ref="H7">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
         <v>24</v>
       </c>
-      <c r="H7" t="str">
+      <c r="I7" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v>Read all article abstracts</v>
       </c>
-      <c r="I7" s="6">
-        <f t="array" ref="I7">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
+      <c r="J7" s="6">
+        <f t="array" ref="J7">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v>0.15625</v>
       </c>
-      <c r="J7" s="30" t="str">
+      <c r="K7" s="50" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="5">
+      <c r="L7" s="2"/>
+      <c r="M7" s="5">
         <v>-12</v>
       </c>
-      <c r="M7" s="30">
+      <c r="N7" s="30">
         <f>MAX(Periods[Id])</f>
         <v>5</v>
       </c>
-      <c r="N7" s="5" t="str">
-        <f t="array" ref="N7">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="O7" t="str">
+      <c r="O7" s="5" t="str">
+        <f t="array" ref="O7">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
+        <v/>
+      </c>
+      <c r="P7" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="Q7" s="5">
+      <c r="R7" s="5">
         <v>-6</v>
       </c>
-      <c r="R7" t="str">
-        <f t="array" ref="R7">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E8" s="5">
+      <c r="S7" t="str">
+        <f t="array" ref="S7">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
+        <v>I have a wedding in OKC on January 14th?</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F8" s="5">
         <v>-9</v>
       </c>
-      <c r="F8" s="30">
+      <c r="G8" s="30">
         <f>MAX(Periods[Id]) -1</f>
         <v>4</v>
       </c>
-      <c r="G8" s="30">
-        <f t="array" ref="G8">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
+      <c r="H8" s="30">
+        <f t="array" ref="H8">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
         <v>29</v>
       </c>
-      <c r="H8" s="15" t="str">
+      <c r="I8" s="15" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v>Integrate into UVA System</v>
       </c>
-      <c r="I8" s="6">
-        <f t="array" ref="I8">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
+      <c r="J8" s="6">
+        <f t="array" ref="J8">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v>9.3749999999999889E-2</v>
       </c>
-      <c r="J8" s="30" t="str">
+      <c r="K8" s="50" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
-      <c r="K8" s="2"/>
-      <c r="L8" s="5">
+      <c r="L8" s="2"/>
+      <c r="M8" s="5">
         <v>-5</v>
       </c>
-      <c r="M8" s="30">
+      <c r="N8" s="30">
         <f>MAX(Periods[Id])</f>
         <v>5</v>
       </c>
-      <c r="N8" s="5" t="str">
-        <f t="array" ref="N8">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="O8" t="str">
+      <c r="O8" s="5" t="str">
+        <f t="array" ref="O8">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
+        <v/>
+      </c>
+      <c r="P8" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="Q8" s="5">
+      <c r="R8" s="5">
         <v>-7</v>
       </c>
-      <c r="R8" t="str">
-        <f t="array" ref="R8">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E9" s="5">
+      <c r="S8" t="str">
+        <f t="array" ref="S8">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
+        <v>Can I use my own branch in literature?</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F9" s="5">
         <v>-8</v>
       </c>
-      <c r="F9" s="30">
+      <c r="G9" s="30">
         <f>MAX(Periods[Id]) -1</f>
         <v>4</v>
       </c>
-      <c r="G9" s="30" t="str">
-        <f t="array" ref="G9">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="H9" t="str">
+      <c r="H9" s="30" t="str">
+        <f t="array" ref="H9">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
+        <v/>
+      </c>
+      <c r="I9" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="I9" s="6" t="str">
-        <f t="array" ref="I9">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v/>
-      </c>
-      <c r="J9" s="30" t="str">
+      <c r="J9" s="6" t="str">
+        <f t="array" ref="J9">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
+        <v/>
+      </c>
+      <c r="K9" s="50" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
-      <c r="K9" s="2"/>
-      <c r="L9" s="5">
+      <c r="L9" s="2"/>
+      <c r="M9" s="5">
         <v>-11</v>
       </c>
-      <c r="M9" s="30">
+      <c r="N9" s="30">
         <f>MAX(Periods[Id])</f>
         <v>5</v>
       </c>
-      <c r="N9" s="5" t="str">
-        <f t="array" ref="N9">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="O9" t="str">
+      <c r="O9" s="5" t="str">
+        <f t="array" ref="O9">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
+        <v/>
+      </c>
+      <c r="P9" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="Q9" s="5">
+      <c r="R9" s="5">
         <v>-8</v>
       </c>
-      <c r="R9" t="str">
-        <f t="array" ref="R9">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E10" s="5">
+      <c r="S9" t="str">
+        <f t="array" ref="S9">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
+        <v>What classes am I "qualified" to GTA?</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F10" s="5">
         <v>-16</v>
       </c>
-      <c r="F10" s="30">
+      <c r="G10" s="30">
         <f>MAX(Periods[Id]) -1</f>
         <v>4</v>
       </c>
-      <c r="G10" s="30" t="str">
-        <f t="array" ref="G10">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
       <c r="H10" s="30" t="str">
+        <f t="array" ref="H10">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
+        <v/>
+      </c>
+      <c r="I10" s="30" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="I10" s="6" t="str">
-        <f t="array" ref="I10">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v/>
-      </c>
-      <c r="J10" s="30" t="str">
+      <c r="J10" s="6" t="str">
+        <f t="array" ref="J10">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
+        <v/>
+      </c>
+      <c r="K10" s="50" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
-      <c r="K10" s="2"/>
-      <c r="L10" s="5">
+      <c r="L10" s="2"/>
+      <c r="M10" s="5">
         <v>-16</v>
       </c>
-      <c r="M10" s="30">
+      <c r="N10" s="30">
         <f>MAX(Periods[Id])</f>
         <v>5</v>
       </c>
-      <c r="N10" s="5" t="str">
-        <f t="array" ref="N10">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="O10" s="30" t="str">
+      <c r="O10" s="5" t="str">
+        <f t="array" ref="O10">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
+        <v/>
+      </c>
+      <c r="P10" s="30" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="Q10" s="5">
+      <c r="R10" s="5">
         <v>-9</v>
       </c>
-      <c r="R10" t="str">
-        <f t="array" ref="R10">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E11" s="5">
+      <c r="S10" t="str">
+        <f t="array" ref="S10">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
+        <v>How have HHS systems been modeled?</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F11" s="5">
         <v>-17</v>
       </c>
-      <c r="F11" s="30">
+      <c r="G11" s="30">
         <f>MAX(Periods[Id]) -1</f>
         <v>4</v>
       </c>
-      <c r="G11" s="30" t="str">
-        <f t="array" ref="G11">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
       <c r="H11" s="30" t="str">
+        <f t="array" ref="H11">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
+        <v/>
+      </c>
+      <c r="I11" s="46" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="I11" s="6" t="str">
-        <f t="array" ref="I11">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v/>
-      </c>
-      <c r="J11" s="30" t="str">
+      <c r="J11" s="6" t="str">
+        <f t="array" ref="J11">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
+        <v/>
+      </c>
+      <c r="K11" s="50" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
-      <c r="K11" s="2"/>
-      <c r="L11" s="5">
+      <c r="L11" s="2"/>
+      <c r="M11" s="5">
         <v>-15</v>
       </c>
-      <c r="M11" s="30">
+      <c r="N11" s="30">
         <f>MAX(Periods[Id])</f>
         <v>5</v>
       </c>
-      <c r="N11" s="5" t="str">
-        <f t="array" ref="N11">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="O11" t="str">
+      <c r="O11" s="5" t="str">
+        <f t="array" ref="O11">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
+        <v/>
+      </c>
+      <c r="P11" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="Q11" s="5">
+      <c r="R11" s="5">
         <v>-10</v>
       </c>
-      <c r="R11" t="str">
-        <f t="array" ref="R11">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E12" s="5">
+      <c r="S11" t="str">
+        <f t="array" ref="S11">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
+        <v>Can we design a CHS conceptual framework that works in all situations?</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F12" s="5">
         <v>-18</v>
       </c>
-      <c r="F12" s="30">
+      <c r="G12" s="30">
         <f>MAX(Periods[Id]) -1</f>
         <v>4</v>
       </c>
-      <c r="G12" s="30" t="str">
-        <f t="array" ref="G12">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
       <c r="H12" s="30" t="str">
+        <f t="array" ref="H12">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
+        <v/>
+      </c>
+      <c r="I12" s="30" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="I12" s="6" t="str">
-        <f t="array" ref="I12">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v/>
-      </c>
-      <c r="J12" s="30" t="str">
+      <c r="J12" s="6" t="str">
+        <f t="array" ref="J12">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
+        <v/>
+      </c>
+      <c r="K12" s="50" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
-      <c r="K12" s="2"/>
-      <c r="L12" s="5">
+      <c r="L12" s="2"/>
+      <c r="M12" s="5">
         <v>-1</v>
       </c>
-      <c r="M12" s="30">
+      <c r="N12" s="30">
         <f>MAX(Periods[Id])</f>
         <v>5</v>
       </c>
-      <c r="N12" s="5" t="str">
-        <f t="array" ref="N12">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="O12" t="str">
+      <c r="O12" s="5" t="str">
+        <f t="array" ref="O12">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
+        <v/>
+      </c>
+      <c r="P12" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E13" s="5">
+      <c r="R12" s="5">
+        <v>-11</v>
+      </c>
+      <c r="S12" s="30" t="str">
+        <f t="array" ref="S12">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F13" s="5">
         <v>-19</v>
       </c>
-      <c r="F13" s="30">
+      <c r="G13" s="30">
         <f>MAX(Periods[Id]) -1</f>
         <v>4</v>
       </c>
-      <c r="G13" s="30" t="str">
-        <f t="array" ref="G13">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
       <c r="H13" s="30" t="str">
+        <f t="array" ref="H13">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
+        <v/>
+      </c>
+      <c r="I13" s="30" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="I13" s="6" t="str">
-        <f t="array" ref="I13">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v/>
-      </c>
-      <c r="J13" s="30" t="str">
+      <c r="J13" s="6" t="str">
+        <f t="array" ref="J13">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
+        <v/>
+      </c>
+      <c r="K13" s="50" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
-      <c r="K13" s="2"/>
-      <c r="L13" s="5">
+      <c r="L13" s="2"/>
+      <c r="M13" s="5">
         <v>-2</v>
       </c>
-      <c r="M13" s="30">
+      <c r="N13" s="30">
         <f>MAX(Periods[Id])</f>
         <v>5</v>
       </c>
-      <c r="N13" s="5" t="str">
-        <f t="array" ref="N13">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="O13" t="str">
+      <c r="O13" s="5" t="str">
+        <f t="array" ref="O13">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
+        <v/>
+      </c>
+      <c r="P13" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E14" s="5">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F14" s="5">
         <v>-20</v>
       </c>
-      <c r="F14" s="30">
+      <c r="G14" s="30">
         <f>MAX(Periods[Id]) -1</f>
         <v>4</v>
       </c>
-      <c r="G14" s="30" t="str">
-        <f t="array" ref="G14">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
       <c r="H14" s="30" t="str">
+        <f t="array" ref="H14">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
+        <v/>
+      </c>
+      <c r="I14" s="30" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="I14" s="6" t="str">
-        <f t="array" ref="I14">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v/>
-      </c>
-      <c r="J14" s="30" t="str">
+      <c r="J14" s="6" t="str">
+        <f t="array" ref="J14">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
+        <v/>
+      </c>
+      <c r="K14" s="50" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
-      <c r="K14" s="2"/>
-      <c r="L14" s="5">
+      <c r="L14" s="2"/>
+      <c r="M14" s="5">
         <v>-3</v>
       </c>
-      <c r="M14" s="30">
+      <c r="N14" s="30">
         <f>MAX(Periods[Id])</f>
         <v>5</v>
       </c>
-      <c r="N14" s="5" t="str">
-        <f t="array" ref="N14">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="O14" t="str">
+      <c r="O14" s="5" t="str">
+        <f t="array" ref="O14">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
+        <v/>
+      </c>
+      <c r="P14" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E15" s="5">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F15" s="5">
         <v>-7</v>
       </c>
-      <c r="F15" s="30">
+      <c r="G15" s="30">
         <f>MAX(Periods[Id]) -1</f>
         <v>4</v>
       </c>
-      <c r="G15" s="30" t="str">
-        <f t="array" ref="G15">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="H15" t="str">
+      <c r="H15" s="30" t="str">
+        <f t="array" ref="H15">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
+        <v/>
+      </c>
+      <c r="I15" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="I15" s="6" t="str">
-        <f t="array" ref="I15">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v/>
-      </c>
-      <c r="J15" s="30" t="str">
+      <c r="J15" s="6" t="str">
+        <f t="array" ref="J15">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
+        <v/>
+      </c>
+      <c r="K15" s="50" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
-      <c r="K15" s="2"/>
-      <c r="L15" s="5">
+      <c r="L15" s="2"/>
+      <c r="M15" s="5">
         <v>-4</v>
       </c>
-      <c r="M15" s="30">
+      <c r="N15" s="30">
         <f>MAX(Periods[Id])</f>
         <v>5</v>
       </c>
-      <c r="N15" s="5" t="str">
-        <f t="array" ref="N15">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="O15" t="str">
+      <c r="O15" s="5" t="str">
+        <f t="array" ref="O15">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
+        <v/>
+      </c>
+      <c r="P15" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E16" s="5">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F16" s="5">
         <v>-6</v>
       </c>
-      <c r="F16" s="30">
+      <c r="G16" s="30">
         <f>MAX(Periods[Id]) -1</f>
         <v>4</v>
       </c>
-      <c r="G16" s="30" t="str">
-        <f t="array" ref="G16">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="H16" t="str">
+      <c r="H16" s="30" t="str">
+        <f t="array" ref="H16">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
+        <v/>
+      </c>
+      <c r="I16" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="I16" s="6" t="str">
-        <f t="array" ref="I16">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v/>
-      </c>
-      <c r="J16" s="30" t="str">
+      <c r="J16" s="6" t="str">
+        <f t="array" ref="J16">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
+        <v/>
+      </c>
+      <c r="K16" s="50" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
-      <c r="K16" s="2"/>
-      <c r="L16" s="5">
+      <c r="L16" s="2"/>
+      <c r="M16" s="5">
         <v>-6</v>
       </c>
-      <c r="M16" s="30">
+      <c r="N16" s="30">
         <f>MAX(Periods[Id])</f>
         <v>5</v>
       </c>
-      <c r="N16" s="5" t="str">
-        <f t="array" ref="N16">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="O16" t="str">
+      <c r="O16" s="5" t="str">
+        <f t="array" ref="O16">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
+        <v/>
+      </c>
+      <c r="P16" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E17" s="5">
+    <row r="17" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F17" s="5">
         <v>-5</v>
       </c>
-      <c r="F17" s="30">
+      <c r="G17" s="30">
         <f>MAX(Periods[Id]) -1</f>
         <v>4</v>
       </c>
-      <c r="G17" s="30" t="str">
-        <f t="array" ref="G17">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="H17" t="str">
+      <c r="H17" s="30" t="str">
+        <f t="array" ref="H17">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
+        <v/>
+      </c>
+      <c r="I17" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="I17" s="6" t="str">
-        <f t="array" ref="I17">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v/>
-      </c>
-      <c r="J17" s="30" t="str">
+      <c r="J17" s="6" t="str">
+        <f t="array" ref="J17">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
+        <v/>
+      </c>
+      <c r="K17" s="50" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
-      <c r="K17" s="2"/>
-      <c r="L17" s="5">
+      <c r="L17" s="2"/>
+      <c r="M17" s="5">
         <v>-7</v>
       </c>
-      <c r="M17" s="30">
+      <c r="N17" s="30">
         <f>MAX(Periods[Id])</f>
         <v>5</v>
       </c>
-      <c r="N17" s="5" t="str">
-        <f t="array" ref="N17">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="O17" t="str">
+      <c r="O17" s="5" t="str">
+        <f t="array" ref="O17">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
+        <v/>
+      </c>
+      <c r="P17" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E18" s="5">
+    <row r="18" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F18" s="5">
         <v>-4</v>
       </c>
-      <c r="F18" s="30">
+      <c r="G18" s="30">
         <f>MAX(Periods[Id]) -1</f>
         <v>4</v>
       </c>
-      <c r="G18" s="30" t="str">
-        <f t="array" ref="G18">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="H18" t="str">
+      <c r="H18" s="30" t="str">
+        <f t="array" ref="H18">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
+        <v/>
+      </c>
+      <c r="I18" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="I18" s="6" t="str">
-        <f t="array" ref="I18">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v/>
-      </c>
-      <c r="J18" s="30" t="str">
+      <c r="J18" s="6" t="str">
+        <f t="array" ref="J18">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
+        <v/>
+      </c>
+      <c r="K18" s="50" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
-      <c r="K18" s="2"/>
-      <c r="L18" s="5">
+      <c r="L18" s="2"/>
+      <c r="M18" s="5">
         <v>-17</v>
       </c>
-      <c r="M18" s="30">
+      <c r="N18" s="30">
         <f>MAX(Periods[Id])</f>
         <v>5</v>
       </c>
-      <c r="N18" s="5" t="str">
-        <f t="array" ref="N18">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="O18" s="30" t="str">
+      <c r="O18" s="5" t="str">
+        <f t="array" ref="O18">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
+        <v/>
+      </c>
+      <c r="P18" s="30" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E19" s="5">
+    <row r="19" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F19" s="5">
         <v>-3</v>
       </c>
-      <c r="F19" s="30">
+      <c r="G19" s="30">
         <f>MAX(Periods[Id]) -1</f>
         <v>4</v>
       </c>
-      <c r="G19" s="30" t="str">
-        <f t="array" ref="G19">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="H19" t="str">
+      <c r="H19" s="30" t="str">
+        <f t="array" ref="H19">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
+        <v/>
+      </c>
+      <c r="I19" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="I19" s="6" t="str">
-        <f t="array" ref="I19">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v/>
-      </c>
-      <c r="J19" s="30" t="str">
+      <c r="J19" s="6" t="str">
+        <f t="array" ref="J19">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
+        <v/>
+      </c>
+      <c r="K19" s="50" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
-      <c r="K19" s="2"/>
-      <c r="L19" s="5">
+      <c r="L19" s="2"/>
+      <c r="M19" s="5">
         <v>-18</v>
       </c>
-      <c r="M19" s="30">
+      <c r="N19" s="30">
         <f>MAX(Periods[Id])</f>
         <v>5</v>
       </c>
-      <c r="N19" s="5" t="str">
-        <f t="array" ref="N19">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="O19" s="30" t="str">
+      <c r="O19" s="5" t="str">
+        <f t="array" ref="O19">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
+        <v/>
+      </c>
+      <c r="P19" s="30" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E20" s="5">
+    <row r="20" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F20" s="5">
         <v>-2</v>
       </c>
-      <c r="F20" s="30">
+      <c r="G20" s="30">
         <f>MAX(Periods[Id]) -1</f>
         <v>4</v>
       </c>
-      <c r="G20" s="30" t="str">
-        <f t="array" ref="G20">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="H20" t="str">
+      <c r="H20" s="30" t="str">
+        <f t="array" ref="H20">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
+        <v/>
+      </c>
+      <c r="I20" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="I20" s="6" t="str">
-        <f t="array" ref="I20">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v/>
-      </c>
-      <c r="J20" s="30" t="str">
+      <c r="J20" s="6" t="str">
+        <f t="array" ref="J20">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
+        <v/>
+      </c>
+      <c r="K20" s="50" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
-      <c r="K20" s="2"/>
-      <c r="L20" s="5">
+      <c r="L20" s="2"/>
+      <c r="M20" s="5">
         <v>-19</v>
       </c>
-      <c r="M20" s="30">
+      <c r="N20" s="30">
         <f>MAX(Periods[Id])</f>
         <v>5</v>
       </c>
-      <c r="N20" s="5" t="str">
-        <f t="array" ref="N20">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="O20" s="30" t="str">
+      <c r="O20" s="5" t="str">
+        <f t="array" ref="O20">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
+        <v/>
+      </c>
+      <c r="P20" s="30" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E21" s="5">
+    <row r="21" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F21" s="5">
         <v>-1</v>
       </c>
-      <c r="F21" s="30">
+      <c r="G21" s="30">
         <f>MAX(Periods[Id]) -1</f>
         <v>4</v>
       </c>
-      <c r="G21" s="30" t="str">
-        <f t="array" ref="G21">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="H21" t="str">
+      <c r="H21" s="30" t="str">
+        <f t="array" ref="H21">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
+        <v/>
+      </c>
+      <c r="I21" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="I21" s="6" t="str">
-        <f t="array" ref="I21">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v/>
-      </c>
-      <c r="J21" s="30" t="str">
+      <c r="J21" s="6" t="str">
+        <f t="array" ref="J21">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
+        <v/>
+      </c>
+      <c r="K21" s="50" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
-      <c r="K21" s="2"/>
-      <c r="L21" s="5">
+      <c r="L21" s="2"/>
+      <c r="M21" s="5">
         <v>-20</v>
       </c>
-      <c r="M21" s="30">
+      <c r="N21" s="30">
         <f>MAX(Periods[Id])</f>
         <v>5</v>
       </c>
-      <c r="N21" s="5" t="str">
-        <f t="array" ref="N21">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="O21" s="30" t="str">
+      <c r="O21" s="5" t="str">
+        <f t="array" ref="O21">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</f>
+        <v/>
+      </c>
+      <c r="P21" s="30" t="str">
         <f>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
@@ -3500,8 +3500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRuler="0" view="pageLayout" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" view="pageLayout" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3513,7 +3513,7 @@
     <col min="7" max="7" width="3.85546875" style="4" customWidth="1"/>
     <col min="8" max="9" width="9.140625" style="4" customWidth="1"/>
     <col min="10" max="10" width="18.42578125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" style="4" customWidth="1"/>
     <col min="12" max="12" width="0.85546875" style="4" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="4"/>
   </cols>
@@ -3530,11 +3530,11 @@
       <c r="G1" s="24"/>
       <c r="H1" s="24"/>
       <c r="I1" s="23"/>
-      <c r="J1" s="41">
+      <c r="J1" s="47">
         <f>MAX(Periods[Start])</f>
         <v>42529</v>
       </c>
-      <c r="K1" s="42"/>
+      <c r="K1" s="48"/>
       <c r="L1" s="13"/>
       <c r="M1" s="7"/>
     </row>
@@ -3581,11 +3581,11 @@
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
-      <c r="D4" s="45">
+      <c r="D4" s="43">
         <f t="array" ref="D4:D12">LastWeekTasks[Hours]</f>
         <v>0</v>
       </c>
-      <c r="E4" s="43" t="str">
+      <c r="E4" s="41" t="str">
         <f t="array" ref="E4:E18">LastWeekTasks[Done]</f>
         <v>X</v>
       </c>
@@ -3607,10 +3607,10 @@
       </c>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
-      <c r="D5" s="46">
+      <c r="D5" s="44">
         <v>0.17708333333333326</v>
       </c>
-      <c r="E5" s="44" t="str">
+      <c r="E5" s="42" t="str">
         <v>X</v>
       </c>
       <c r="F5" s="15"/>
@@ -3631,10 +3631,10 @@
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
-      <c r="D6" s="47">
+      <c r="D6" s="45">
         <v>2.083333333333337E-2</v>
       </c>
-      <c r="E6" s="43" t="str">
+      <c r="E6" s="41" t="str">
         <v>X</v>
       </c>
       <c r="F6" s="15"/>
@@ -3655,10 +3655,10 @@
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
-      <c r="D7" s="47">
-        <v>0.19791666666666674</v>
-      </c>
-      <c r="E7" s="43" t="str">
+      <c r="D7" s="45">
+        <v>0.26041666666666674</v>
+      </c>
+      <c r="E7" s="41" t="str">
         <v/>
       </c>
       <c r="F7" s="15"/>
@@ -3679,10 +3679,10 @@
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
-      <c r="D8" s="47">
+      <c r="D8" s="45">
         <v>0</v>
       </c>
-      <c r="E8" s="43" t="str">
+      <c r="E8" s="41" t="str">
         <v/>
       </c>
       <c r="F8" s="15"/>
@@ -3704,10 +3704,10 @@
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
-      <c r="D9" s="47">
+      <c r="D9" s="45">
         <v>0.15625</v>
       </c>
-      <c r="E9" s="43" t="str">
+      <c r="E9" s="41" t="str">
         <v/>
       </c>
       <c r="F9" s="15"/>
@@ -3729,10 +3729,10 @@
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
-      <c r="D10" s="47">
+      <c r="D10" s="45">
         <v>9.3749999999999889E-2</v>
       </c>
-      <c r="E10" s="43" t="str">
+      <c r="E10" s="41" t="str">
         <v/>
       </c>
       <c r="F10" s="15"/>
@@ -3754,10 +3754,10 @@
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
-      <c r="D11" s="47" t="str">
-        <v/>
-      </c>
-      <c r="E11" s="43" t="str">
+      <c r="D11" s="45" t="str">
+        <v/>
+      </c>
+      <c r="E11" s="41" t="str">
         <v/>
       </c>
       <c r="F11" s="15"/>
@@ -3779,10 +3779,10 @@
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
-      <c r="D12" s="45" t="str">
-        <v/>
-      </c>
-      <c r="E12" s="43" t="str">
+      <c r="D12" s="43" t="str">
+        <v/>
+      </c>
+      <c r="E12" s="41" t="str">
         <v/>
       </c>
       <c r="F12" s="12"/>
@@ -3953,12 +3953,12 @@
     <row r="21" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="str">
         <f t="array" ref="A21:A30">ThisWeekQuestions[Question]</f>
-        <v>Can I use my own branch in literature?</v>
+        <v>Can we look at how physical infrastructure impacts a community for inspiration?</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
-      <c r="E21" s="37"/>
+      <c r="E21" s="51"/>
       <c r="F21" s="40"/>
       <c r="G21" s="40"/>
       <c r="H21" s="40"/>
@@ -3970,12 +3970,12 @@
     </row>
     <row r="22" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A22" s="32" t="str">
-        <v>What classes am I "qualified" to GTA?</v>
+        <v>Can we model ubiquitious computing's impact on any or just one at a time?</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
-      <c r="E22" s="11"/>
+      <c r="E22" s="52"/>
       <c r="F22" s="20"/>
       <c r="G22" s="20"/>
       <c r="H22" s="20"/>
@@ -3987,12 +3987,12 @@
     </row>
     <row r="23" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="str">
-        <v>How have HHS systems been modeled?</v>
+        <v>Can we model ubiquitious computing's impact on a community without individuals?</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
-      <c r="E23" s="11"/>
+      <c r="E23" s="52"/>
       <c r="F23" s="20"/>
       <c r="G23" s="20"/>
       <c r="H23" s="20"/>
@@ -4004,7 +4004,7 @@
     </row>
     <row r="24" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="str">
-        <v>Can we design a CHS conceptual framework that works in all situations</v>
+        <v>I'm interested in machine learning but does that help me model?</v>
       </c>
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
@@ -4021,7 +4021,7 @@
     </row>
     <row r="25" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="str">
-        <v/>
+        <v>Human system isn't idempotent. It learns based on past inputs.</v>
       </c>
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
@@ -4038,7 +4038,7 @@
     </row>
     <row r="26" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="str">
-        <v/>
+        <v>I have a wedding in OKC on January 14th?</v>
       </c>
       <c r="B26" s="20"/>
       <c r="C26" s="20"/>
@@ -4054,8 +4054,8 @@
       <c r="M26"/>
     </row>
     <row r="27" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A27" s="19" t="str">
-        <v/>
+      <c r="A27" s="10" t="str">
+        <v>Can I use my own branch in literature?</v>
       </c>
       <c r="B27" s="20"/>
       <c r="C27" s="20"/>
@@ -4071,8 +4071,8 @@
       <c r="M27"/>
     </row>
     <row r="28" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A28" s="19" t="str">
-        <v/>
+      <c r="A28" s="10" t="str">
+        <v>What classes am I "qualified" to GTA?</v>
       </c>
       <c r="B28" s="20"/>
       <c r="C28" s="20"/>
@@ -4088,8 +4088,8 @@
       <c r="M28"/>
     </row>
     <row r="29" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A29" s="19" t="str">
-        <v/>
+      <c r="A29" s="10" t="str">
+        <v>How have HHS systems been modeled?</v>
       </c>
       <c r="B29" s="20"/>
       <c r="C29" s="20"/>
@@ -4105,8 +4105,8 @@
       <c r="M29"/>
     </row>
     <row r="30" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A30" s="19" t="str">
-        <v/>
+      <c r="A30" s="10" t="str">
+        <v>Can we design a CHS conceptual framework that works in all situations?</v>
       </c>
       <c r="B30" s="20"/>
       <c r="C30" s="20"/>
@@ -4232,65 +4232,65 @@
     <mergeCell ref="J1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:E18">
-    <cfRule type="expression" dxfId="20" priority="13">
+    <cfRule type="expression" dxfId="15" priority="13">
       <formula>INDIRECT("A"&amp;ROW()) &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="14">
+    <cfRule type="expression" dxfId="14" priority="14">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="15">
+    <cfRule type="expression" dxfId="13" priority="15">
       <formula>INDIRECT("A"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:K18">
-    <cfRule type="expression" dxfId="6" priority="10">
+    <cfRule type="expression" dxfId="12" priority="10">
       <formula>INDIRECT("H"&amp;ROW()) &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="11">
+    <cfRule type="expression" dxfId="11" priority="11">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="12">
+    <cfRule type="expression" dxfId="10" priority="12">
       <formula>INDIRECT("H"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:K30">
-    <cfRule type="expression" dxfId="15" priority="7">
+    <cfRule type="expression" dxfId="9" priority="7">
       <formula>INDIRECT("A"&amp;ROW()) &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="8">
+    <cfRule type="expression" dxfId="8" priority="8">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="9">
+    <cfRule type="expression" dxfId="7" priority="9">
       <formula>INDIRECT("A"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H12">
-    <cfRule type="expression" dxfId="12" priority="6">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>INDIRECT("H"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:K12">
-    <cfRule type="expression" dxfId="11" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>INDIRECT("H"&amp;ROW()) &lt;&gt; ""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A12">
-    <cfRule type="expression" dxfId="10" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>INDIRECT("A"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E12">
-    <cfRule type="expression" dxfId="9" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>INDIRECT("A"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:A30">
-    <cfRule type="expression" dxfId="8" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>INDIRECT("A"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21:K30">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>INDIRECT("A"&amp;ROW()) &lt;&gt; ""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Adding notes and my weekly update.
</commit_message>
<xml_diff>
--- a/updates/Updates.xlsx
+++ b/updates/Updates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Goals" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B28" authorId="0" shapeId="0">
+    <comment ref="B29" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B30" authorId="0" shapeId="0">
+    <comment ref="B31" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="102">
   <si>
     <t>Install JabRef on my personal machine</t>
   </si>
@@ -380,17 +380,22 @@
   </si>
   <si>
     <t>How does the University handle source code I write while a student?</t>
+  </si>
+  <si>
+    <t>Uploading Open Source Data Library</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="6">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="169" formatCode="[h]:mm;@"/>
+    <numFmt numFmtId="170" formatCode="[h]:mm"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -591,7 +596,7 @@
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -651,15 +656,6 @@
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -676,6 +672,17 @@
     <xf numFmtId="165" fontId="8" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma 2" xfId="3"/>
@@ -684,7 +691,23 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="57">
+    <dxf>
+      <numFmt numFmtId="170" formatCode="[h]:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="[h]:mm;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
     <dxf>
       <border>
         <right style="thin">
@@ -807,6 +830,127 @@
       </border>
     </dxf>
     <dxf>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -833,16 +977,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -854,12 +988,6 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
@@ -909,42 +1037,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Goals" displayName="Goals" ref="A1:F31" totalsRowShown="0">
-  <autoFilter ref="A1:F31">
-    <filterColumn colId="5">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
-  <sortState ref="A21:F31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Goals" displayName="Goals" ref="A1:F32" totalsRowShown="0">
+  <autoFilter ref="A1:F32"/>
+  <sortState ref="A2:F32">
     <sortCondition ref="F2:F31"/>
     <sortCondition ref="E2:E31"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="8" name="Id" dataDxfId="41"/>
+    <tableColumn id="8" name="Id" dataDxfId="56"/>
     <tableColumn id="1" name="Description"/>
     <tableColumn id="2" name="Comments"/>
-    <tableColumn id="4" name="Due" dataDxfId="40"/>
-    <tableColumn id="3" name="Started" dataDxfId="39"/>
-    <tableColumn id="5" name="Finished" dataDxfId="38"/>
+    <tableColumn id="4" name="Due" dataDxfId="55"/>
+    <tableColumn id="3" name="Started" dataDxfId="54"/>
+    <tableColumn id="5" name="Finished" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Times" displayName="Times" ref="A1:H23" totalsRowShown="0">
-  <autoFilter ref="A1:H23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Times" displayName="Times" ref="A1:H27" totalsRowShown="0">
+  <autoFilter ref="A1:H27"/>
   <tableColumns count="8">
     <tableColumn id="4" name="Work"/>
     <tableColumn id="9" name="Period"/>
     <tableColumn id="5" name="Date"/>
-    <tableColumn id="6" name="Start" dataDxfId="37"/>
-    <tableColumn id="7" name="End" dataDxfId="36"/>
-    <tableColumn id="1" name="Hours" dataDxfId="35">
+    <tableColumn id="6" name="Start" dataDxfId="52"/>
+    <tableColumn id="7" name="End" dataDxfId="51"/>
+    <tableColumn id="1" name="Hours" dataDxfId="50">
       <calculatedColumnFormula>Times[[#This Row],[End]]-Times[[#This Row],[Start]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Goal" dataDxfId="34"/>
-    <tableColumn id="3" name="Goal Description" dataDxfId="33">
+    <tableColumn id="2" name="Goal" dataDxfId="49"/>
+    <tableColumn id="3" name="Goal Description" dataDxfId="48">
       <calculatedColumnFormula>VLOOKUP(Times[[#This Row],[Goal]], Goals[], 2, FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -972,12 +1096,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Periods" displayName="Periods" ref="A1:D7" totalsRowShown="0">
   <autoFilter ref="A1:D7"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Id" dataDxfId="32"/>
-    <tableColumn id="2" name="Start" dataDxfId="31"/>
-    <tableColumn id="3" name="End" dataDxfId="30">
+    <tableColumn id="1" name="Id" dataDxfId="47"/>
+    <tableColumn id="2" name="Start" dataDxfId="46"/>
+    <tableColumn id="3" name="End" dataDxfId="4">
       <calculatedColumnFormula>Periods[[#This Row],[Start]] + (7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Hours" dataDxfId="29">
+    <tableColumn id="4" name="Hours" dataDxfId="1">
       <calculatedColumnFormula array="1">SUM((Times[Period] = Periods[[#This Row],[Id]]) * Times[Hours])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -993,23 +1117,23 @@
     <sortCondition ref="F2:F21"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="2" name="Index" dataDxfId="28"/>
-    <tableColumn id="4" name="Period" dataDxfId="27">
+    <tableColumn id="2" name="Index" dataDxfId="45"/>
+    <tableColumn id="4" name="Period" dataDxfId="44">
       <calculatedColumnFormula>MAX(Periods[Id]) -1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Show" dataDxfId="26">
+    <tableColumn id="7" name="Show" dataDxfId="43">
       <calculatedColumnFormula>LastWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Goal" dataDxfId="25">
+    <tableColumn id="5" name="Goal" dataDxfId="42">
       <calculatedColumnFormula array="1">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Goal Description" dataDxfId="24">
+    <tableColumn id="1" name="Goal Description" dataDxfId="3">
       <calculatedColumnFormula>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Hours" dataDxfId="23">
+    <tableColumn id="6" name="Hours" dataDxfId="0">
       <calculatedColumnFormula array="1">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Done" dataDxfId="22">
+    <tableColumn id="3" name="Done" dataDxfId="2">
       <calculatedColumnFormula>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1025,17 +1149,17 @@
     <sortCondition ref="N2:N21"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="2" name="Index" dataDxfId="21"/>
-    <tableColumn id="6" name="Period" dataDxfId="20">
+    <tableColumn id="2" name="Index" dataDxfId="41"/>
+    <tableColumn id="6" name="Period" dataDxfId="40">
       <calculatedColumnFormula>MAX(Periods[Id])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Show" dataDxfId="19">
+    <tableColumn id="3" name="Show" dataDxfId="39">
       <calculatedColumnFormula>ThisWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Goal" dataDxfId="18">
+    <tableColumn id="5" name="Goal" dataDxfId="38">
       <calculatedColumnFormula array="1">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Description" dataDxfId="17">
+    <tableColumn id="1" name="Description" dataDxfId="37">
       <calculatedColumnFormula>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1050,8 +1174,8 @@
     <sortCondition descending="1" ref="T1:T21"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="2" name="Index" dataDxfId="16"/>
-    <tableColumn id="1" name="Question" dataDxfId="15">
+    <tableColumn id="2" name="Index" dataDxfId="36"/>
+    <tableColumn id="1" name="Question" dataDxfId="35">
       <calculatedColumnFormula array="1">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1346,10 +1470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1388,7 +1512,7 @@
         <v>Current Period: 5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1405,7 +1529,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1422,7 +1546,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1439,7 +1563,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1456,7 +1580,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1473,7 +1597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1490,7 +1614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>8</v>
       </c>
@@ -1507,7 +1631,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>10</v>
       </c>
@@ -1524,7 +1648,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>11</v>
       </c>
@@ -1541,7 +1665,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>12</v>
       </c>
@@ -1558,7 +1682,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>9</v>
       </c>
@@ -1575,7 +1699,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>7</v>
       </c>
@@ -1592,7 +1716,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>23</v>
       </c>
@@ -1609,7 +1733,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>15</v>
       </c>
@@ -1626,7 +1750,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>13</v>
       </c>
@@ -1643,7 +1767,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>25</v>
       </c>
@@ -1660,7 +1784,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>26</v>
       </c>
@@ -1677,7 +1801,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>27</v>
       </c>
@@ -1694,7 +1818,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -1713,36 +1837,38 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="30">
-        <v>2</v>
-      </c>
-      <c r="F21" s="30"/>
+        <v>5</v>
+      </c>
+      <c r="F21" s="30">
+        <v>5</v>
+      </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>96</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" s="30"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>92</v>
+        <v>5</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="30">
@@ -1753,91 +1879,91 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
-        <v>29</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>76</v>
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>92</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="30">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F24" s="30"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
-        <v>16</v>
-      </c>
-      <c r="B25" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="2">
-        <v>42577</v>
-      </c>
-      <c r="E25" s="30"/>
+        <v>29</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="30">
+        <v>4</v>
+      </c>
       <c r="F25" s="30"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="D26" s="2">
-        <v>42583</v>
+        <v>42577</v>
       </c>
       <c r="E26" s="30"/>
       <c r="F26" s="30"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="D27" s="2">
-        <v>42585</v>
+        <v>42583</v>
       </c>
       <c r="E27" s="30"/>
       <c r="F27" s="30"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
-        <v>19</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>7</v>
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>71</v>
       </c>
       <c r="D28" s="2">
-        <v>42586</v>
+        <v>42585</v>
       </c>
       <c r="E28" s="30"/>
       <c r="F28" s="30"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
-        <v>17</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" t="s">
-        <v>4</v>
+        <v>19</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>7</v>
       </c>
       <c r="D29" s="2">
-        <v>42587</v>
+        <v>42586</v>
       </c>
       <c r="E29" s="30"/>
       <c r="F29" s="30"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
-        <v>27</v>
-      </c>
-      <c r="B30" t="s">
-        <v>70</v>
+        <v>17</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
       </c>
       <c r="D30" s="2">
         <v>42587</v>
@@ -1847,20 +1973,33 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>50</v>
-      </c>
-      <c r="D31" s="2"/>
+        <v>70</v>
+      </c>
+      <c r="D31" s="2">
+        <v>42587</v>
+      </c>
       <c r="E31" s="30"/>
       <c r="F31" s="30"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" location="heading=h.q544jq4bo7vu" display="https://docs.google.com/document/d/1WtVePtADr7xStL5Ac2lepzWibRBYoZs5Y_515wGqzFw/edit - heading=h.q544jq4bo7vu"/>
     <hyperlink ref="B7" r:id="rId2" location="heading=h.q544jq4bo7vu" display="https://docs.google.com/document/d/1WtVePtADr7xStL5Ac2lepzWibRBYoZs5Y_515wGqzFw/edit - heading=h.q544jq4bo7vu"/>
-    <hyperlink ref="B29" r:id="rId3" location="inbox/154e7d1ce0153b1e"/>
+    <hyperlink ref="B30" r:id="rId3" location="inbox/154e7d1ce0153b1e"/>
     <hyperlink ref="B9" r:id="rId4" location="heading=h.4uv9il96waak" display="https://docs.google.com/document/d/1WtVePtADr7xStL5Ac2lepzWibRBYoZs5Y_515wGqzFw/edit - heading=h.4uv9il96waak"/>
     <hyperlink ref="B10" r:id="rId5" location="heading=h.kwuhphhohs6l" display="https://docs.google.com/document/d/1WtVePtADr7xStL5Ac2lepzWibRBYoZs5Y_515wGqzFw/edit - heading=h.kwuhphhohs6l"/>
     <hyperlink ref="B11" r:id="rId6" location="heading=h.kwuhphhohs6l" display="https://docs.google.com/document/d/1WtVePtADr7xStL5Ac2lepzWibRBYoZs5Y_515wGqzFw/edit - heading=h.kwuhphhohs6l"/>
@@ -1877,10 +2016,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2532,10 +2671,130 @@
         <v>Reinforcement Learning an Introduction</v>
       </c>
     </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24" s="3">
+        <v>42533</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E24" s="6">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="F24" s="6">
+        <f>Times[[#This Row],[End]]-Times[[#This Row],[Start]]</f>
+        <v>0.25</v>
+      </c>
+      <c r="G24" s="30">
+        <v>32</v>
+      </c>
+      <c r="H24" s="6" t="str">
+        <f>VLOOKUP(Times[[#This Row],[Goal]], Goals[], 2, FALSE)</f>
+        <v>Uploading Open Source Data Library</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25" s="3">
+        <v>42534</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E25" s="6">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="F25" s="6">
+        <f>Times[[#This Row],[End]]-Times[[#This Row],[Start]]</f>
+        <v>0.20833333333333326</v>
+      </c>
+      <c r="G25" s="30">
+        <v>32</v>
+      </c>
+      <c r="H25" s="6" t="str">
+        <f>VLOOKUP(Times[[#This Row],[Goal]], Goals[], 2, FALSE)</f>
+        <v>Uploading Open Source Data Library</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="C26" s="3">
+        <v>42535</v>
+      </c>
+      <c r="D26" s="6">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E26" s="6">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="F26" s="6">
+        <f>Times[[#This Row],[End]]-Times[[#This Row],[Start]]</f>
+        <v>0.1875</v>
+      </c>
+      <c r="G26" s="30">
+        <v>32</v>
+      </c>
+      <c r="H26" s="6" t="str">
+        <f>VLOOKUP(Times[[#This Row],[Goal]], Goals[], 2, FALSE)</f>
+        <v>Uploading Open Source Data Library</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="C27" s="3">
+        <v>42536</v>
+      </c>
+      <c r="D27" s="6">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E27" s="6">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="F27" s="6">
+        <f>Times[[#This Row],[End]]-Times[[#This Row],[Start]]</f>
+        <v>8.3333333333333259E-2</v>
+      </c>
+      <c r="G27" s="30">
+        <v>14</v>
+      </c>
+      <c r="H27" s="6" t="str">
+        <f>VLOOKUP(Times[[#This Row],[Goal]], Goals[], 2, FALSE)</f>
+        <v>Reinforcement Learning an Introduction</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F31" s="30"/>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" sqref="G2:H23"/>
+    <dataValidation allowBlank="1" showInputMessage="1" sqref="G2:H27"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2549,8 +2808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2743,7 +3002,7 @@
   <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2836,13 +3095,13 @@
         <f>Periods[[#This Row],[Start]] + (7)</f>
         <v>42508</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="51">
         <f t="array" ref="D2">SUM((Times[Period] = Periods[[#This Row],[Id]]) * Times[Hours])</f>
         <v>0</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="5">
-        <v>-13</v>
+        <v>-14</v>
       </c>
       <c r="G2" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -2860,11 +3119,11 @@
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v>Finish first year class plan</v>
       </c>
-      <c r="K2" s="6">
+      <c r="K2" s="52">
         <f t="array" ref="K2">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v>3.125E-2</v>
       </c>
-      <c r="L2" s="48" t="str">
+      <c r="L2" s="45" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v>X</v>
       </c>
@@ -2907,13 +3166,13 @@
         <f>Periods[[#This Row],[Start]] + (7)</f>
         <v>42515</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="51">
         <f t="array" ref="D3">SUM((Times[Period] = Periods[[#This Row],[Id]]) * Times[Hours])</f>
         <v>0</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="5">
-        <v>-12</v>
+        <v>-13</v>
       </c>
       <c r="G3" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -2931,11 +3190,11 @@
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v>Send Jayne my TA preferences</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="52">
         <f t="array" ref="K3">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v>2.083333333333337E-2</v>
       </c>
-      <c r="L3" s="48" t="str">
+      <c r="L3" s="45" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v>X</v>
       </c>
@@ -2978,12 +3237,12 @@
         <f>Periods[[#This Row],[Start]] + (7)</f>
         <v>42522</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="51">
         <f t="array" ref="D4">SUM((Times[Period] = Periods[[#This Row],[Id]]) * Times[Hours])</f>
         <v>0.25000000000000006</v>
       </c>
       <c r="F4" s="5">
-        <v>-11</v>
+        <v>-12</v>
       </c>
       <c r="G4" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -2995,19 +3254,19 @@
       </c>
       <c r="I4" s="30">
         <f t="array" ref="I4">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J4" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v>Introduction to Statistical Learning</v>
-      </c>
-      <c r="K4" s="6">
+        <v>Uploading Open Source Data Library</v>
+      </c>
+      <c r="K4" s="52">
         <f t="array" ref="K4">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v>0</v>
-      </c>
-      <c r="L4" s="47" t="str">
+        <v>0.64583333333333326</v>
+      </c>
+      <c r="L4" s="45" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="5">
@@ -3048,12 +3307,12 @@
         <f>Periods[[#This Row],[Start]] + (7)</f>
         <v>42529</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="51">
         <f t="array" ref="D5">SUM((Times[Period] = Periods[[#This Row],[Id]]) * Times[Hours])</f>
         <v>0.72916666666666663</v>
       </c>
       <c r="F5" s="5">
-        <v>-10</v>
+        <v>-11</v>
       </c>
       <c r="G5" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -3065,17 +3324,17 @@
       </c>
       <c r="I5" s="30">
         <f t="array" ref="I5">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="J5" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v>Reinforcement Learning an Introduction</v>
-      </c>
-      <c r="K5" s="6">
-        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", -1, SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
+        <v>Introduction to Statistical Learning</v>
+      </c>
+      <c r="K5" s="52">
+        <f t="array" ref="K5">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v>0</v>
       </c>
-      <c r="L5" s="48" t="str">
+      <c r="L5" s="44" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
@@ -3118,12 +3377,12 @@
         <f>Periods[[#This Row],[Start]] + (7)</f>
         <v>42536</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="52">
         <f t="array" ref="D6">SUM((Times[Period] = Periods[[#This Row],[Id]]) * Times[Hours])</f>
-        <v>0.30208333333333331</v>
+        <v>1.0312499999999998</v>
       </c>
       <c r="F6" s="5">
-        <v>-9</v>
+        <v>-10</v>
       </c>
       <c r="G6" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -3135,17 +3394,17 @@
       </c>
       <c r="I6" s="30">
         <f t="array" ref="I6">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>24</v>
-      </c>
-      <c r="J6" s="15" t="str">
+        <v>14</v>
+      </c>
+      <c r="J6" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v>Read article abstracts</v>
-      </c>
-      <c r="K6" s="6">
+        <v>Reinforcement Learning an Introduction</v>
+      </c>
+      <c r="K6" s="52">
         <f t="array" ref="K6">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v>0</v>
-      </c>
-      <c r="L6" s="48" t="str">
+        <v>0.32291666666666657</v>
+      </c>
+      <c r="L6" s="45" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
@@ -3188,12 +3447,12 @@
         <f>Periods[[#This Row],[Start]] + (7)</f>
         <v>42543</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="51">
         <f t="array" ref="D7">SUM((Times[Period] = Periods[[#This Row],[Id]]) * Times[Hours])</f>
         <v>0</v>
       </c>
       <c r="F7" s="5">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="G7" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -3205,17 +3464,17 @@
       </c>
       <c r="I7" s="30">
         <f t="array" ref="I7">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>29</v>
-      </c>
-      <c r="J7" t="str">
+        <v>24</v>
+      </c>
+      <c r="J7" s="15" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v>Integrate into UVA System</v>
-      </c>
-      <c r="K7" s="6">
+        <v>Read article abstracts</v>
+      </c>
+      <c r="K7" s="52">
         <f t="array" ref="K7">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v>0</v>
       </c>
-      <c r="L7" s="48" t="str">
+      <c r="L7" s="45" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
@@ -3249,7 +3508,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F8" s="5">
-        <v>-20</v>
+        <v>-8</v>
       </c>
       <c r="G8" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -3257,21 +3516,21 @@
       </c>
       <c r="H8" s="30" t="b">
         <f>LastWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
+        <v>1</v>
+      </c>
+      <c r="I8" s="30">
+        <f t="array" ref="I8">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
+        <v>29</v>
+      </c>
+      <c r="J8" t="str">
+        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
+        <v>Integrate into UVA System</v>
+      </c>
+      <c r="K8" s="52">
+        <f t="array" ref="K8">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v>0</v>
       </c>
-      <c r="I8" s="30" t="str">
-        <f t="array" ref="I8">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v/>
-      </c>
-      <c r="J8" s="30" t="str">
-        <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K8" s="6" t="str">
-        <f t="array" ref="K8">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v/>
-      </c>
-      <c r="L8" s="48" t="str">
+      <c r="L8" s="45" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
@@ -3305,7 +3564,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F9" s="5">
-        <v>-19</v>
+        <v>-20</v>
       </c>
       <c r="G9" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -3323,11 +3582,11 @@
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="K9" s="6" t="str">
+      <c r="K9" s="52" t="str">
         <f t="array" ref="K9">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v/>
       </c>
-      <c r="L9" s="48" t="str">
+      <c r="L9" s="45" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
@@ -3361,7 +3620,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F10" s="5">
-        <v>-18</v>
+        <v>-19</v>
       </c>
       <c r="G10" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -3375,15 +3634,15 @@
         <f t="array" ref="I10">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
         <v/>
       </c>
-      <c r="J10" s="51" t="str">
+      <c r="J10" s="30" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="K10" s="6" t="str">
+      <c r="K10" s="52" t="str">
         <f t="array" ref="K10">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v/>
       </c>
-      <c r="L10" s="48" t="str">
+      <c r="L10" s="45" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
@@ -3417,7 +3676,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F11" s="5">
-        <v>-17</v>
+        <v>-18</v>
       </c>
       <c r="G11" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -3431,15 +3690,15 @@
         <f t="array" ref="I11">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
         <v/>
       </c>
-      <c r="J11" s="46" t="str">
+      <c r="J11" s="48" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="K11" s="6" t="str">
+      <c r="K11" s="52" t="str">
         <f t="array" ref="K11">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v/>
       </c>
-      <c r="L11" s="48" t="str">
+      <c r="L11" s="45" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
@@ -3473,7 +3732,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F12" s="5">
-        <v>-16</v>
+        <v>-17</v>
       </c>
       <c r="G12" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -3487,15 +3746,15 @@
         <f t="array" ref="I12">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
         <v/>
       </c>
-      <c r="J12" s="30" t="str">
+      <c r="J12" s="43" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="K12" s="6" t="str">
+      <c r="K12" s="52" t="str">
         <f t="array" ref="K12">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v/>
       </c>
-      <c r="L12" s="48" t="str">
+      <c r="L12" s="45" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
@@ -3529,7 +3788,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F13" s="5">
-        <v>-15</v>
+        <v>-16</v>
       </c>
       <c r="G13" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -3543,15 +3802,15 @@
         <f t="array" ref="I13">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
         <v/>
       </c>
-      <c r="J13" t="str">
+      <c r="J13" s="30" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="K13" s="6" t="str">
+      <c r="K13" s="52" t="str">
         <f t="array" ref="K13">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v/>
       </c>
-      <c r="L13" s="48" t="str">
+      <c r="L13" s="45" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
@@ -3578,7 +3837,7 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F14" s="5">
-        <v>-14</v>
+        <v>-15</v>
       </c>
       <c r="G14" s="30">
         <f>MAX(Periods[Id]) -1</f>
@@ -3596,11 +3855,11 @@
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="K14" s="6" t="str">
+      <c r="K14" s="52" t="str">
         <f t="array" ref="K14">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v/>
       </c>
-      <c r="L14" s="48" t="str">
+      <c r="L14" s="45" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
@@ -3645,11 +3904,11 @@
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="K15" s="6" t="str">
+      <c r="K15" s="52" t="str">
         <f t="array" ref="K15">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v/>
       </c>
-      <c r="L15" s="48" t="str">
+      <c r="L15" s="45" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
@@ -3694,11 +3953,11 @@
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="K16" s="6" t="str">
+      <c r="K16" s="52" t="str">
         <f t="array" ref="K16">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v/>
       </c>
-      <c r="L16" s="48" t="str">
+      <c r="L16" s="45" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
@@ -3743,11 +4002,11 @@
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="K17" s="6" t="str">
+      <c r="K17" s="52" t="str">
         <f t="array" ref="K17">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v/>
       </c>
-      <c r="L17" s="48" t="str">
+      <c r="L17" s="45" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
@@ -3792,11 +4051,11 @@
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="K18" s="6" t="str">
+      <c r="K18" s="52" t="str">
         <f t="array" ref="K18">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v/>
       </c>
-      <c r="L18" s="48" t="str">
+      <c r="L18" s="45" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
@@ -3841,11 +4100,11 @@
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="K19" s="6" t="str">
+      <c r="K19" s="52" t="str">
         <f t="array" ref="K19">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v/>
       </c>
-      <c r="L19" s="48" t="str">
+      <c r="L19" s="45" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
@@ -3890,11 +4149,11 @@
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="K20" s="6" t="str">
+      <c r="K20" s="52" t="str">
         <f t="array" ref="K20">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v/>
       </c>
-      <c r="L20" s="48" t="str">
+      <c r="L20" s="45" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
@@ -3939,11 +4198,11 @@
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="K21" s="6" t="str">
+      <c r="K21" s="52" t="str">
         <f t="array" ref="K21">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v/>
       </c>
-      <c r="L21" s="48" t="str">
+      <c r="L21" s="45" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
@@ -3984,8 +4243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRuler="0" view="pageLayout" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" view="pageLayout" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4014,11 +4273,11 @@
       <c r="G1" s="24"/>
       <c r="H1" s="24"/>
       <c r="I1" s="23"/>
-      <c r="J1" s="52">
+      <c r="J1" s="49">
         <f>MAX(Periods[Start])</f>
         <v>42536</v>
       </c>
-      <c r="K1" s="53"/>
+      <c r="K1" s="50"/>
       <c r="L1" s="13"/>
       <c r="M1" s="7"/>
     </row>
@@ -4065,7 +4324,7 @@
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
-      <c r="D4" s="43">
+      <c r="D4" s="53">
         <f t="array" ref="D4:D12">LastWeekTasks[Hours]</f>
         <v>3.125E-2</v>
       </c>
@@ -4091,7 +4350,7 @@
       </c>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
-      <c r="D5" s="44">
+      <c r="D5" s="54">
         <v>2.083333333333337E-2</v>
       </c>
       <c r="E5" s="42" t="str">
@@ -4111,15 +4370,15 @@
     </row>
     <row r="6" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="str">
-        <v>Introduction to Statistical Learning</v>
+        <v>Uploading Open Source Data Library</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
-      <c r="D6" s="45">
-        <v>0</v>
+      <c r="D6" s="55">
+        <v>0.64583333333333326</v>
       </c>
       <c r="E6" s="41" t="str">
-        <v/>
+        <v>X</v>
       </c>
       <c r="F6" s="15"/>
       <c r="H6" s="10" t="str">
@@ -4135,11 +4394,11 @@
     </row>
     <row r="7" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="str">
-        <v>Reinforcement Learning an Introduction</v>
+        <v>Introduction to Statistical Learning</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
-      <c r="D7" s="45">
+      <c r="D7" s="55">
         <v>0</v>
       </c>
       <c r="E7" s="41" t="str">
@@ -4159,12 +4418,12 @@
     </row>
     <row r="8" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="str">
-        <v>Read article abstracts</v>
+        <v>Reinforcement Learning an Introduction</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
-      <c r="D8" s="45">
-        <v>0</v>
+      <c r="D8" s="55">
+        <v>0.32291666666666657</v>
       </c>
       <c r="E8" s="41" t="str">
         <v/>
@@ -4184,11 +4443,11 @@
     </row>
     <row r="9" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="str">
-        <v>Integrate into UVA System</v>
+        <v>Read article abstracts</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
-      <c r="D9" s="45">
+      <c r="D9" s="55">
         <v>0</v>
       </c>
       <c r="E9" s="41" t="str">
@@ -4209,12 +4468,12 @@
     </row>
     <row r="10" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="str">
-        <v/>
+        <v>Integrate into UVA System</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
-      <c r="D10" s="45" t="str">
-        <v/>
+      <c r="D10" s="55">
+        <v>0</v>
       </c>
       <c r="E10" s="41" t="str">
         <v/>
@@ -4238,7 +4497,7 @@
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
-      <c r="D11" s="45" t="str">
+      <c r="D11" s="55" t="str">
         <v/>
       </c>
       <c r="E11" s="41" t="str">
@@ -4263,7 +4522,7 @@
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
-      <c r="D12" s="43" t="str">
+      <c r="D12" s="53" t="str">
         <v/>
       </c>
       <c r="E12" s="41" t="str">
@@ -4442,7 +4701,7 @@
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
-      <c r="E21" s="49"/>
+      <c r="E21" s="46"/>
       <c r="F21" s="40"/>
       <c r="G21" s="40"/>
       <c r="H21" s="40"/>
@@ -4459,7 +4718,7 @@
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
-      <c r="E22" s="50"/>
+      <c r="E22" s="47"/>
       <c r="F22" s="20"/>
       <c r="G22" s="20"/>
       <c r="H22" s="20"/>
@@ -4476,7 +4735,7 @@
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
-      <c r="E23" s="50"/>
+      <c r="E23" s="47"/>
       <c r="F23" s="20"/>
       <c r="G23" s="20"/>
       <c r="H23" s="20"/>
@@ -4716,65 +4975,65 @@
     <mergeCell ref="J1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:E18">
-    <cfRule type="expression" dxfId="14" priority="13">
+    <cfRule type="expression" dxfId="19" priority="13">
       <formula>INDIRECT("A"&amp;ROW()) &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="14">
+    <cfRule type="expression" dxfId="18" priority="14">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="15">
+    <cfRule type="expression" dxfId="17" priority="15">
       <formula>INDIRECT("A"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:K18">
-    <cfRule type="expression" dxfId="11" priority="10">
+    <cfRule type="expression" dxfId="16" priority="10">
       <formula>INDIRECT("H"&amp;ROW()) &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="15" priority="11">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="12">
+    <cfRule type="expression" dxfId="14" priority="12">
       <formula>INDIRECT("H"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:K30">
-    <cfRule type="expression" dxfId="8" priority="7">
+    <cfRule type="expression" dxfId="13" priority="7">
       <formula>INDIRECT("A"&amp;ROW()) &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8">
-      <formula>MOD(ROW(),2)=1</formula>
+    <cfRule type="expression" dxfId="12" priority="8">
+      <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="9">
+    <cfRule type="expression" dxfId="11" priority="9">
       <formula>INDIRECT("A"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H12">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="10" priority="6">
       <formula>INDIRECT("H"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:K12">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>INDIRECT("H"&amp;ROW()) &lt;&gt; ""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A12">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>INDIRECT("A"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E12">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>INDIRECT("A"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:A30">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>INDIRECT("A"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21:K30">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>INDIRECT("A"&amp;ROW()) &lt;&gt; ""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
More notes and updates
</commit_message>
<xml_diff>
--- a/updates/Updates.xlsx
+++ b/updates/Updates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Goals" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="108">
   <si>
     <t>Install JabRef on my personal machine</t>
   </si>
@@ -383,6 +383,24 @@
   </si>
   <si>
     <t>Uploading Open Source Data Library</t>
+  </si>
+  <si>
+    <t>How important are Markov Decision Processes to learning</t>
+  </si>
+  <si>
+    <t>Is Machine Learning being used to create models of systems?</t>
+  </si>
+  <si>
+    <t>Is there research into how systems interact to make "intelligent" decisions?</t>
+  </si>
+  <si>
+    <t>Writing email asking about IP</t>
+  </si>
+  <si>
+    <t>Attending weekly lab meeting</t>
+  </si>
+  <si>
+    <t>Do we having anything like self-regulating self-correcting systems?</t>
   </si>
 </sst>
 </file>
@@ -394,8 +412,8 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="169" formatCode="[h]:mm;@"/>
-    <numFmt numFmtId="170" formatCode="[h]:mm"/>
+    <numFmt numFmtId="166" formatCode="[h]:mm;@"/>
+    <numFmt numFmtId="167" formatCode="[h]:mm"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -666,22 +684,22 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -691,144 +709,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="57">
-    <dxf>
-      <numFmt numFmtId="170" formatCode="[h]:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="[h]:mm;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="42">
     <dxf>
       <border>
         <right style="thin">
@@ -977,6 +858,16 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="[h]:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -988,6 +879,12 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="[h]:mm;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
@@ -1044,31 +941,31 @@
     <sortCondition ref="E2:E31"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="8" name="Id" dataDxfId="56"/>
+    <tableColumn id="8" name="Id" dataDxfId="41"/>
     <tableColumn id="1" name="Description"/>
     <tableColumn id="2" name="Comments"/>
-    <tableColumn id="4" name="Due" dataDxfId="55"/>
-    <tableColumn id="3" name="Started" dataDxfId="54"/>
-    <tableColumn id="5" name="Finished" dataDxfId="53"/>
+    <tableColumn id="4" name="Due" dataDxfId="40"/>
+    <tableColumn id="3" name="Started" dataDxfId="39"/>
+    <tableColumn id="5" name="Finished" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Times" displayName="Times" ref="A1:H27" totalsRowShown="0">
-  <autoFilter ref="A1:H27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Times" displayName="Times" ref="A1:H37" totalsRowShown="0">
+  <autoFilter ref="A1:H37"/>
   <tableColumns count="8">
     <tableColumn id="4" name="Work"/>
     <tableColumn id="9" name="Period"/>
     <tableColumn id="5" name="Date"/>
-    <tableColumn id="6" name="Start" dataDxfId="52"/>
-    <tableColumn id="7" name="End" dataDxfId="51"/>
-    <tableColumn id="1" name="Hours" dataDxfId="50">
+    <tableColumn id="6" name="Start" dataDxfId="37"/>
+    <tableColumn id="7" name="End" dataDxfId="36"/>
+    <tableColumn id="1" name="Hours" dataDxfId="35">
       <calculatedColumnFormula>Times[[#This Row],[End]]-Times[[#This Row],[Start]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Goal" dataDxfId="49"/>
-    <tableColumn id="3" name="Goal Description" dataDxfId="48">
+    <tableColumn id="2" name="Goal" dataDxfId="34"/>
+    <tableColumn id="3" name="Goal Description" dataDxfId="33">
       <calculatedColumnFormula>VLOOKUP(Times[[#This Row],[Goal]], Goals[], 2, FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1077,8 +974,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Questions" displayName="Questions" ref="A1:C16" totalsRowShown="0">
-  <autoFilter ref="A1:C16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Questions" displayName="Questions" ref="A1:C20" totalsRowShown="0">
+  <autoFilter ref="A1:C20">
     <filterColumn colId="2">
       <filters blank="1"/>
     </filterColumn>
@@ -1093,15 +990,15 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Periods" displayName="Periods" ref="A1:D7" totalsRowShown="0">
-  <autoFilter ref="A1:D7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Periods" displayName="Periods" ref="A1:D8" totalsRowShown="0">
+  <autoFilter ref="A1:D8"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Id" dataDxfId="47"/>
-    <tableColumn id="2" name="Start" dataDxfId="46"/>
-    <tableColumn id="3" name="End" dataDxfId="4">
+    <tableColumn id="1" name="Id" dataDxfId="32"/>
+    <tableColumn id="2" name="Start" dataDxfId="31"/>
+    <tableColumn id="3" name="End" dataDxfId="30">
       <calculatedColumnFormula>Periods[[#This Row],[Start]] + (7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Hours" dataDxfId="1">
+    <tableColumn id="4" name="Hours" dataDxfId="29">
       <calculatedColumnFormula array="1">SUM((Times[Period] = Periods[[#This Row],[Id]]) * Times[Hours])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1117,23 +1014,23 @@
     <sortCondition ref="F2:F21"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="2" name="Index" dataDxfId="45"/>
-    <tableColumn id="4" name="Period" dataDxfId="44">
+    <tableColumn id="2" name="Index" dataDxfId="28"/>
+    <tableColumn id="4" name="Period" dataDxfId="27">
       <calculatedColumnFormula>MAX(Periods[Id]) -1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Show" dataDxfId="43">
+    <tableColumn id="7" name="Show" dataDxfId="26">
       <calculatedColumnFormula>LastWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Goal" dataDxfId="42">
+    <tableColumn id="5" name="Goal" dataDxfId="25">
       <calculatedColumnFormula array="1">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Goal Description" dataDxfId="3">
+    <tableColumn id="1" name="Goal Description" dataDxfId="24">
       <calculatedColumnFormula>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Hours" dataDxfId="0">
+    <tableColumn id="6" name="Hours" dataDxfId="23">
       <calculatedColumnFormula array="1">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Done" dataDxfId="2">
+    <tableColumn id="3" name="Done" dataDxfId="22">
       <calculatedColumnFormula>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1149,17 +1046,17 @@
     <sortCondition ref="N2:N21"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="2" name="Index" dataDxfId="41"/>
-    <tableColumn id="6" name="Period" dataDxfId="40">
+    <tableColumn id="2" name="Index" dataDxfId="21"/>
+    <tableColumn id="6" name="Period" dataDxfId="20">
       <calculatedColumnFormula>MAX(Periods[Id])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Show" dataDxfId="39">
+    <tableColumn id="3" name="Show" dataDxfId="19">
       <calculatedColumnFormula>ThisWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Goal" dataDxfId="38">
+    <tableColumn id="5" name="Goal" dataDxfId="18">
       <calculatedColumnFormula array="1">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= ThisWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = ThisWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + ThisWeekTasks[[#This Row],[Index]] + 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Description" dataDxfId="37">
+    <tableColumn id="1" name="Description" dataDxfId="17">
       <calculatedColumnFormula>IF(ThisWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(ThisWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1174,8 +1071,8 @@
     <sortCondition descending="1" ref="T1:T21"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="2" name="Index" dataDxfId="36"/>
-    <tableColumn id="1" name="Question" dataDxfId="35">
+    <tableColumn id="2" name="Index" dataDxfId="16"/>
+    <tableColumn id="1" name="Question" dataDxfId="15">
       <calculatedColumnFormula array="1">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1509,7 +1406,7 @@
       </c>
       <c r="H1" t="str">
         <f xml:space="preserve"> "Current Period: " &amp; MAX(Periods[Id]) -1</f>
-        <v>Current Period: 5</v>
+        <v>Current Period: 6</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2016,10 +1913,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2783,18 +2680,288 @@
         <v>Reinforcement Learning an Introduction</v>
       </c>
     </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28">
+        <v>6</v>
+      </c>
+      <c r="C28" s="3">
+        <v>42536</v>
+      </c>
+      <c r="D28" s="6">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E28" s="6">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="F28" s="6">
+        <f>Times[[#This Row],[End]]-Times[[#This Row],[Start]]</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="G28" s="30">
+        <v>14</v>
+      </c>
+      <c r="H28" s="6" t="str">
+        <f>VLOOKUP(Times[[#This Row],[Goal]], Goals[], 2, FALSE)</f>
+        <v>Reinforcement Learning an Introduction</v>
+      </c>
+    </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>97</v>
+      </c>
+      <c r="B29">
+        <v>6</v>
+      </c>
+      <c r="C29" s="3">
+        <v>42537</v>
+      </c>
+      <c r="D29" s="6">
+        <v>0.59375</v>
+      </c>
+      <c r="E29" s="6">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="F29" s="6">
+        <f>Times[[#This Row],[End]]-Times[[#This Row],[Start]]</f>
+        <v>5.208333333333337E-2</v>
+      </c>
+      <c r="G29" s="30">
+        <v>14</v>
+      </c>
+      <c r="H29" s="6" t="str">
+        <f>VLOOKUP(Times[[#This Row],[Goal]], Goals[], 2, FALSE)</f>
+        <v>Reinforcement Learning an Introduction</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30">
+        <v>6</v>
+      </c>
+      <c r="C30" s="3">
+        <v>42538</v>
+      </c>
+      <c r="D30" s="6">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="E30" s="6">
+        <v>0.6875</v>
+      </c>
+      <c r="F30" s="6">
+        <f>Times[[#This Row],[End]]-Times[[#This Row],[Start]]</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="G30" s="30">
+        <v>29</v>
+      </c>
+      <c r="H30" s="6" t="str">
+        <f>VLOOKUP(Times[[#This Row],[Goal]], Goals[], 2, FALSE)</f>
+        <v>Integrate into UVA System</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F31" s="30"/>
+      <c r="A31" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31">
+        <v>6</v>
+      </c>
+      <c r="C31" s="3">
+        <v>42539</v>
+      </c>
+      <c r="D31" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="E31" s="6">
+        <v>0.53125</v>
+      </c>
+      <c r="F31" s="6">
+        <f>Times[[#This Row],[End]]-Times[[#This Row],[Start]]</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="G31" s="30">
+        <v>14</v>
+      </c>
+      <c r="H31" s="6" t="str">
+        <f>VLOOKUP(Times[[#This Row],[Goal]], Goals[], 2, FALSE)</f>
+        <v>Reinforcement Learning an Introduction</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32">
+        <v>6</v>
+      </c>
+      <c r="C32" s="3">
+        <v>42540</v>
+      </c>
+      <c r="D32" s="6">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E32" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="F32" s="6">
+        <f>Times[[#This Row],[End]]-Times[[#This Row],[Start]]</f>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="G32" s="30">
+        <v>14</v>
+      </c>
+      <c r="H32" s="6" t="str">
+        <f>VLOOKUP(Times[[#This Row],[Goal]], Goals[], 2, FALSE)</f>
+        <v>Reinforcement Learning an Introduction</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33">
+        <v>6</v>
+      </c>
+      <c r="C33" s="3">
+        <v>42541</v>
+      </c>
+      <c r="D33" s="6">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="E33" s="6">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="F33" s="6">
+        <f>Times[[#This Row],[End]]-Times[[#This Row],[Start]]</f>
+        <v>4.1666666666666741E-2</v>
+      </c>
+      <c r="G33" s="30">
+        <v>14</v>
+      </c>
+      <c r="H33" s="6" t="str">
+        <f>VLOOKUP(Times[[#This Row],[Goal]], Goals[], 2, FALSE)</f>
+        <v>Reinforcement Learning an Introduction</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34">
+        <v>6</v>
+      </c>
+      <c r="C34" s="3">
+        <v>42541</v>
+      </c>
+      <c r="D34" s="6">
+        <v>0.86458333333333337</v>
+      </c>
+      <c r="E34" s="6">
+        <v>0.9375</v>
+      </c>
+      <c r="F34" s="6">
+        <f>Times[[#This Row],[End]]-Times[[#This Row],[Start]]</f>
+        <v>7.291666666666663E-2</v>
+      </c>
+      <c r="G34" s="30">
+        <v>14</v>
+      </c>
+      <c r="H34" s="6" t="str">
+        <f>VLOOKUP(Times[[#This Row],[Goal]], Goals[], 2, FALSE)</f>
+        <v>Reinforcement Learning an Introduction</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>106</v>
+      </c>
+      <c r="B35">
+        <v>6</v>
+      </c>
+      <c r="C35" s="3">
+        <v>42542</v>
+      </c>
+      <c r="D35" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="E35" s="6">
+        <v>0.5625</v>
+      </c>
+      <c r="F35" s="6">
+        <f>Times[[#This Row],[End]]-Times[[#This Row],[Start]]</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="G35" s="30"/>
+      <c r="H35" s="6" t="str">
+        <f>VLOOKUP(Times[[#This Row],[Goal]], Goals[], 2, FALSE)</f>
+        <v>Miscellaneous</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36">
+        <v>6</v>
+      </c>
+      <c r="C36" s="3">
+        <v>42542</v>
+      </c>
+      <c r="D36" s="6">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="E36" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="F36" s="6">
+        <f>Times[[#This Row],[End]]-Times[[#This Row],[Start]]</f>
+        <v>5.208333333333337E-2</v>
+      </c>
+      <c r="G36" s="30">
+        <v>14</v>
+      </c>
+      <c r="H36" s="6" t="str">
+        <f>VLOOKUP(Times[[#This Row],[Goal]], Goals[], 2, FALSE)</f>
+        <v>Reinforcement Learning an Introduction</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>97</v>
+      </c>
+      <c r="B37">
+        <v>6</v>
+      </c>
+      <c r="C37" s="3">
+        <v>42542</v>
+      </c>
+      <c r="D37" s="6">
+        <v>0.88541666666666663</v>
+      </c>
+      <c r="E37" s="6">
+        <v>0.92708333333333337</v>
+      </c>
+      <c r="F37" s="6">
+        <f>Times[[#This Row],[End]]-Times[[#This Row],[Start]]</f>
+        <v>4.1666666666666741E-2</v>
+      </c>
+      <c r="G37" s="30">
+        <v>14</v>
+      </c>
+      <c r="H37" s="6" t="str">
+        <f>VLOOKUP(Times[[#This Row],[Goal]], Goals[], 2, FALSE)</f>
+        <v>Reinforcement Learning an Introduction</v>
+      </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" sqref="G2:H27"/>
+    <dataValidation allowBlank="1" showInputMessage="1" sqref="G2:H35"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2806,10 +2973,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2987,6 +3154,27 @@
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>100</v>
+      </c>
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -3095,17 +3283,17 @@
         <f>Periods[[#This Row],[Start]] + (7)</f>
         <v>42508</v>
       </c>
-      <c r="D2" s="51">
+      <c r="D2" s="49">
         <f t="array" ref="D2">SUM((Times[Period] = Periods[[#This Row],[Id]]) * Times[Hours])</f>
         <v>0</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="5">
-        <v>-14</v>
+        <v>-11</v>
       </c>
       <c r="G2" s="30">
         <f>MAX(Periods[Id]) -1</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H2" s="30" t="b">
         <f>LastWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -3113,19 +3301,19 @@
       </c>
       <c r="I2" s="30">
         <f t="array" ref="I2">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="J2" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v>Finish first year class plan</v>
-      </c>
-      <c r="K2" s="52">
+        <v>Introduction to Statistical Learning</v>
+      </c>
+      <c r="K2" s="50">
         <f t="array" ref="K2">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v>3.125E-2</v>
-      </c>
-      <c r="L2" s="45" t="str">
+        <v>0</v>
+      </c>
+      <c r="L2" s="44" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="5">
@@ -3133,7 +3321,7 @@
       </c>
       <c r="O2" s="30">
         <f>MAX(Periods[Id])</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P2" s="30" t="b">
         <f>ThisWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -3152,7 +3340,7 @@
       </c>
       <c r="U2" t="str">
         <f t="array" ref="U2">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v>How does the University handle source code I write while a student?</v>
+        <v>Do we having anything like self-regulating self-correcting systems?</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -3166,17 +3354,17 @@
         <f>Periods[[#This Row],[Start]] + (7)</f>
         <v>42515</v>
       </c>
-      <c r="D3" s="51">
+      <c r="D3" s="49">
         <f t="array" ref="D3">SUM((Times[Period] = Periods[[#This Row],[Id]]) * Times[Hours])</f>
         <v>0</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="5">
-        <v>-13</v>
+        <v>-10</v>
       </c>
       <c r="G3" s="30">
         <f>MAX(Periods[Id]) -1</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H3" s="30" t="b">
         <f>LastWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -3184,19 +3372,19 @@
       </c>
       <c r="I3" s="30">
         <f t="array" ref="I3">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J3" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v>Send Jayne my TA preferences</v>
-      </c>
-      <c r="K3" s="52">
+        <v>Reinforcement Learning an Introduction</v>
+      </c>
+      <c r="K3" s="50">
         <f t="array" ref="K3">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v>2.083333333333337E-2</v>
+        <v>0.43750000000000022</v>
       </c>
       <c r="L3" s="45" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="5">
@@ -3204,7 +3392,7 @@
       </c>
       <c r="O3" s="30">
         <f>MAX(Periods[Id])</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P3" s="30" t="b">
         <f>ThisWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -3223,7 +3411,7 @@
       </c>
       <c r="U3" t="str">
         <f t="array" ref="U3">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v/>
+        <v>Is there research into how systems interact to make "intelligent" decisions?</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -3237,16 +3425,16 @@
         <f>Periods[[#This Row],[Start]] + (7)</f>
         <v>42522</v>
       </c>
-      <c r="D4" s="51">
+      <c r="D4" s="49">
         <f t="array" ref="D4">SUM((Times[Period] = Periods[[#This Row],[Id]]) * Times[Hours])</f>
         <v>0.25000000000000006</v>
       </c>
       <c r="F4" s="5">
-        <v>-12</v>
+        <v>-9</v>
       </c>
       <c r="G4" s="30">
         <f>MAX(Periods[Id]) -1</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H4" s="30" t="b">
         <f>LastWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -3254,19 +3442,19 @@
       </c>
       <c r="I4" s="30">
         <f t="array" ref="I4">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>32</v>
-      </c>
-      <c r="J4" t="str">
+        <v>24</v>
+      </c>
+      <c r="J4" s="15" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v>Uploading Open Source Data Library</v>
-      </c>
-      <c r="K4" s="52">
+        <v>Read article abstracts</v>
+      </c>
+      <c r="K4" s="50">
         <f t="array" ref="K4">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v>0.64583333333333326</v>
+        <v>0</v>
       </c>
       <c r="L4" s="45" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="5">
@@ -3274,7 +3462,7 @@
       </c>
       <c r="O4" s="30">
         <f>MAX(Periods[Id])</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P4" s="30" t="b">
         <f>ThisWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -3293,7 +3481,7 @@
       </c>
       <c r="U4" t="str">
         <f t="array" ref="U4">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v/>
+        <v>Is Machine Learning being used to create models of systems?</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -3307,16 +3495,16 @@
         <f>Periods[[#This Row],[Start]] + (7)</f>
         <v>42529</v>
       </c>
-      <c r="D5" s="51">
+      <c r="D5" s="49">
         <f t="array" ref="D5">SUM((Times[Period] = Periods[[#This Row],[Id]]) * Times[Hours])</f>
         <v>0.72916666666666663</v>
       </c>
       <c r="F5" s="5">
-        <v>-11</v>
+        <v>-8</v>
       </c>
       <c r="G5" s="30">
         <f>MAX(Periods[Id]) -1</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H5" s="30" t="b">
         <f>LastWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -3324,17 +3512,17 @@
       </c>
       <c r="I5" s="30">
         <f t="array" ref="I5">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J5" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v>Introduction to Statistical Learning</v>
-      </c>
-      <c r="K5" s="52">
+        <v>Integrate into UVA System</v>
+      </c>
+      <c r="K5" s="50">
         <f t="array" ref="K5">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v>0</v>
-      </c>
-      <c r="L5" s="44" t="str">
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="L5" s="45" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
         <v/>
       </c>
@@ -3344,7 +3532,7 @@
       </c>
       <c r="O5" s="30">
         <f>MAX(Periods[Id])</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P5" s="30" t="b">
         <f>ThisWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -3363,7 +3551,7 @@
       </c>
       <c r="U5" t="str">
         <f t="array" ref="U5">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v/>
+        <v>How important are Markov Decision Processes to learning</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -3377,32 +3565,32 @@
         <f>Periods[[#This Row],[Start]] + (7)</f>
         <v>42536</v>
       </c>
-      <c r="D6" s="52">
+      <c r="D6" s="50">
         <f t="array" ref="D6">SUM((Times[Period] = Periods[[#This Row],[Id]]) * Times[Hours])</f>
         <v>1.0312499999999998</v>
       </c>
       <c r="F6" s="5">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="G6" s="30">
         <f>MAX(Periods[Id]) -1</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H6" s="30" t="b">
         <f>LastWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
-        <v>1</v>
-      </c>
-      <c r="I6" s="30">
+        <v>0</v>
+      </c>
+      <c r="I6" s="30" t="str">
         <f t="array" ref="I6">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>14</v>
-      </c>
-      <c r="J6" t="str">
+        <v/>
+      </c>
+      <c r="J6" s="30" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v>Reinforcement Learning an Introduction</v>
-      </c>
-      <c r="K6" s="52">
+        <v/>
+      </c>
+      <c r="K6" s="50" t="str">
         <f t="array" ref="K6">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v>0.32291666666666657</v>
+        <v/>
       </c>
       <c r="L6" s="45" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
@@ -3414,7 +3602,7 @@
       </c>
       <c r="O6" s="30">
         <f>MAX(Periods[Id])</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P6" s="30" t="b">
         <f>ThisWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -3433,7 +3621,7 @@
       </c>
       <c r="U6" t="str">
         <f t="array" ref="U6">IF(ISERR(INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1)), "", INDEX(IF(ISBLANK(Questions[Answer]), Questions[Question], "" ), COUNTA(Questions[Question]) + ThisWeekQuestions[[#This Row],[Index]] + 1))</f>
-        <v/>
+        <v>How does the University handle source code I write while a student?</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -3447,32 +3635,32 @@
         <f>Periods[[#This Row],[Start]] + (7)</f>
         <v>42543</v>
       </c>
-      <c r="D7" s="51">
+      <c r="D7" s="49">
         <f t="array" ref="D7">SUM((Times[Period] = Periods[[#This Row],[Id]]) * Times[Hours])</f>
-        <v>0</v>
+        <v>0.54166666666666685</v>
       </c>
       <c r="F7" s="5">
-        <v>-9</v>
+        <v>-19</v>
       </c>
       <c r="G7" s="30">
         <f>MAX(Periods[Id]) -1</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H7" s="30" t="b">
         <f>LastWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
-        <v>1</v>
-      </c>
-      <c r="I7" s="30">
+        <v>0</v>
+      </c>
+      <c r="I7" s="30" t="str">
         <f t="array" ref="I7">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>24</v>
-      </c>
-      <c r="J7" s="15" t="str">
+        <v/>
+      </c>
+      <c r="J7" s="30" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v>Read article abstracts</v>
-      </c>
-      <c r="K7" s="52">
+        <v/>
+      </c>
+      <c r="K7" s="50" t="str">
         <f t="array" ref="K7">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="L7" s="45" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
@@ -3484,7 +3672,7 @@
       </c>
       <c r="O7" s="30">
         <f>MAX(Periods[Id])</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P7" s="30" t="b">
         <f>ThisWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -3507,28 +3695,40 @@
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="30">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3">
+        <f>Periods[[#This Row],[Start]] + (7)</f>
+        <v>7</v>
+      </c>
+      <c r="D8" s="49">
+        <f t="array" ref="D8">SUM((Times[Period] = Periods[[#This Row],[Id]]) * Times[Hours])</f>
+        <v>0</v>
+      </c>
       <c r="F8" s="5">
-        <v>-8</v>
+        <v>-18</v>
       </c>
       <c r="G8" s="30">
         <f>MAX(Periods[Id]) -1</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H8" s="30" t="b">
         <f>LastWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
-        <v>1</v>
-      </c>
-      <c r="I8" s="30">
+        <v>0</v>
+      </c>
+      <c r="I8" s="30" t="str">
         <f t="array" ref="I8">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
-        <v>29</v>
-      </c>
-      <c r="J8" t="str">
+        <v/>
+      </c>
+      <c r="J8" s="48" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
-        <v>Integrate into UVA System</v>
-      </c>
-      <c r="K8" s="52">
+        <v/>
+      </c>
+      <c r="K8" s="50" t="str">
         <f t="array" ref="K8">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="L8" s="45" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", IF(NOT(ISBLANK(VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 6, FALSE))), "X", ""))</f>
@@ -3540,7 +3740,7 @@
       </c>
       <c r="O8" s="30">
         <f>MAX(Periods[Id])</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P8" s="30" t="b">
         <f>ThisWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -3564,11 +3764,11 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F9" s="5">
-        <v>-20</v>
+        <v>-17</v>
       </c>
       <c r="G9" s="30">
         <f>MAX(Periods[Id]) -1</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H9" s="30" t="b">
         <f>LastWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -3578,11 +3778,11 @@
         <f t="array" ref="I9">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
         <v/>
       </c>
-      <c r="J9" s="30" t="str">
+      <c r="J9" s="43" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="K9" s="52" t="str">
+      <c r="K9" s="50" t="str">
         <f t="array" ref="K9">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v/>
       </c>
@@ -3596,7 +3796,7 @@
       </c>
       <c r="O9" s="30">
         <f>MAX(Periods[Id])</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P9" s="30" t="b">
         <f>ThisWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -3620,11 +3820,11 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F10" s="5">
-        <v>-19</v>
+        <v>-16</v>
       </c>
       <c r="G10" s="30">
         <f>MAX(Periods[Id]) -1</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H10" s="30" t="b">
         <f>LastWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -3638,7 +3838,7 @@
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="K10" s="52" t="str">
+      <c r="K10" s="50" t="str">
         <f t="array" ref="K10">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v/>
       </c>
@@ -3652,7 +3852,7 @@
       </c>
       <c r="O10" s="30">
         <f>MAX(Periods[Id])</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P10" s="30" t="b">
         <f>ThisWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -3676,11 +3876,11 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F11" s="5">
-        <v>-18</v>
+        <v>-15</v>
       </c>
       <c r="G11" s="30">
         <f>MAX(Periods[Id]) -1</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H11" s="30" t="b">
         <f>LastWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -3690,11 +3890,11 @@
         <f t="array" ref="I11">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
         <v/>
       </c>
-      <c r="J11" s="48" t="str">
+      <c r="J11" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="K11" s="52" t="str">
+      <c r="K11" s="50" t="str">
         <f t="array" ref="K11">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v/>
       </c>
@@ -3708,7 +3908,7 @@
       </c>
       <c r="O11" s="30">
         <f>MAX(Periods[Id])</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P11" s="30" t="b">
         <f>ThisWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -3732,11 +3932,11 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F12" s="5">
-        <v>-17</v>
+        <v>-14</v>
       </c>
       <c r="G12" s="30">
         <f>MAX(Periods[Id]) -1</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H12" s="30" t="b">
         <f>LastWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -3746,11 +3946,11 @@
         <f t="array" ref="I12">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
         <v/>
       </c>
-      <c r="J12" s="43" t="str">
+      <c r="J12" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="K12" s="52" t="str">
+      <c r="K12" s="50" t="str">
         <f t="array" ref="K12">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v/>
       </c>
@@ -3764,7 +3964,7 @@
       </c>
       <c r="O12" s="30">
         <f>MAX(Periods[Id])</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P12" s="30" t="b">
         <f>ThisWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -3788,11 +3988,11 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F13" s="5">
-        <v>-16</v>
+        <v>-13</v>
       </c>
       <c r="G13" s="30">
         <f>MAX(Periods[Id]) -1</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H13" s="30" t="b">
         <f>LastWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -3802,11 +4002,11 @@
         <f t="array" ref="I13">INDEX(IF((Goals[Started] &gt; 0) * (Goals[Started] &lt;= LastWeekTasks[[#This Row],[Period]]) * ((Goals[Finished] = LastWeekTasks[[#This Row],[Period]]) + (Goals[Finished] =  0 )),  Goals[Id], "" ), COUNT(Goals[Id]) + LastWeekTasks[[#This Row],[Index]] + 1)</f>
         <v/>
       </c>
-      <c r="J13" s="30" t="str">
+      <c r="J13" t="str">
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="K13" s="52" t="str">
+      <c r="K13" s="50" t="str">
         <f t="array" ref="K13">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v/>
       </c>
@@ -3820,7 +4020,7 @@
       </c>
       <c r="O13" s="30">
         <f>MAX(Periods[Id])</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P13" s="30" t="b">
         <f>ThisWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -3837,11 +4037,11 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F14" s="5">
-        <v>-15</v>
+        <v>-12</v>
       </c>
       <c r="G14" s="30">
         <f>MAX(Periods[Id]) -1</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H14" s="30" t="b">
         <f>LastWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -3855,7 +4055,7 @@
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="K14" s="52" t="str">
+      <c r="K14" s="50" t="str">
         <f t="array" ref="K14">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v/>
       </c>
@@ -3869,7 +4069,7 @@
       </c>
       <c r="O14" s="30">
         <f>MAX(Periods[Id])</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P14" s="30" t="b">
         <f>ThisWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -3890,7 +4090,7 @@
       </c>
       <c r="G15" s="30">
         <f>MAX(Periods[Id]) -1</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H15" s="30" t="b">
         <f>LastWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -3904,7 +4104,7 @@
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="K15" s="52" t="str">
+      <c r="K15" s="50" t="str">
         <f t="array" ref="K15">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v/>
       </c>
@@ -3918,7 +4118,7 @@
       </c>
       <c r="O15" s="30">
         <f>MAX(Periods[Id])</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P15" s="30" t="b">
         <f>ThisWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -3939,7 +4139,7 @@
       </c>
       <c r="G16" s="30">
         <f>MAX(Periods[Id]) -1</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H16" s="30" t="b">
         <f>LastWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -3953,7 +4153,7 @@
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="K16" s="52" t="str">
+      <c r="K16" s="50" t="str">
         <f t="array" ref="K16">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v/>
       </c>
@@ -3967,7 +4167,7 @@
       </c>
       <c r="O16" s="30">
         <f>MAX(Periods[Id])</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P16" s="30" t="b">
         <f>ThisWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -3988,7 +4188,7 @@
       </c>
       <c r="G17" s="30">
         <f>MAX(Periods[Id]) -1</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H17" s="30" t="b">
         <f>LastWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -4002,7 +4202,7 @@
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="K17" s="52" t="str">
+      <c r="K17" s="50" t="str">
         <f t="array" ref="K17">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v/>
       </c>
@@ -4016,7 +4216,7 @@
       </c>
       <c r="O17" s="30">
         <f>MAX(Periods[Id])</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P17" s="30" t="b">
         <f>ThisWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -4037,7 +4237,7 @@
       </c>
       <c r="G18" s="30">
         <f>MAX(Periods[Id]) -1</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H18" s="30" t="b">
         <f>LastWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -4051,7 +4251,7 @@
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="K18" s="52" t="str">
+      <c r="K18" s="50" t="str">
         <f t="array" ref="K18">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v/>
       </c>
@@ -4065,7 +4265,7 @@
       </c>
       <c r="O18" s="30">
         <f>MAX(Periods[Id])</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P18" s="30" t="b">
         <f>ThisWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -4086,7 +4286,7 @@
       </c>
       <c r="G19" s="30">
         <f>MAX(Periods[Id]) -1</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H19" s="30" t="b">
         <f>LastWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -4100,7 +4300,7 @@
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="K19" s="52" t="str">
+      <c r="K19" s="50" t="str">
         <f t="array" ref="K19">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v/>
       </c>
@@ -4114,7 +4314,7 @@
       </c>
       <c r="O19" s="30">
         <f>MAX(Periods[Id])</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P19" s="30" t="b">
         <f>ThisWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -4135,7 +4335,7 @@
       </c>
       <c r="G20" s="30">
         <f>MAX(Periods[Id]) -1</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H20" s="30" t="b">
         <f>LastWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -4149,7 +4349,7 @@
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="K20" s="52" t="str">
+      <c r="K20" s="50" t="str">
         <f t="array" ref="K20">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v/>
       </c>
@@ -4163,7 +4363,7 @@
       </c>
       <c r="O20" s="30">
         <f>MAX(Periods[Id])</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P20" s="30" t="b">
         <f>ThisWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -4184,7 +4384,7 @@
       </c>
       <c r="G21" s="30">
         <f>MAX(Periods[Id]) -1</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H21" s="30" t="b">
         <f>LastWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -4198,7 +4398,7 @@
         <f>IF(LastWeekTasks[[#This Row],[Goal]] = "", "", VLOOKUP(LastWeekTasks[[#This Row],[Goal]], Goals[], 2, FALSE))</f>
         <v/>
       </c>
-      <c r="K21" s="52" t="str">
+      <c r="K21" s="50" t="str">
         <f t="array" ref="K21">IF(LastWeekTasks[[#This Row],[Goal]] = "", "", SUM((Times[Period] = LastWeekTasks[[#This Row],[Period]]) * (Times[Goal] = LastWeekTasks[[#This Row],[Goal]]) * (Times[Hours])))</f>
         <v/>
       </c>
@@ -4212,7 +4412,7 @@
       </c>
       <c r="O21" s="30">
         <f>MAX(Periods[Id])</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P21" s="30" t="b">
         <f>ThisWeekTasks[[#This Row],[Goal]] &lt;&gt; ""</f>
@@ -4243,8 +4443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" view="pageLayout" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView showGridLines="0" showRuler="0" view="pageLayout" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4273,11 +4473,11 @@
       <c r="G1" s="24"/>
       <c r="H1" s="24"/>
       <c r="I1" s="23"/>
-      <c r="J1" s="49">
+      <c r="J1" s="54">
         <f>MAX(Periods[Start])</f>
         <v>42536</v>
       </c>
-      <c r="K1" s="50"/>
+      <c r="K1" s="55"/>
       <c r="L1" s="13"/>
       <c r="M1" s="7"/>
     </row>
@@ -4320,17 +4520,17 @@
     <row r="4" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="str">
         <f t="array" ref="A4:A18">LastWeekTasks[Goal Description]</f>
-        <v>Finish first year class plan</v>
+        <v>Introduction to Statistical Learning</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
-      <c r="D4" s="53">
+      <c r="D4" s="51">
         <f t="array" ref="D4:D12">LastWeekTasks[Hours]</f>
-        <v>3.125E-2</v>
+        <v>0</v>
       </c>
       <c r="E4" s="41" t="str">
         <f t="array" ref="E4:E18">LastWeekTasks[Done]</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="F4" s="16"/>
       <c r="H4" s="17" t="str">
@@ -4346,15 +4546,15 @@
     </row>
     <row r="5" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="32" t="str">
-        <v>Send Jayne my TA preferences</v>
+        <v>Reinforcement Learning an Introduction</v>
       </c>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
-      <c r="D5" s="54">
-        <v>2.083333333333337E-2</v>
+      <c r="D5" s="52">
+        <v>0.43750000000000022</v>
       </c>
       <c r="E5" s="42" t="str">
-        <v>X</v>
+        <v/>
       </c>
       <c r="F5" s="15"/>
       <c r="H5" s="32" t="str">
@@ -4370,15 +4570,15 @@
     </row>
     <row r="6" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="str">
-        <v>Uploading Open Source Data Library</v>
+        <v>Read article abstracts</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
-      <c r="D6" s="55">
-        <v>0.64583333333333326</v>
+      <c r="D6" s="53">
+        <v>0</v>
       </c>
       <c r="E6" s="41" t="str">
-        <v>X</v>
+        <v/>
       </c>
       <c r="F6" s="15"/>
       <c r="H6" s="10" t="str">
@@ -4394,12 +4594,12 @@
     </row>
     <row r="7" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="str">
-        <v>Introduction to Statistical Learning</v>
+        <v>Integrate into UVA System</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
-      <c r="D7" s="55">
-        <v>0</v>
+      <c r="D7" s="53">
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="E7" s="41" t="str">
         <v/>
@@ -4418,12 +4618,12 @@
     </row>
     <row r="8" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="str">
-        <v>Reinforcement Learning an Introduction</v>
+        <v/>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
-      <c r="D8" s="55">
-        <v>0.32291666666666657</v>
+      <c r="D8" s="53" t="str">
+        <v/>
       </c>
       <c r="E8" s="41" t="str">
         <v/>
@@ -4443,12 +4643,12 @@
     </row>
     <row r="9" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="str">
-        <v>Read article abstracts</v>
+        <v/>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
-      <c r="D9" s="55">
-        <v>0</v>
+      <c r="D9" s="53" t="str">
+        <v/>
       </c>
       <c r="E9" s="41" t="str">
         <v/>
@@ -4468,12 +4668,12 @@
     </row>
     <row r="10" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="str">
-        <v>Integrate into UVA System</v>
+        <v/>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
-      <c r="D10" s="55">
-        <v>0</v>
+      <c r="D10" s="53" t="str">
+        <v/>
       </c>
       <c r="E10" s="41" t="str">
         <v/>
@@ -4497,7 +4697,7 @@
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
-      <c r="D11" s="55" t="str">
+      <c r="D11" s="53" t="str">
         <v/>
       </c>
       <c r="E11" s="41" t="str">
@@ -4522,7 +4722,7 @@
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
-      <c r="D12" s="53" t="str">
+      <c r="D12" s="51" t="str">
         <v/>
       </c>
       <c r="E12" s="41" t="str">
@@ -4696,7 +4896,7 @@
     <row r="21" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="str">
         <f t="array" ref="A21:A30">ThisWeekQuestions[Question]</f>
-        <v>How does the University handle source code I write while a student?</v>
+        <v>Do we having anything like self-regulating self-correcting systems?</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -4713,7 +4913,7 @@
     </row>
     <row r="22" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A22" s="32" t="str">
-        <v/>
+        <v>Is there research into how systems interact to make "intelligent" decisions?</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
@@ -4730,7 +4930,7 @@
     </row>
     <row r="23" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="str">
-        <v/>
+        <v>Is Machine Learning being used to create models of systems?</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
@@ -4747,7 +4947,7 @@
     </row>
     <row r="24" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="str">
-        <v/>
+        <v>How important are Markov Decision Processes to learning</v>
       </c>
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
@@ -4764,7 +4964,7 @@
     </row>
     <row r="25" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="str">
-        <v/>
+        <v>How does the University handle source code I write while a student?</v>
       </c>
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
@@ -4975,65 +5175,65 @@
     <mergeCell ref="J1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:E18">
-    <cfRule type="expression" dxfId="19" priority="13">
+    <cfRule type="expression" dxfId="14" priority="13">
       <formula>INDIRECT("A"&amp;ROW()) &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="14">
+    <cfRule type="expression" dxfId="13" priority="14">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="15">
+    <cfRule type="expression" dxfId="12" priority="15">
       <formula>INDIRECT("A"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:K18">
-    <cfRule type="expression" dxfId="16" priority="10">
+    <cfRule type="expression" dxfId="11" priority="10">
       <formula>INDIRECT("H"&amp;ROW()) &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="11">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="12">
+    <cfRule type="expression" dxfId="9" priority="12">
       <formula>INDIRECT("H"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:K30">
-    <cfRule type="expression" dxfId="13" priority="7">
+    <cfRule type="expression" dxfId="8" priority="7">
       <formula>INDIRECT("A"&amp;ROW()) &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="8">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="9">
+    <cfRule type="expression" dxfId="6" priority="9">
       <formula>INDIRECT("A"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H12">
-    <cfRule type="expression" dxfId="10" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>INDIRECT("H"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:K12">
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>INDIRECT("H"&amp;ROW()) &lt;&gt; ""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A12">
-    <cfRule type="expression" dxfId="8" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>INDIRECT("A"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E12">
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>INDIRECT("A"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:A30">
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>INDIRECT("A"&amp;ROW())&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21:K30">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>INDIRECT("A"&amp;ROW()) &lt;&gt; ""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>